<commit_message>
fix in spongebob season 2 sequels
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad\vue-dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85025792-3DDC-4F9F-9E28-13A1CEF4CED1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC82EC78-8FF4-4AF4-BEDA-619056B015D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6884" uniqueCount="1825">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6884" uniqueCount="1826">
   <si>
     <t>Title</t>
   </si>
@@ -5503,6 +5503,9 @@
   </si>
   <si>
     <t>A masterpiece. Linguistics and Aliens are an unlikely combination but it all makes sense and this movie has a twist that will forever leave me with my jaw on the floor just like the first time I saw it. Villeneuve, Adams, Renner. What else do you want? Kangaroo 🤷</t>
+  </si>
+  <si>
+    <t>Spongebob Squarepants [Season 3], Spongebob Squarepants [Season 4], Spongebob Squarepants [Season 5], Spongebob Squarepants [Season 6], Spongebob Squarepants [Season 7], Spongebob Squarepants [Season 8]</t>
   </si>
 </sst>
 </file>
@@ -5898,9 +5901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O15" sqref="O15"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J255" sqref="J255"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21536,7 +21539,7 @@
         <v>458</v>
       </c>
       <c r="J253" s="4" t="s">
-        <v>683</v>
+        <v>1825</v>
       </c>
       <c r="K253" s="3" t="s">
         <v>420</v>

</xml_diff>

<commit_message>
jodie star wars fix
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad\vue-dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC82EC78-8FF4-4AF4-BEDA-619056B015D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9705D225-7183-4C9C-AB9A-1A17550392E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6884" uniqueCount="1826">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6878" uniqueCount="1826">
   <si>
     <t>Title</t>
   </si>
@@ -5901,9 +5901,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T384"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A219" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J255" sqref="J255"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A246" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F260" sqref="F260"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -21988,22 +21988,22 @@
         <v>1287</v>
       </c>
       <c r="O260" s="4" t="s">
-        <v>1133</v>
+        <v>1780</v>
       </c>
       <c r="P260" s="4" t="s">
-        <v>1133</v>
+        <v>97</v>
       </c>
       <c r="Q260" s="4" t="s">
-        <v>1133</v>
+        <v>1639</v>
       </c>
       <c r="R260" s="4" t="s">
-        <v>1133</v>
+        <v>1765</v>
       </c>
       <c r="S260" s="4" t="s">
-        <v>1133</v>
+        <v>1782</v>
       </c>
       <c r="T260" s="4" t="s">
-        <v>1133</v>
+        <v>1781</v>
       </c>
     </row>
     <row r="261" spans="1:20" x14ac:dyDescent="0.25">
@@ -22110,24 +22110,6 @@
       </c>
       <c r="N262" s="4" t="s">
         <v>1287</v>
-      </c>
-      <c r="O262" s="4" t="s">
-        <v>1780</v>
-      </c>
-      <c r="P262" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="Q262" s="4" t="s">
-        <v>1639</v>
-      </c>
-      <c r="R262" s="4" t="s">
-        <v>1765</v>
-      </c>
-      <c r="S262" s="4" t="s">
-        <v>1782</v>
-      </c>
-      <c r="T262" s="4" t="s">
-        <v>1781</v>
       </c>
     </row>
     <row r="263" spans="1:20" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
added the wild robot
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B09DEB8E-8B2F-428A-BD23-143FC0073354}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4ECDC79-0DF1-4394-843C-10F231E7769B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6926" uniqueCount="1893">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6939" uniqueCount="1902">
   <si>
     <t>Title</t>
   </si>
@@ -5707,6 +5707,33 @@
   </si>
   <si>
     <t>signed by Linus Sandgren, also available in Farsi</t>
+  </si>
+  <si>
+    <t>The_Wild_Robot_2024</t>
+  </si>
+  <si>
+    <t>The Wild Robot</t>
+  </si>
+  <si>
+    <t>Chris Sanders</t>
+  </si>
+  <si>
+    <t>Animation, Drama, Coming-of-Age</t>
+  </si>
+  <si>
+    <t>A movie that leaves me with tears pouring down my face and questioning if Ratatouille should still be my favorite animated movie of all time. It comes in as a definitive close second and might even overtake it at some point as time passes. The Wild Robot is genuinely one of the most beautiful films I have ever seen both visually and dramaturgically. I can see how it will mean different things to different people and I can definitely see how even I will see different things in the movie as life goes on. This movie is truly art and if it doesn't win the Oscar this year, it will be the second Robot-Animation film in a row to be snubbed for Best Animated Feature.</t>
+  </si>
+  <si>
+    <t>Chris Sanders, Peter Brown</t>
+  </si>
+  <si>
+    <t>Kris Bowers</t>
+  </si>
+  <si>
+    <t>Chris Stover</t>
+  </si>
+  <si>
+    <t>Lupita Nyong'o, Pedro Pascal, Kit Connor, Bill Nighy, Stephanie Hsu, Ving Rhames, Mark Hamill, Catherine O'Hara, Matt Berry</t>
   </si>
 </sst>
 </file>
@@ -6100,11 +6127,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U386"/>
+  <dimension ref="A1:U387"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A366" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H386" sqref="H386"/>
+      <pane ySplit="1" topLeftCell="A365" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C387" sqref="C387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27537,70 +27564,54 @@
     </row>
     <row r="342" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A342" s="4" t="s">
-        <v>1066</v>
-      </c>
-      <c r="B342" s="4" t="s">
+        <v>1893</v>
+      </c>
+      <c r="B342" s="2" t="s">
         <v>415</v>
       </c>
       <c r="C342" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="D342" s="4" t="s">
-        <v>188</v>
+        <v>48</v>
+      </c>
+      <c r="D342" s="2" t="s">
+        <v>1894</v>
       </c>
       <c r="E342" s="3">
-        <v>2017</v>
-      </c>
-      <c r="F342" s="4" t="s">
-        <v>189</v>
-      </c>
-      <c r="G342" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="H342" s="3"/>
-      <c r="I342" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="J342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="K342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="L342" s="3" t="s">
-        <v>1133</v>
-      </c>
-      <c r="M342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="N342" s="3">
-        <v>122</v>
+        <v>2024</v>
+      </c>
+      <c r="F342" s="5" t="s">
+        <v>1895</v>
+      </c>
+      <c r="G342" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I342" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="N342" s="9">
+        <v>102</v>
       </c>
       <c r="O342" s="4" t="s">
-        <v>1194</v>
-      </c>
-      <c r="P342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="Q342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="R342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="S342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="T342" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="U342" s="4" t="s">
-        <v>1133</v>
+        <v>1896</v>
+      </c>
+      <c r="P342" t="s">
+        <v>1897</v>
+      </c>
+      <c r="Q342" t="s">
+        <v>1898</v>
+      </c>
+      <c r="R342" t="s">
+        <v>1899</v>
+      </c>
+      <c r="S342" t="s">
+        <v>1900</v>
+      </c>
+      <c r="U342" t="s">
+        <v>1901</v>
       </c>
     </row>
     <row r="343" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A343" s="4" t="s">
-        <v>1067</v>
+        <v>1066</v>
       </c>
       <c r="B343" s="4" t="s">
         <v>415</v>
@@ -27609,16 +27620,16 @@
         <v>6</v>
       </c>
       <c r="D343" s="4" t="s">
-        <v>559</v>
+        <v>188</v>
       </c>
       <c r="E343" s="3">
-        <v>2001</v>
+        <v>2017</v>
       </c>
       <c r="F343" s="4" t="s">
-        <v>560</v>
+        <v>189</v>
       </c>
       <c r="G343" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H343" s="3"/>
       <c r="I343" s="3" t="s">
@@ -27637,10 +27648,10 @@
         <v>1133</v>
       </c>
       <c r="N343" s="3">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="O343" s="4" t="s">
-        <v>1383</v>
+        <v>1194</v>
       </c>
       <c r="P343" s="4" t="s">
         <v>1133</v>
@@ -27663,29 +27674,29 @@
     </row>
     <row r="344" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A344" s="4" t="s">
-        <v>1068</v>
+        <v>1067</v>
       </c>
       <c r="B344" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C344" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D344" s="4" t="s">
-        <v>117</v>
+        <v>559</v>
       </c>
       <c r="E344" s="3">
-        <v>2017</v>
+        <v>2001</v>
       </c>
       <c r="F344" s="4" t="s">
-        <v>118</v>
+        <v>560</v>
       </c>
       <c r="G344" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H344" s="3"/>
       <c r="I344" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J344" s="4" t="s">
         <v>1133</v>
@@ -27694,61 +27705,61 @@
         <v>1133</v>
       </c>
       <c r="L344" s="3" t="s">
-        <v>418</v>
+        <v>1133</v>
       </c>
       <c r="M344" s="4" t="s">
-        <v>1185</v>
+        <v>1133</v>
       </c>
       <c r="N344" s="3">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="O344" s="4" t="s">
-        <v>1241</v>
+        <v>1383</v>
       </c>
       <c r="P344" s="4" t="s">
-        <v>1657</v>
+        <v>1133</v>
       </c>
       <c r="Q344" s="4" t="s">
-        <v>1662</v>
+        <v>1133</v>
       </c>
       <c r="R344" s="4" t="s">
-        <v>1659</v>
+        <v>1133</v>
       </c>
       <c r="S344" s="4" t="s">
-        <v>1660</v>
+        <v>1133</v>
       </c>
       <c r="T344" s="4" t="s">
-        <v>1661</v>
+        <v>1133</v>
       </c>
       <c r="U344" s="4" t="s">
-        <v>1658</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="345" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A345" s="4" t="s">
-        <v>1069</v>
+        <v>1068</v>
       </c>
       <c r="B345" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C345" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D345" s="4" t="s">
-        <v>607</v>
+        <v>117</v>
       </c>
       <c r="E345" s="3">
-        <v>2022</v>
+        <v>2017</v>
       </c>
       <c r="F345" s="4" t="s">
-        <v>608</v>
+        <v>118</v>
       </c>
       <c r="G345" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H345" s="3"/>
       <c r="I345" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J345" s="4" t="s">
         <v>1133</v>
@@ -27757,52 +27768,54 @@
         <v>1133</v>
       </c>
       <c r="L345" s="3" t="s">
-        <v>1133</v>
+        <v>418</v>
       </c>
       <c r="M345" s="4" t="s">
-        <v>1133</v>
+        <v>1185</v>
       </c>
       <c r="N345" s="3">
-        <v>104</v>
+        <v>130</v>
       </c>
       <c r="O345" s="4" t="s">
-        <v>1240</v>
+        <v>1241</v>
       </c>
       <c r="P345" s="4" t="s">
-        <v>1133</v>
+        <v>1657</v>
       </c>
       <c r="Q345" s="4" t="s">
-        <v>1133</v>
+        <v>1662</v>
       </c>
       <c r="R345" s="4" t="s">
-        <v>1133</v>
+        <v>1659</v>
       </c>
       <c r="S345" s="4" t="s">
-        <v>1133</v>
+        <v>1660</v>
       </c>
       <c r="T345" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="U345" s="4"/>
+        <v>1661</v>
+      </c>
+      <c r="U345" s="4" t="s">
+        <v>1658</v>
+      </c>
     </row>
     <row r="346" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A346" s="4" t="s">
-        <v>1070</v>
+        <v>1069</v>
       </c>
       <c r="B346" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C346" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D346" s="4" t="s">
-        <v>166</v>
+        <v>607</v>
       </c>
       <c r="E346" s="3">
-        <v>2018</v>
+        <v>2022</v>
       </c>
       <c r="F346" s="4" t="s">
-        <v>167</v>
+        <v>608</v>
       </c>
       <c r="G346" s="3" t="s">
         <v>420</v>
@@ -27824,10 +27837,10 @@
         <v>1133</v>
       </c>
       <c r="N346" s="3">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="O346" s="4" t="s">
-        <v>1239</v>
+        <v>1240</v>
       </c>
       <c r="P346" s="4" t="s">
         <v>1133</v>
@@ -27844,35 +27857,33 @@
       <c r="T346" s="4" t="s">
         <v>1133</v>
       </c>
-      <c r="U346" s="4" t="s">
-        <v>1133</v>
-      </c>
+      <c r="U346" s="4"/>
     </row>
     <row r="347" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A347" s="4" t="s">
-        <v>1071</v>
+        <v>1070</v>
       </c>
       <c r="B347" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C347" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D347" s="4" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
       <c r="E347" s="3">
-        <v>1986</v>
+        <v>2018</v>
       </c>
       <c r="F347" s="4" t="s">
-        <v>77</v>
+        <v>167</v>
       </c>
       <c r="G347" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H347" s="3"/>
       <c r="I347" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J347" s="4" t="s">
         <v>1133</v>
@@ -27881,16 +27892,16 @@
         <v>1133</v>
       </c>
       <c r="L347" s="3" t="s">
-        <v>418</v>
+        <v>1133</v>
       </c>
       <c r="M347" s="4" t="s">
-        <v>1186</v>
+        <v>1133</v>
       </c>
       <c r="N347" s="3">
-        <v>105</v>
+        <v>118</v>
       </c>
       <c r="O347" s="4" t="s">
-        <v>1238</v>
+        <v>1239</v>
       </c>
       <c r="P347" s="4" t="s">
         <v>1133</v>
@@ -27913,7 +27924,7 @@
     </row>
     <row r="348" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A348" s="4" t="s">
-        <v>1072</v>
+        <v>1071</v>
       </c>
       <c r="B348" s="4" t="s">
         <v>415</v>
@@ -27922,16 +27933,16 @@
         <v>6</v>
       </c>
       <c r="D348" s="4" t="s">
-        <v>571</v>
+        <v>76</v>
       </c>
       <c r="E348" s="3">
-        <v>1995</v>
+        <v>1986</v>
       </c>
       <c r="F348" s="4" t="s">
-        <v>572</v>
+        <v>77</v>
       </c>
       <c r="G348" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H348" s="3"/>
       <c r="I348" s="3" t="s">
@@ -27941,19 +27952,19 @@
         <v>1133</v>
       </c>
       <c r="K348" s="4" t="s">
-        <v>710</v>
+        <v>1133</v>
       </c>
       <c r="L348" s="3" t="s">
         <v>418</v>
       </c>
       <c r="M348" s="4" t="s">
-        <v>1187</v>
+        <v>1186</v>
       </c>
       <c r="N348" s="3">
-        <v>78</v>
+        <v>105</v>
       </c>
       <c r="O348" s="4" t="s">
-        <v>1237</v>
+        <v>1238</v>
       </c>
       <c r="P348" s="4" t="s">
         <v>1133</v>
@@ -27976,7 +27987,7 @@
     </row>
     <row r="349" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A349" s="4" t="s">
-        <v>1073</v>
+        <v>1072</v>
       </c>
       <c r="B349" s="4" t="s">
         <v>415</v>
@@ -27985,10 +27996,10 @@
         <v>6</v>
       </c>
       <c r="D349" s="4" t="s">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="E349" s="3">
-        <v>1999</v>
+        <v>1995</v>
       </c>
       <c r="F349" s="4" t="s">
         <v>572</v>
@@ -28001,10 +28012,10 @@
         <v>420</v>
       </c>
       <c r="J349" s="4" t="s">
-        <v>571</v>
+        <v>1133</v>
       </c>
       <c r="K349" s="4" t="s">
-        <v>569</v>
+        <v>710</v>
       </c>
       <c r="L349" s="3" t="s">
         <v>418</v>
@@ -28013,7 +28024,7 @@
         <v>1187</v>
       </c>
       <c r="N349" s="3">
-        <v>89</v>
+        <v>78</v>
       </c>
       <c r="O349" s="4" t="s">
         <v>1237</v>
@@ -28039,7 +28050,7 @@
     </row>
     <row r="350" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A350" s="4" t="s">
-        <v>1074</v>
+        <v>1073</v>
       </c>
       <c r="B350" s="4" t="s">
         <v>415</v>
@@ -28048,13 +28059,13 @@
         <v>6</v>
       </c>
       <c r="D350" s="4" t="s">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="E350" s="3">
-        <v>2010</v>
+        <v>1999</v>
       </c>
       <c r="F350" s="4" t="s">
-        <v>573</v>
+        <v>572</v>
       </c>
       <c r="G350" s="3" t="s">
         <v>420</v>
@@ -28064,10 +28075,10 @@
         <v>420</v>
       </c>
       <c r="J350" s="4" t="s">
-        <v>711</v>
+        <v>571</v>
       </c>
       <c r="K350" s="4" t="s">
-        <v>1133</v>
+        <v>569</v>
       </c>
       <c r="L350" s="3" t="s">
         <v>418</v>
@@ -28076,7 +28087,7 @@
         <v>1187</v>
       </c>
       <c r="N350" s="3">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="O350" s="4" t="s">
         <v>1237</v>
@@ -28102,7 +28113,7 @@
     </row>
     <row r="351" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A351" s="4" t="s">
-        <v>1075</v>
+        <v>1074</v>
       </c>
       <c r="B351" s="4" t="s">
         <v>415</v>
@@ -28111,13 +28122,13 @@
         <v>6</v>
       </c>
       <c r="D351" s="4" t="s">
-        <v>260</v>
+        <v>569</v>
       </c>
       <c r="E351" s="3">
-        <v>2016</v>
+        <v>2010</v>
       </c>
       <c r="F351" s="4" t="s">
-        <v>262</v>
+        <v>573</v>
       </c>
       <c r="G351" s="3" t="s">
         <v>420</v>
@@ -28127,22 +28138,22 @@
         <v>420</v>
       </c>
       <c r="J351" s="4" t="s">
-        <v>1133</v>
+        <v>711</v>
       </c>
       <c r="K351" s="4" t="s">
-        <v>748</v>
+        <v>1133</v>
       </c>
       <c r="L351" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="M351" s="4" t="s">
-        <v>1133</v>
+        <v>1187</v>
       </c>
       <c r="N351" s="3">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="O351" s="4" t="s">
-        <v>1236</v>
+        <v>1237</v>
       </c>
       <c r="P351" s="4" t="s">
         <v>1133</v>
@@ -28165,7 +28176,7 @@
     </row>
     <row r="352" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A352" s="4" t="s">
-        <v>1076</v>
+        <v>1075</v>
       </c>
       <c r="B352" s="4" t="s">
         <v>415</v>
@@ -28174,26 +28185,26 @@
         <v>6</v>
       </c>
       <c r="D352" s="4" t="s">
-        <v>745</v>
+        <v>260</v>
       </c>
       <c r="E352" s="3">
-        <v>2023</v>
+        <v>2016</v>
       </c>
       <c r="F352" s="4" t="s">
-        <v>746</v>
+        <v>262</v>
       </c>
       <c r="G352" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H352" s="3"/>
       <c r="I352" s="3" t="s">
         <v>420</v>
       </c>
       <c r="J352" s="4" t="s">
-        <v>747</v>
+        <v>1133</v>
       </c>
       <c r="K352" s="4" t="s">
-        <v>1133</v>
+        <v>748</v>
       </c>
       <c r="L352" s="3" t="s">
         <v>420</v>
@@ -28202,7 +28213,7 @@
         <v>1133</v>
       </c>
       <c r="N352" s="3">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="O352" s="4" t="s">
         <v>1236</v>
@@ -28228,7 +28239,7 @@
     </row>
     <row r="353" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A353" s="4" t="s">
-        <v>1077</v>
+        <v>1076</v>
       </c>
       <c r="B353" s="4" t="s">
         <v>415</v>
@@ -28237,26 +28248,26 @@
         <v>6</v>
       </c>
       <c r="D353" s="4" t="s">
-        <v>605</v>
+        <v>745</v>
       </c>
       <c r="E353" s="3">
-        <v>2020</v>
+        <v>2023</v>
       </c>
       <c r="F353" s="4" t="s">
-        <v>606</v>
+        <v>746</v>
       </c>
       <c r="G353" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H353" s="3"/>
       <c r="I353" s="3" t="s">
         <v>420</v>
       </c>
       <c r="J353" s="4" t="s">
-        <v>260</v>
+        <v>747</v>
       </c>
       <c r="K353" s="4" t="s">
-        <v>745</v>
+        <v>1133</v>
       </c>
       <c r="L353" s="3" t="s">
         <v>420</v>
@@ -28291,7 +28302,7 @@
     </row>
     <row r="354" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A354" s="4" t="s">
-        <v>1078</v>
+        <v>1077</v>
       </c>
       <c r="B354" s="4" t="s">
         <v>415</v>
@@ -28300,38 +28311,38 @@
         <v>6</v>
       </c>
       <c r="D354" s="4" t="s">
-        <v>391</v>
+        <v>605</v>
       </c>
       <c r="E354" s="3">
-        <v>2010</v>
+        <v>2020</v>
       </c>
       <c r="F354" s="4" t="s">
-        <v>392</v>
+        <v>606</v>
       </c>
       <c r="G354" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H354" s="3"/>
       <c r="I354" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J354" s="4" t="s">
-        <v>1133</v>
+        <v>260</v>
       </c>
       <c r="K354" s="4" t="s">
-        <v>1133</v>
+        <v>745</v>
       </c>
       <c r="L354" s="3" t="s">
-        <v>1133</v>
+        <v>420</v>
       </c>
       <c r="M354" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N354" s="3">
-        <v>106</v>
+        <v>91</v>
       </c>
       <c r="O354" s="4" t="s">
-        <v>1235</v>
+        <v>1236</v>
       </c>
       <c r="P354" s="4" t="s">
         <v>1133</v>
@@ -28354,7 +28365,7 @@
     </row>
     <row r="355" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A355" s="4" t="s">
-        <v>1079</v>
+        <v>1078</v>
       </c>
       <c r="B355" s="4" t="s">
         <v>415</v>
@@ -28363,38 +28374,38 @@
         <v>6</v>
       </c>
       <c r="D355" s="4" t="s">
-        <v>69</v>
+        <v>391</v>
       </c>
       <c r="E355" s="3">
-        <v>2000</v>
+        <v>2010</v>
       </c>
       <c r="F355" s="4" t="s">
-        <v>68</v>
+        <v>392</v>
       </c>
       <c r="G355" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H355" s="3"/>
       <c r="I355" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J355" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="K355" s="4" t="s">
-        <v>712</v>
+        <v>1133</v>
       </c>
       <c r="L355" s="3" t="s">
-        <v>420</v>
+        <v>1133</v>
       </c>
       <c r="M355" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N355" s="3">
-        <v>102</v>
+        <v>106</v>
       </c>
       <c r="O355" s="4" t="s">
-        <v>1234</v>
+        <v>1235</v>
       </c>
       <c r="P355" s="4" t="s">
         <v>1133</v>
@@ -28417,7 +28428,7 @@
     </row>
     <row r="356" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A356" s="4" t="s">
-        <v>1080</v>
+        <v>1079</v>
       </c>
       <c r="B356" s="4" t="s">
         <v>415</v>
@@ -28426,38 +28437,38 @@
         <v>6</v>
       </c>
       <c r="D356" s="4" t="s">
-        <v>214</v>
+        <v>69</v>
       </c>
       <c r="E356" s="3">
-        <v>2009</v>
+        <v>2000</v>
       </c>
       <c r="F356" s="4" t="s">
-        <v>215</v>
+        <v>68</v>
       </c>
       <c r="G356" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H356" s="3"/>
       <c r="I356" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J356" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="K356" s="4" t="s">
-        <v>1133</v>
+        <v>712</v>
       </c>
       <c r="L356" s="3" t="s">
-        <v>1133</v>
+        <v>420</v>
       </c>
       <c r="M356" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N356" s="3">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="O356" s="4" t="s">
-        <v>1220</v>
+        <v>1234</v>
       </c>
       <c r="P356" s="4" t="s">
         <v>1133</v>
@@ -28480,7 +28491,7 @@
     </row>
     <row r="357" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A357" s="4" t="s">
-        <v>1081</v>
+        <v>1080</v>
       </c>
       <c r="B357" s="4" t="s">
         <v>415</v>
@@ -28489,13 +28500,13 @@
         <v>6</v>
       </c>
       <c r="D357" s="4" t="s">
-        <v>354</v>
+        <v>214</v>
       </c>
       <c r="E357" s="3">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="F357" s="4" t="s">
-        <v>66</v>
+        <v>215</v>
       </c>
       <c r="G357" s="3" t="s">
         <v>420</v>
@@ -28517,10 +28528,10 @@
         <v>1133</v>
       </c>
       <c r="N357" s="3">
-        <v>111</v>
+        <v>105</v>
       </c>
       <c r="O357" s="4" t="s">
-        <v>1233</v>
+        <v>1220</v>
       </c>
       <c r="P357" s="4" t="s">
         <v>1133</v>
@@ -28543,7 +28554,7 @@
     </row>
     <row r="358" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A358" s="4" t="s">
-        <v>1082</v>
+        <v>1081</v>
       </c>
       <c r="B358" s="4" t="s">
         <v>415</v>
@@ -28552,20 +28563,20 @@
         <v>6</v>
       </c>
       <c r="D358" s="4" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="E358" s="3">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F358" s="4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="G358" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H358" s="3"/>
       <c r="I358" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J358" s="4" t="s">
         <v>1133</v>
@@ -28574,16 +28585,16 @@
         <v>1133</v>
       </c>
       <c r="L358" s="3" t="s">
-        <v>418</v>
+        <v>1133</v>
       </c>
       <c r="M358" s="4" t="s">
-        <v>1188</v>
+        <v>1133</v>
       </c>
       <c r="N358" s="3">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="O358" s="4" t="s">
-        <v>1227</v>
+        <v>1233</v>
       </c>
       <c r="P358" s="4" t="s">
         <v>1133</v>
@@ -28606,7 +28617,7 @@
     </row>
     <row r="359" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A359" s="4" t="s">
-        <v>1083</v>
+        <v>1082</v>
       </c>
       <c r="B359" s="4" t="s">
         <v>415</v>
@@ -28615,20 +28626,20 @@
         <v>6</v>
       </c>
       <c r="D359" s="4" t="s">
-        <v>380</v>
+        <v>360</v>
       </c>
       <c r="E359" s="3">
         <v>2018</v>
       </c>
       <c r="F359" s="4" t="s">
-        <v>381</v>
+        <v>58</v>
       </c>
       <c r="G359" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H359" s="3"/>
       <c r="I359" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J359" s="4" t="s">
         <v>1133</v>
@@ -28637,19 +28648,19 @@
         <v>1133</v>
       </c>
       <c r="L359" s="3" t="s">
-        <v>1133</v>
+        <v>418</v>
       </c>
       <c r="M359" s="4" t="s">
-        <v>1133</v>
+        <v>1188</v>
       </c>
       <c r="N359" s="3">
-        <v>129</v>
+        <v>108</v>
       </c>
       <c r="O359" s="4" t="s">
-        <v>1208</v>
+        <v>1227</v>
       </c>
       <c r="P359" s="4" t="s">
-        <v>1461</v>
+        <v>1133</v>
       </c>
       <c r="Q359" s="4" t="s">
         <v>1133</v>
@@ -28669,163 +28680,163 @@
     </row>
     <row r="360" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A360" s="4" t="s">
-        <v>1860</v>
-      </c>
-      <c r="B360" s="2" t="s">
+        <v>1083</v>
+      </c>
+      <c r="B360" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C360" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D360" s="2" t="s">
-        <v>1861</v>
+      <c r="D360" s="4" t="s">
+        <v>380</v>
       </c>
       <c r="E360" s="3">
         <v>2018</v>
       </c>
-      <c r="F360" s="5" t="s">
-        <v>1862</v>
-      </c>
-      <c r="G360" s="10" t="s">
-        <v>420</v>
-      </c>
-      <c r="I360" s="9" t="s">
-        <v>418</v>
-      </c>
-      <c r="N360" s="9">
-        <v>114</v>
+      <c r="F360" s="4" t="s">
+        <v>381</v>
+      </c>
+      <c r="G360" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="H360" s="3"/>
+      <c r="I360" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="J360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="K360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L360" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="M360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="N360" s="3">
+        <v>129</v>
       </c>
       <c r="O360" s="4" t="s">
-        <v>1220</v>
-      </c>
-      <c r="P360" t="s">
-        <v>1878</v>
-      </c>
-      <c r="Q360" t="s">
-        <v>1863</v>
-      </c>
-      <c r="R360" t="s">
-        <v>1873</v>
-      </c>
-      <c r="S360" t="s">
-        <v>1864</v>
-      </c>
-      <c r="T360" t="s">
-        <v>1874</v>
-      </c>
-      <c r="U360" t="s">
-        <v>1867</v>
+        <v>1208</v>
+      </c>
+      <c r="P360" s="4" t="s">
+        <v>1461</v>
+      </c>
+      <c r="Q360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="R360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="S360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="T360" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="U360" s="4" t="s">
+        <v>1133</v>
       </c>
     </row>
     <row r="361" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A361" s="4" t="s">
-        <v>1084</v>
-      </c>
-      <c r="B361" s="4" t="s">
+        <v>1860</v>
+      </c>
+      <c r="B361" s="2" t="s">
         <v>415</v>
       </c>
       <c r="C361" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D361" s="4" t="s">
-        <v>42</v>
+      <c r="D361" s="2" t="s">
+        <v>1861</v>
       </c>
       <c r="E361" s="3">
-        <v>1998</v>
-      </c>
-      <c r="F361" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="G361" s="3" t="s">
-        <v>420</v>
-      </c>
-      <c r="H361" s="3"/>
-      <c r="I361" s="3" t="s">
-        <v>418</v>
-      </c>
-      <c r="J361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="K361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="L361" s="3" t="s">
-        <v>1133</v>
-      </c>
-      <c r="M361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="N361" s="3">
-        <v>87</v>
+        <v>2018</v>
+      </c>
+      <c r="F361" s="5" t="s">
+        <v>1862</v>
+      </c>
+      <c r="G361" s="10" t="s">
+        <v>420</v>
+      </c>
+      <c r="I361" s="9" t="s">
+        <v>418</v>
+      </c>
+      <c r="N361" s="9">
+        <v>114</v>
       </c>
       <c r="O361" s="4" t="s">
-        <v>1219</v>
-      </c>
-      <c r="P361" s="4" t="s">
-        <v>1462</v>
-      </c>
-      <c r="Q361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="R361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="S361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="T361" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="U361" s="4" t="s">
-        <v>1133</v>
+        <v>1220</v>
+      </c>
+      <c r="P361" t="s">
+        <v>1878</v>
+      </c>
+      <c r="Q361" t="s">
+        <v>1863</v>
+      </c>
+      <c r="R361" t="s">
+        <v>1873</v>
+      </c>
+      <c r="S361" t="s">
+        <v>1864</v>
+      </c>
+      <c r="T361" t="s">
+        <v>1874</v>
+      </c>
+      <c r="U361" t="s">
+        <v>1867</v>
       </c>
     </row>
     <row r="362" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A362" s="4" t="s">
-        <v>1085</v>
+        <v>1084</v>
       </c>
       <c r="B362" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C362" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D362" s="4" t="s">
-        <v>515</v>
+        <v>42</v>
       </c>
       <c r="E362" s="3">
-        <v>2017</v>
+        <v>1998</v>
       </c>
       <c r="F362" s="4" t="s">
-        <v>516</v>
+        <v>43</v>
       </c>
       <c r="G362" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H362" s="3"/>
       <c r="I362" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J362" s="4" t="s">
-        <v>342</v>
+        <v>1133</v>
       </c>
       <c r="K362" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="L362" s="3" t="s">
-        <v>418</v>
+        <v>1133</v>
       </c>
       <c r="M362" s="4" t="s">
-        <v>1175</v>
+        <v>1133</v>
       </c>
       <c r="N362" s="3">
-        <v>140</v>
+        <v>87</v>
       </c>
       <c r="O362" s="4" t="s">
-        <v>1218</v>
+        <v>1219</v>
       </c>
       <c r="P362" s="4" t="s">
-        <v>1133</v>
+        <v>1462</v>
       </c>
       <c r="Q362" s="4" t="s">
         <v>1133</v>
@@ -28845,47 +28856,47 @@
     </row>
     <row r="363" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A363" s="4" t="s">
-        <v>1086</v>
+        <v>1085</v>
       </c>
       <c r="B363" s="4" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C363" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D363" s="4" t="s">
-        <v>526</v>
+        <v>515</v>
       </c>
       <c r="E363" s="3">
-        <v>2019</v>
+        <v>2017</v>
       </c>
       <c r="F363" s="4" t="s">
-        <v>531</v>
+        <v>516</v>
       </c>
       <c r="G363" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H363" s="3"/>
       <c r="I363" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J363" s="4" t="s">
-        <v>1133</v>
+        <v>342</v>
       </c>
       <c r="K363" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="L363" s="3" t="s">
-        <v>1133</v>
+        <v>418</v>
       </c>
       <c r="M363" s="4" t="s">
-        <v>1189</v>
+        <v>1175</v>
       </c>
       <c r="N363" s="3">
-        <v>56</v>
+        <v>140</v>
       </c>
       <c r="O363" s="4" t="s">
-        <v>1382</v>
+        <v>1218</v>
       </c>
       <c r="P363" s="4" t="s">
         <v>1133</v>
@@ -28908,22 +28919,22 @@
     </row>
     <row r="364" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A364" s="4" t="s">
-        <v>1087</v>
+        <v>1086</v>
       </c>
       <c r="B364" s="4" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C364" s="4" t="s">
         <v>6</v>
       </c>
       <c r="D364" s="4" t="s">
-        <v>38</v>
+        <v>526</v>
       </c>
       <c r="E364" s="3">
-        <v>2013</v>
+        <v>2019</v>
       </c>
       <c r="F364" s="4" t="s">
-        <v>39</v>
+        <v>531</v>
       </c>
       <c r="G364" s="3" t="s">
         <v>420</v>
@@ -28942,13 +28953,13 @@
         <v>1133</v>
       </c>
       <c r="M364" s="4" t="s">
-        <v>1133</v>
+        <v>1189</v>
       </c>
       <c r="N364" s="3">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="O364" s="4" t="s">
-        <v>1219</v>
+        <v>1382</v>
       </c>
       <c r="P364" s="4" t="s">
         <v>1133</v>
@@ -28971,7 +28982,7 @@
     </row>
     <row r="365" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A365" s="4" t="s">
-        <v>1088</v>
+        <v>1087</v>
       </c>
       <c r="B365" s="4" t="s">
         <v>415</v>
@@ -28980,13 +28991,13 @@
         <v>6</v>
       </c>
       <c r="D365" s="4" t="s">
-        <v>506</v>
+        <v>38</v>
       </c>
       <c r="E365" s="3">
-        <v>2019</v>
+        <v>2013</v>
       </c>
       <c r="F365" s="4" t="s">
-        <v>505</v>
+        <v>39</v>
       </c>
       <c r="G365" s="3" t="s">
         <v>420</v>
@@ -29008,48 +29019,48 @@
         <v>1133</v>
       </c>
       <c r="N365" s="3">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="O365" s="4" t="s">
-        <v>1220</v>
+        <v>1219</v>
       </c>
       <c r="P365" s="4" t="s">
-        <v>1663</v>
+        <v>1133</v>
       </c>
       <c r="Q365" s="4" t="s">
-        <v>1664</v>
+        <v>1133</v>
       </c>
       <c r="R365" s="4" t="s">
-        <v>1668</v>
+        <v>1133</v>
       </c>
       <c r="S365" s="4" t="s">
-        <v>1667</v>
+        <v>1133</v>
       </c>
       <c r="T365" s="4" t="s">
-        <v>1666</v>
+        <v>1133</v>
       </c>
       <c r="U365" s="4" t="s">
-        <v>1665</v>
+        <v>1133</v>
       </c>
     </row>
     <row r="366" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A366" s="4" t="s">
-        <v>1089</v>
+        <v>1088</v>
       </c>
       <c r="B366" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C366" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D366" s="4" t="s">
-        <v>232</v>
+        <v>506</v>
       </c>
       <c r="E366" s="3">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="F366" s="4" t="s">
-        <v>233</v>
+        <v>505</v>
       </c>
       <c r="G366" s="3" t="s">
         <v>420</v>
@@ -29071,48 +29082,48 @@
         <v>1133</v>
       </c>
       <c r="N366" s="3">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O366" s="4" t="s">
-        <v>1221</v>
+        <v>1220</v>
       </c>
       <c r="P366" s="4" t="s">
-        <v>1460</v>
+        <v>1663</v>
       </c>
       <c r="Q366" s="4" t="s">
-        <v>1133</v>
+        <v>1664</v>
       </c>
       <c r="R366" s="4" t="s">
-        <v>1133</v>
+        <v>1668</v>
       </c>
       <c r="S366" s="4" t="s">
-        <v>1133</v>
+        <v>1667</v>
       </c>
       <c r="T366" s="4" t="s">
-        <v>1133</v>
+        <v>1666</v>
       </c>
       <c r="U366" s="4" t="s">
-        <v>1133</v>
+        <v>1665</v>
       </c>
     </row>
     <row r="367" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A367" s="4" t="s">
-        <v>1090</v>
+        <v>1089</v>
       </c>
       <c r="B367" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C367" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D367" s="4" t="s">
-        <v>417</v>
+        <v>232</v>
       </c>
       <c r="E367" s="3">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="F367" s="4" t="s">
-        <v>31</v>
+        <v>233</v>
       </c>
       <c r="G367" s="3" t="s">
         <v>420</v>
@@ -29137,10 +29148,10 @@
         <v>107</v>
       </c>
       <c r="O367" s="4" t="s">
-        <v>1219</v>
+        <v>1221</v>
       </c>
       <c r="P367" s="4" t="s">
-        <v>1133</v>
+        <v>1460</v>
       </c>
       <c r="Q367" s="4" t="s">
         <v>1133</v>
@@ -29160,7 +29171,7 @@
     </row>
     <row r="368" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A368" s="4" t="s">
-        <v>1091</v>
+        <v>1090</v>
       </c>
       <c r="B368" s="4" t="s">
         <v>415</v>
@@ -29169,13 +29180,13 @@
         <v>6</v>
       </c>
       <c r="D368" s="4" t="s">
-        <v>74</v>
+        <v>417</v>
       </c>
       <c r="E368" s="3">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="F368" s="4" t="s">
-        <v>75</v>
+        <v>31</v>
       </c>
       <c r="G368" s="3" t="s">
         <v>420</v>
@@ -29197,10 +29208,10 @@
         <v>1133</v>
       </c>
       <c r="N368" s="3">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="O368" s="4" t="s">
-        <v>1222</v>
+        <v>1219</v>
       </c>
       <c r="P368" s="4" t="s">
         <v>1133</v>
@@ -29223,7 +29234,7 @@
     </row>
     <row r="369" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A369" s="4" t="s">
-        <v>1092</v>
+        <v>1091</v>
       </c>
       <c r="B369" s="4" t="s">
         <v>415</v>
@@ -29232,13 +29243,13 @@
         <v>6</v>
       </c>
       <c r="D369" s="4" t="s">
-        <v>372</v>
+        <v>74</v>
       </c>
       <c r="E369" s="3">
-        <v>2018</v>
+        <v>2014</v>
       </c>
       <c r="F369" s="4" t="s">
-        <v>373</v>
+        <v>75</v>
       </c>
       <c r="G369" s="3" t="s">
         <v>420</v>
@@ -29260,10 +29271,10 @@
         <v>1133</v>
       </c>
       <c r="N369" s="3">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="O369" s="4" t="s">
-        <v>1223</v>
+        <v>1222</v>
       </c>
       <c r="P369" s="4" t="s">
         <v>1133</v>
@@ -29286,25 +29297,25 @@
     </row>
     <row r="370" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A370" s="4" t="s">
-        <v>1093</v>
+        <v>1092</v>
       </c>
       <c r="B370" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C370" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D370" s="4" t="s">
-        <v>357</v>
+        <v>372</v>
       </c>
       <c r="E370" s="3">
         <v>2018</v>
       </c>
       <c r="F370" s="4" t="s">
-        <v>358</v>
+        <v>373</v>
       </c>
       <c r="G370" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H370" s="3"/>
       <c r="I370" s="3" t="s">
@@ -29323,10 +29334,10 @@
         <v>1133</v>
       </c>
       <c r="N370" s="3">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="O370" s="4" t="s">
-        <v>1224</v>
+        <v>1223</v>
       </c>
       <c r="P370" s="4" t="s">
         <v>1133</v>
@@ -29349,22 +29360,22 @@
     </row>
     <row r="371" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A371" s="4" t="s">
-        <v>1094</v>
+        <v>1093</v>
       </c>
       <c r="B371" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C371" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D371" s="4" t="s">
-        <v>562</v>
+        <v>357</v>
       </c>
       <c r="E371" s="3">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F371" s="4" t="s">
-        <v>563</v>
+        <v>358</v>
       </c>
       <c r="G371" s="3" t="s">
         <v>418</v>
@@ -29386,10 +29397,10 @@
         <v>1133</v>
       </c>
       <c r="N371" s="3">
-        <v>103</v>
+        <v>109</v>
       </c>
       <c r="O371" s="4" t="s">
-        <v>1220</v>
+        <v>1224</v>
       </c>
       <c r="P371" s="4" t="s">
         <v>1133</v>
@@ -29412,7 +29423,7 @@
     </row>
     <row r="372" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A372" s="4" t="s">
-        <v>1095</v>
+        <v>1094</v>
       </c>
       <c r="B372" s="4" t="s">
         <v>415</v>
@@ -29421,38 +29432,38 @@
         <v>6</v>
       </c>
       <c r="D372" s="4" t="s">
-        <v>290</v>
+        <v>562</v>
       </c>
       <c r="E372" s="3">
         <v>2017</v>
       </c>
       <c r="F372" s="4" t="s">
-        <v>291</v>
+        <v>563</v>
       </c>
       <c r="G372" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H372" s="3"/>
       <c r="I372" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J372" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="K372" s="4" t="s">
-        <v>509</v>
+        <v>1133</v>
       </c>
       <c r="L372" s="3" t="s">
-        <v>420</v>
+        <v>1133</v>
       </c>
       <c r="M372" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N372" s="3">
-        <v>135</v>
+        <v>103</v>
       </c>
       <c r="O372" s="4" t="s">
-        <v>1226</v>
+        <v>1220</v>
       </c>
       <c r="P372" s="4" t="s">
         <v>1133</v>
@@ -29475,35 +29486,35 @@
     </row>
     <row r="373" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A373" s="4" t="s">
-        <v>1096</v>
+        <v>1095</v>
       </c>
       <c r="B373" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C373" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D373" s="4" t="s">
-        <v>509</v>
+        <v>290</v>
       </c>
       <c r="E373" s="3">
-        <v>2020</v>
+        <v>2017</v>
       </c>
       <c r="F373" s="4" t="s">
         <v>291</v>
       </c>
       <c r="G373" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="H373" s="3"/>
       <c r="I373" s="3" t="s">
         <v>420</v>
       </c>
       <c r="J373" s="4" t="s">
-        <v>290</v>
+        <v>1133</v>
       </c>
       <c r="K373" s="4" t="s">
-        <v>1133</v>
+        <v>509</v>
       </c>
       <c r="L373" s="3" t="s">
         <v>420</v>
@@ -29512,7 +29523,7 @@
         <v>1133</v>
       </c>
       <c r="N373" s="3">
-        <v>153</v>
+        <v>135</v>
       </c>
       <c r="O373" s="4" t="s">
         <v>1226</v>
@@ -29538,47 +29549,47 @@
     </row>
     <row r="374" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A374" s="4" t="s">
-        <v>1097</v>
+        <v>1096</v>
       </c>
       <c r="B374" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C374" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D374" s="4" t="s">
-        <v>61</v>
+        <v>509</v>
       </c>
       <c r="E374" s="3">
-        <v>2013</v>
+        <v>2020</v>
       </c>
       <c r="F374" s="4" t="s">
-        <v>62</v>
+        <v>291</v>
       </c>
       <c r="G374" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H374" s="3"/>
       <c r="I374" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J374" s="4" t="s">
-        <v>1133</v>
+        <v>290</v>
       </c>
       <c r="K374" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="L374" s="3" t="s">
-        <v>1133</v>
+        <v>420</v>
       </c>
       <c r="M374" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N374" s="3">
-        <v>112</v>
+        <v>153</v>
       </c>
       <c r="O374" s="4" t="s">
-        <v>1225</v>
+        <v>1226</v>
       </c>
       <c r="P374" s="4" t="s">
         <v>1133</v>
@@ -29601,7 +29612,7 @@
     </row>
     <row r="375" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A375" s="4" t="s">
-        <v>1098</v>
+        <v>1097</v>
       </c>
       <c r="B375" s="4" t="s">
         <v>415</v>
@@ -29610,38 +29621,38 @@
         <v>6</v>
       </c>
       <c r="D375" s="4" t="s">
-        <v>125</v>
+        <v>61</v>
       </c>
       <c r="E375" s="3">
-        <v>2000</v>
+        <v>2013</v>
       </c>
       <c r="F375" s="4" t="s">
-        <v>120</v>
+        <v>62</v>
       </c>
       <c r="G375" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H375" s="3"/>
       <c r="I375" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J375" s="4" t="s">
-        <v>722</v>
+        <v>1133</v>
       </c>
       <c r="K375" s="4" t="s">
-        <v>723</v>
+        <v>1133</v>
       </c>
       <c r="L375" s="3" t="s">
-        <v>420</v>
+        <v>1133</v>
       </c>
       <c r="M375" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N375" s="3">
-        <v>100</v>
+        <v>112</v>
       </c>
       <c r="O375" s="4" t="s">
-        <v>1227</v>
+        <v>1225</v>
       </c>
       <c r="P375" s="4" t="s">
         <v>1133</v>
@@ -29664,7 +29675,7 @@
     </row>
     <row r="376" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A376" s="4" t="s">
-        <v>1099</v>
+        <v>1098</v>
       </c>
       <c r="B376" s="4" t="s">
         <v>415</v>
@@ -29673,10 +29684,10 @@
         <v>6</v>
       </c>
       <c r="D376" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E376" s="3">
-        <v>2003</v>
+        <v>2000</v>
       </c>
       <c r="F376" s="4" t="s">
         <v>120</v>
@@ -29689,10 +29700,10 @@
         <v>420</v>
       </c>
       <c r="J376" s="4" t="s">
-        <v>720</v>
+        <v>722</v>
       </c>
       <c r="K376" s="4" t="s">
-        <v>721</v>
+        <v>723</v>
       </c>
       <c r="L376" s="3" t="s">
         <v>420</v>
@@ -29701,7 +29712,7 @@
         <v>1133</v>
       </c>
       <c r="N376" s="3">
-        <v>128</v>
+        <v>100</v>
       </c>
       <c r="O376" s="4" t="s">
         <v>1227</v>
@@ -29727,7 +29738,7 @@
     </row>
     <row r="377" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A377" s="4" t="s">
-        <v>1100</v>
+        <v>1099</v>
       </c>
       <c r="B377" s="4" t="s">
         <v>415</v>
@@ -29736,10 +29747,10 @@
         <v>6</v>
       </c>
       <c r="D377" s="4" t="s">
-        <v>119</v>
+        <v>126</v>
       </c>
       <c r="E377" s="3">
-        <v>2016</v>
+        <v>2003</v>
       </c>
       <c r="F377" s="4" t="s">
         <v>120</v>
@@ -29752,10 +29763,10 @@
         <v>420</v>
       </c>
       <c r="J377" s="4" t="s">
-        <v>718</v>
+        <v>720</v>
       </c>
       <c r="K377" s="4" t="s">
-        <v>719</v>
+        <v>721</v>
       </c>
       <c r="L377" s="3" t="s">
         <v>420</v>
@@ -29764,7 +29775,7 @@
         <v>1133</v>
       </c>
       <c r="N377" s="3">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="O377" s="4" t="s">
         <v>1227</v>
@@ -29790,7 +29801,7 @@
     </row>
     <row r="378" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A378" s="4" t="s">
-        <v>1101</v>
+        <v>1100</v>
       </c>
       <c r="B378" s="4" t="s">
         <v>415</v>
@@ -29799,13 +29810,13 @@
         <v>6</v>
       </c>
       <c r="D378" s="4" t="s">
-        <v>477</v>
+        <v>119</v>
       </c>
       <c r="E378" s="3">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="F378" s="4" t="s">
-        <v>479</v>
+        <v>120</v>
       </c>
       <c r="G378" s="3" t="s">
         <v>420</v>
@@ -29815,10 +29826,10 @@
         <v>420</v>
       </c>
       <c r="J378" s="4" t="s">
-        <v>716</v>
+        <v>718</v>
       </c>
       <c r="K378" s="4" t="s">
-        <v>717</v>
+        <v>719</v>
       </c>
       <c r="L378" s="3" t="s">
         <v>420</v>
@@ -29827,7 +29838,7 @@
         <v>1133</v>
       </c>
       <c r="N378" s="3">
-        <v>109</v>
+        <v>138</v>
       </c>
       <c r="O378" s="4" t="s">
         <v>1227</v>
@@ -29853,7 +29864,7 @@
     </row>
     <row r="379" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A379" s="4" t="s">
-        <v>1102</v>
+        <v>1101</v>
       </c>
       <c r="B379" s="4" t="s">
         <v>415</v>
@@ -29862,13 +29873,13 @@
         <v>6</v>
       </c>
       <c r="D379" s="4" t="s">
-        <v>121</v>
+        <v>477</v>
       </c>
       <c r="E379" s="3">
-        <v>2014</v>
+        <v>2019</v>
       </c>
       <c r="F379" s="4" t="s">
-        <v>120</v>
+        <v>479</v>
       </c>
       <c r="G379" s="3" t="s">
         <v>420</v>
@@ -29878,10 +29889,10 @@
         <v>420</v>
       </c>
       <c r="J379" s="4" t="s">
-        <v>122</v>
+        <v>716</v>
       </c>
       <c r="K379" s="4" t="s">
-        <v>715</v>
+        <v>717</v>
       </c>
       <c r="L379" s="3" t="s">
         <v>420</v>
@@ -29890,7 +29901,7 @@
         <v>1133</v>
       </c>
       <c r="N379" s="3">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="O379" s="4" t="s">
         <v>1227</v>
@@ -29916,7 +29927,7 @@
     </row>
     <row r="380" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A380" s="4" t="s">
-        <v>1103</v>
+        <v>1102</v>
       </c>
       <c r="B380" s="4" t="s">
         <v>415</v>
@@ -29925,13 +29936,13 @@
         <v>6</v>
       </c>
       <c r="D380" s="4" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E380" s="3">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="F380" s="4" t="s">
-        <v>83</v>
+        <v>120</v>
       </c>
       <c r="G380" s="3" t="s">
         <v>420</v>
@@ -29941,10 +29952,10 @@
         <v>420</v>
       </c>
       <c r="J380" s="4" t="s">
-        <v>1133</v>
+        <v>122</v>
       </c>
       <c r="K380" s="4" t="s">
-        <v>713</v>
+        <v>715</v>
       </c>
       <c r="L380" s="3" t="s">
         <v>420</v>
@@ -29979,7 +29990,7 @@
     </row>
     <row r="381" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A381" s="4" t="s">
-        <v>1104</v>
+        <v>1103</v>
       </c>
       <c r="B381" s="4" t="s">
         <v>415</v>
@@ -29988,13 +29999,13 @@
         <v>6</v>
       </c>
       <c r="D381" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E381" s="3">
-        <v>2006</v>
+        <v>2011</v>
       </c>
       <c r="F381" s="4" t="s">
-        <v>124</v>
+        <v>83</v>
       </c>
       <c r="G381" s="3" t="s">
         <v>420</v>
@@ -30004,10 +30015,10 @@
         <v>420</v>
       </c>
       <c r="J381" s="4" t="s">
-        <v>714</v>
+        <v>1133</v>
       </c>
       <c r="K381" s="4" t="s">
-        <v>1133</v>
+        <v>713</v>
       </c>
       <c r="L381" s="3" t="s">
         <v>420</v>
@@ -30016,7 +30027,7 @@
         <v>1133</v>
       </c>
       <c r="N381" s="3">
-        <v>100</v>
+        <v>126</v>
       </c>
       <c r="O381" s="4" t="s">
         <v>1227</v>
@@ -30042,47 +30053,47 @@
     </row>
     <row r="382" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A382" s="4" t="s">
-        <v>1105</v>
+        <v>1104</v>
       </c>
       <c r="B382" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C382" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D382" s="4" t="s">
-        <v>514</v>
+        <v>123</v>
       </c>
       <c r="E382" s="3">
-        <v>2015</v>
+        <v>2006</v>
       </c>
       <c r="F382" s="4" t="s">
-        <v>517</v>
+        <v>124</v>
       </c>
       <c r="G382" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H382" s="3"/>
       <c r="I382" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J382" s="4" t="s">
-        <v>1133</v>
+        <v>714</v>
       </c>
       <c r="K382" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="L382" s="3" t="s">
-        <v>1133</v>
+        <v>420</v>
       </c>
       <c r="M382" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N382" s="3">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="O382" s="4" t="s">
-        <v>1228</v>
+        <v>1227</v>
       </c>
       <c r="P382" s="4" t="s">
         <v>1133</v>
@@ -30105,7 +30116,7 @@
     </row>
     <row r="383" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A383" s="4" t="s">
-        <v>1106</v>
+        <v>1105</v>
       </c>
       <c r="B383" s="4" t="s">
         <v>415</v>
@@ -30114,13 +30125,13 @@
         <v>48</v>
       </c>
       <c r="D383" s="4" t="s">
-        <v>522</v>
+        <v>514</v>
       </c>
       <c r="E383" s="3">
-        <v>2012</v>
+        <v>2015</v>
       </c>
       <c r="F383" s="4" t="s">
-        <v>523</v>
+        <v>517</v>
       </c>
       <c r="G383" s="3" t="s">
         <v>420</v>
@@ -30142,13 +30153,13 @@
         <v>1133</v>
       </c>
       <c r="N383" s="3">
-        <v>157</v>
+        <v>98</v>
       </c>
       <c r="O383" s="4" t="s">
-        <v>1229</v>
+        <v>1228</v>
       </c>
       <c r="P383" s="4" t="s">
-        <v>1458</v>
+        <v>1133</v>
       </c>
       <c r="Q383" s="4" t="s">
         <v>1133</v>
@@ -30168,50 +30179,50 @@
     </row>
     <row r="384" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A384" s="4" t="s">
-        <v>1107</v>
+        <v>1106</v>
       </c>
       <c r="B384" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C384" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D384" s="4" t="s">
-        <v>57</v>
+        <v>522</v>
       </c>
       <c r="E384" s="3">
-        <v>2009</v>
+        <v>2012</v>
       </c>
       <c r="F384" s="4" t="s">
-        <v>58</v>
+        <v>523</v>
       </c>
       <c r="G384" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H384" s="3"/>
       <c r="I384" s="3" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="J384" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="K384" s="4" t="s">
-        <v>359</v>
+        <v>1133</v>
       </c>
       <c r="L384" s="3" t="s">
-        <v>420</v>
+        <v>1133</v>
       </c>
       <c r="M384" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N384" s="3">
-        <v>84</v>
+        <v>157</v>
       </c>
       <c r="O384" s="4" t="s">
-        <v>1230</v>
+        <v>1229</v>
       </c>
       <c r="P384" s="4" t="s">
-        <v>1133</v>
+        <v>1458</v>
       </c>
       <c r="Q384" s="4" t="s">
         <v>1133</v>
@@ -30231,19 +30242,19 @@
     </row>
     <row r="385" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A385" s="4" t="s">
-        <v>1108</v>
+        <v>1107</v>
       </c>
       <c r="B385" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C385" s="4" t="s">
-        <v>48</v>
+        <v>6</v>
       </c>
       <c r="D385" s="4" t="s">
-        <v>359</v>
+        <v>57</v>
       </c>
       <c r="E385" s="3">
-        <v>2019</v>
+        <v>2009</v>
       </c>
       <c r="F385" s="4" t="s">
         <v>58</v>
@@ -30256,10 +30267,10 @@
         <v>420</v>
       </c>
       <c r="J385" s="4" t="s">
-        <v>57</v>
+        <v>1133</v>
       </c>
       <c r="K385" s="4" t="s">
-        <v>1133</v>
+        <v>359</v>
       </c>
       <c r="L385" s="3" t="s">
         <v>420</v>
@@ -30268,7 +30279,7 @@
         <v>1133</v>
       </c>
       <c r="N385" s="3">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="O385" s="4" t="s">
         <v>1230</v>
@@ -30294,70 +30305,133 @@
     </row>
     <row r="386" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A386" s="4" t="s">
-        <v>1109</v>
+        <v>1108</v>
       </c>
       <c r="B386" s="4" t="s">
         <v>415</v>
       </c>
       <c r="C386" s="4" t="s">
-        <v>6</v>
+        <v>48</v>
       </c>
       <c r="D386" s="4" t="s">
-        <v>244</v>
+        <v>359</v>
       </c>
       <c r="E386" s="3">
-        <v>2016</v>
+        <v>2019</v>
       </c>
       <c r="F386" s="4" t="s">
-        <v>245</v>
+        <v>58</v>
       </c>
       <c r="G386" s="3" t="s">
         <v>420</v>
       </c>
       <c r="H386" s="3"/>
       <c r="I386" s="3" t="s">
-        <v>418</v>
+        <v>420</v>
       </c>
       <c r="J386" s="4" t="s">
-        <v>1133</v>
+        <v>57</v>
       </c>
       <c r="K386" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="L386" s="3" t="s">
-        <v>1133</v>
+        <v>420</v>
       </c>
       <c r="M386" s="4" t="s">
         <v>1133</v>
       </c>
       <c r="N386" s="3">
+        <v>99</v>
+      </c>
+      <c r="O386" s="4" t="s">
+        <v>1230</v>
+      </c>
+      <c r="P386" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Q386" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="R386" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="S386" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="T386" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="U386" s="4" t="s">
+        <v>1133</v>
+      </c>
+    </row>
+    <row r="387" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A387" s="4" t="s">
+        <v>1109</v>
+      </c>
+      <c r="B387" s="4" t="s">
+        <v>415</v>
+      </c>
+      <c r="C387" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D387" s="4" t="s">
+        <v>244</v>
+      </c>
+      <c r="E387" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F387" s="4" t="s">
+        <v>245</v>
+      </c>
+      <c r="G387" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="H387" s="3"/>
+      <c r="I387" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="J387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="K387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="L387" s="3" t="s">
+        <v>1133</v>
+      </c>
+      <c r="M387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="N387" s="3">
         <v>104</v>
       </c>
-      <c r="O386" s="4" t="s">
+      <c r="O387" s="4" t="s">
         <v>1231</v>
       </c>
-      <c r="P386" s="4" t="s">
+      <c r="P387" s="4" t="s">
         <v>1459</v>
       </c>
-      <c r="Q386" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="R386" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="S386" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="T386" s="4" t="s">
-        <v>1133</v>
-      </c>
-      <c r="U386" s="4" t="s">
+      <c r="Q387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="R387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="S387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="T387" s="4" t="s">
+        <v>1133</v>
+      </c>
+      <c r="U387" s="4" t="s">
         <v>1133</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:U384" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U386">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U387">
       <sortCondition ref="D1:D384"/>
     </sortState>
   </autoFilter>

</xml_diff>

<commit_message>
eyd update 2025 my favorite cake, the apprentice
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29FB83FD-09C5-49B5-8A34-8E832980048F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D09949F-FDA5-4A7D-802E-FBB8DCA6C582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7037" uniqueCount="1947">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7062" uniqueCount="1961">
   <si>
     <t>ID</t>
   </si>
@@ -5880,6 +5880,48 @@
   </si>
   <si>
     <t>Michael Keaton, Zach Galifianakis, Edward Norton, Andrea Riseborough, Emma Stone, Naomi Watts, Merritt Wever, Amy Ryan</t>
+  </si>
+  <si>
+    <t>The Apprentice</t>
+  </si>
+  <si>
+    <t>My Favorite Cake</t>
+  </si>
+  <si>
+    <t>My_Favorite_Cake_2024</t>
+  </si>
+  <si>
+    <t>The_Apprentice_2024</t>
+  </si>
+  <si>
+    <t>Ali Abbasi</t>
+  </si>
+  <si>
+    <t>Maryam Moghadam, Behtash Sanaeeha</t>
+  </si>
+  <si>
+    <t>Gabriel Sherman</t>
+  </si>
+  <si>
+    <t>Sebastian Stan, Jeremy Strong, Martin Donovan, Maria Bakalova, Catherine McNally, Charlie Carrick, Ben Sullivan, Mark Rendall, Joe Pingue</t>
+  </si>
+  <si>
+    <t>Martin Dirkov, David Holmes, Brian Irvine</t>
+  </si>
+  <si>
+    <t>Kasper Tuxen</t>
+  </si>
+  <si>
+    <t>Laura Montgomery</t>
+  </si>
+  <si>
+    <t>Lili Farhadpour, Esmaeel Mehrabi, Mansoore Ilkhani, Soraya Orang, Homa Mottahedin, Sima Esmaeili</t>
+  </si>
+  <si>
+    <t>Mohamad Hadidi</t>
+  </si>
+  <si>
+    <t>Maryam Moghadam</t>
   </si>
 </sst>
 </file>
@@ -5923,7 +5965,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -5959,7 +6001,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -6274,11 +6315,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U394"/>
+  <dimension ref="A1:U396"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -23184,7 +23225,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="270" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A270" s="4" t="s">
         <v>1386</v>
       </c>
@@ -23247,7 +23288,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="271" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A271" s="4" t="s">
         <v>1390</v>
       </c>
@@ -23310,7 +23351,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="272" spans="1:21" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A272" s="4" t="s">
         <v>1393</v>
       </c>
@@ -26810,20 +26851,19 @@
       <c r="O328" s="4" t="s">
         <v>1922</v>
       </c>
-      <c r="P328" s="13"/>
-      <c r="Q328" s="13" t="s">
+      <c r="Q328" t="s">
         <v>1923</v>
       </c>
-      <c r="R328" s="13" t="s">
+      <c r="R328" t="s">
         <v>1925</v>
       </c>
-      <c r="S328" s="13" t="s">
+      <c r="S328" t="s">
         <v>1926</v>
       </c>
-      <c r="T328" s="13" t="s">
+      <c r="T328" t="s">
         <v>1927</v>
       </c>
-      <c r="U328" s="13" t="s">
+      <c r="U328" t="s">
         <v>1924</v>
       </c>
     </row>
@@ -26867,20 +26907,19 @@
       <c r="O329" s="4" t="s">
         <v>1922</v>
       </c>
-      <c r="P329" s="13"/>
-      <c r="Q329" s="13" t="s">
+      <c r="Q329" t="s">
         <v>1923</v>
       </c>
-      <c r="R329" s="13" t="s">
+      <c r="R329" t="s">
         <v>1925</v>
       </c>
-      <c r="S329" s="13" t="s">
+      <c r="S329" t="s">
         <v>1926</v>
       </c>
-      <c r="T329" s="13" t="s">
+      <c r="T329" t="s">
         <v>1927</v>
       </c>
-      <c r="U329" s="13" t="s">
+      <c r="U329" t="s">
         <v>1934</v>
       </c>
     </row>
@@ -26926,20 +26965,19 @@
       <c r="O330" s="4" t="s">
         <v>1922</v>
       </c>
-      <c r="P330" s="13"/>
-      <c r="Q330" s="13" t="s">
+      <c r="Q330" t="s">
         <v>1923</v>
       </c>
-      <c r="R330" s="13" t="s">
+      <c r="R330" t="s">
         <v>1925</v>
       </c>
-      <c r="S330" s="13" t="s">
+      <c r="S330" t="s">
         <v>1926</v>
       </c>
-      <c r="T330" s="13" t="s">
+      <c r="T330" t="s">
         <v>1927</v>
       </c>
-      <c r="U330" s="13" t="s">
+      <c r="U330" t="s">
         <v>1931</v>
       </c>
     </row>
@@ -30942,6 +30980,97 @@
       </c>
       <c r="U394" s="4" t="s">
         <v>28</v>
+      </c>
+    </row>
+    <row r="395" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A395" s="4" t="s">
+        <v>1950</v>
+      </c>
+      <c r="B395" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C395" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D395" s="2" t="s">
+        <v>1947</v>
+      </c>
+      <c r="E395" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F395" s="5" t="s">
+        <v>1951</v>
+      </c>
+      <c r="G395" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I395" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N395" s="9">
+        <v>122</v>
+      </c>
+      <c r="O395" s="4" t="s">
+        <v>1643</v>
+      </c>
+      <c r="Q395" t="s">
+        <v>1953</v>
+      </c>
+      <c r="R395" t="s">
+        <v>1955</v>
+      </c>
+      <c r="S395" t="s">
+        <v>1956</v>
+      </c>
+      <c r="T395" t="s">
+        <v>1957</v>
+      </c>
+      <c r="U395" t="s">
+        <v>1954</v>
+      </c>
+    </row>
+    <row r="396" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A396" s="4" t="s">
+        <v>1949</v>
+      </c>
+      <c r="B396" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C396" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D396" s="2" t="s">
+        <v>1948</v>
+      </c>
+      <c r="E396" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F396" s="5" t="s">
+        <v>1952</v>
+      </c>
+      <c r="G396" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I396" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N396" s="9">
+        <v>97</v>
+      </c>
+      <c r="O396" s="4" t="s">
+        <v>1905</v>
+      </c>
+      <c r="R396" s="5" t="s">
+        <v>1952</v>
+      </c>
+      <c r="S396" t="s">
+        <v>1959</v>
+      </c>
+      <c r="T396" t="s">
+        <v>1960</v>
+      </c>
+      <c r="U396" t="s">
+        <v>1958</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
birthday and london update
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D09949F-FDA5-4A7D-802E-FBB8DCA6C582}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AF06B7-6010-4840-9677-CF70A95EA1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7062" uniqueCount="1961">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7253" uniqueCount="2070">
   <si>
     <t>ID</t>
   </si>
@@ -5922,6 +5922,333 @@
   </si>
   <si>
     <t>Maryam Moghadam</t>
+  </si>
+  <si>
+    <t>Duel_1971</t>
+  </si>
+  <si>
+    <t>Duel</t>
+  </si>
+  <si>
+    <t>Richard Matheson</t>
+  </si>
+  <si>
+    <t>Dennis Weaver, Jacqueline Scott, Eddie Firestone, Lou Frizzell, Gene Dynarski, Lucille Benson</t>
+  </si>
+  <si>
+    <t>Billy Goldenberg</t>
+  </si>
+  <si>
+    <t>Jack A. Marta</t>
+  </si>
+  <si>
+    <t>Robert S. Smith (Art Director)</t>
+  </si>
+  <si>
+    <t>The_Last_Emperor_1987</t>
+  </si>
+  <si>
+    <t>The Last Emperor</t>
+  </si>
+  <si>
+    <t>Bernardo Bertolucci</t>
+  </si>
+  <si>
+    <t>John Lone, Joan Chen, Peter O'Toole, Ruocheng Ying, Victor Wong, Dennis Dun, Ryuichi Sakamoto, Maggie Han</t>
+  </si>
+  <si>
+    <t>Enzo Ungari, Mark Peploe, Bernardo Bertolucci</t>
+  </si>
+  <si>
+    <t>David Byrne, Ryuichi Sakamoto, Cong Su</t>
+  </si>
+  <si>
+    <t>Vittorio Storaro</t>
+  </si>
+  <si>
+    <t>James Acheson</t>
+  </si>
+  <si>
+    <t>The_Zone_Of_Interest_2023</t>
+  </si>
+  <si>
+    <t>The Zone of Interest</t>
+  </si>
+  <si>
+    <t>Jonathan Glazer</t>
+  </si>
+  <si>
+    <t>Drama, History, War</t>
+  </si>
+  <si>
+    <t>Jonathan Glazer, Martin Amis</t>
+  </si>
+  <si>
+    <t>Mica Levi</t>
+  </si>
+  <si>
+    <t>Lukasz Zal</t>
+  </si>
+  <si>
+    <t>Malgorzata Karpiuk</t>
+  </si>
+  <si>
+    <t>Christian Friedel, Sandra Hüller, Johann Karthaus, Luis Noah Witte, Nele Ahrensmeier, Lilli Falk, Max Beck</t>
+  </si>
+  <si>
+    <t>Marcel the Shell with Shoes on</t>
+  </si>
+  <si>
+    <t>Marcel_The_Shell_With_Shoes_On_2021</t>
+  </si>
+  <si>
+    <t>Dean Fleischer Camp</t>
+  </si>
+  <si>
+    <t>Animation, Comedy, Biography</t>
+  </si>
+  <si>
+    <t>Dean Fleischer Camp, Jenny Slate, Nick Paley</t>
+  </si>
+  <si>
+    <t>Disasterpeace</t>
+  </si>
+  <si>
+    <t>Eric Adkins, Bianca Cline</t>
+  </si>
+  <si>
+    <t>Jamie Catino</t>
+  </si>
+  <si>
+    <t>Jenny Slate, Dean Fleischer Camp, Isabella Rossellini, Joe Gabler</t>
+  </si>
+  <si>
+    <t>The_Outfit_2022</t>
+  </si>
+  <si>
+    <t>The Outfit</t>
+  </si>
+  <si>
+    <t>Graham Moore</t>
+  </si>
+  <si>
+    <t>Crime, Thriller, Drama</t>
+  </si>
+  <si>
+    <t>Graham Moore, Jonathan McClain</t>
+  </si>
+  <si>
+    <t>Mark Rylance, Zoey Deutch, Dylan O'Brien, Johnny Flynn, Simon Russell Beale, Alan Mehdizadeh</t>
+  </si>
+  <si>
+    <t>Dick Pope</t>
+  </si>
+  <si>
+    <t>Sophie O'Neill, Zac Posen</t>
+  </si>
+  <si>
+    <t>Cocaine_Bear_2023</t>
+  </si>
+  <si>
+    <t>Cocaine Bear</t>
+  </si>
+  <si>
+    <t>Jimmy Warden</t>
+  </si>
+  <si>
+    <t>Keri Russell, Alden Ehrenreich, O'Shea Jackson Jr., Ray Liotta, Isiah Whitlock Jr., Brooklyn Prince, Christian Convery, Margo Martindale, Jesse Tyler Ferguson, Matthew Rhys</t>
+  </si>
+  <si>
+    <t>Tiziana Corvisieri</t>
+  </si>
+  <si>
+    <t>West_Side_Story_1961</t>
+  </si>
+  <si>
+    <t>West Side Story</t>
+  </si>
+  <si>
+    <t>Jerome Robbins, Robert Wise</t>
+  </si>
+  <si>
+    <t>Musical, Drama, Romance</t>
+  </si>
+  <si>
+    <t>Ernest Lehman, Arthur Laurents, Jerome Robbins</t>
+  </si>
+  <si>
+    <t>Natalie Wood, George Chakiris, Richard Beymer, Russ Tamblyn, Rita Moreno, Simon Oakland, Ned Glass, William Bramley, Tucker Smith</t>
+  </si>
+  <si>
+    <t>Leonard Bernstein</t>
+  </si>
+  <si>
+    <t>Daniel L. Fapp</t>
+  </si>
+  <si>
+    <t>Irene Sharaff</t>
+  </si>
+  <si>
+    <t>The_Edge_of_Seventeen_2016</t>
+  </si>
+  <si>
+    <t>The Edge of Seventeen</t>
+  </si>
+  <si>
+    <t>Kelly Fremon Craig</t>
+  </si>
+  <si>
+    <t>Hailee Steinfeld, Haley Lu Richardson, Blake Jenner, Kyra Sedgwick, Woody Harrelson</t>
+  </si>
+  <si>
+    <t>Atli Örvarsson</t>
+  </si>
+  <si>
+    <t>Doug Emmett</t>
+  </si>
+  <si>
+    <t>Carla Hetland</t>
+  </si>
+  <si>
+    <t>Beetlejuice_1988</t>
+  </si>
+  <si>
+    <t>Beetlejuice</t>
+  </si>
+  <si>
+    <t>Beetlejuice Beetlejuice</t>
+  </si>
+  <si>
+    <t>Comedy, Fantasy, Seasonal</t>
+  </si>
+  <si>
+    <t>Michael McDowell, Larry Wilson, Warren Skaaren</t>
+  </si>
+  <si>
+    <t>Alec Baldwin, Geena Davis, Michael Keaton, Annie McEnroe, Marice Page, Hugo Stanger, Rachel Mittelman, Catherine O'Hara, Jeffrey Jones, Winona Ryder</t>
+  </si>
+  <si>
+    <t>Danny Elfman</t>
+  </si>
+  <si>
+    <t>Thomas E. Ackerman</t>
+  </si>
+  <si>
+    <t>Aggie Guerard Rodgers</t>
+  </si>
+  <si>
+    <t>Rumours_2024</t>
+  </si>
+  <si>
+    <t>Rumours</t>
+  </si>
+  <si>
+    <t>Evan Johnson, Galen Johnson, Guy Maddin</t>
+  </si>
+  <si>
+    <t>Comedy, Drama, Horror</t>
+  </si>
+  <si>
+    <t>Evan Johnson, Guy Maddin, Galen Johnson</t>
+  </si>
+  <si>
+    <t>Cate Blanchett, Roy Dupuis, Denis Ménochet, Charles Dance, Nikki Amuka-Bird, Rolando Ravello, Takehiro Hira, Alicia Vikander</t>
+  </si>
+  <si>
+    <t>Kristian Eidnes Andersen</t>
+  </si>
+  <si>
+    <t>Stefan Ciupek</t>
+  </si>
+  <si>
+    <t>Bina Daigeler</t>
+  </si>
+  <si>
+    <t>Willy_Wonka_and_The_Chocolate_Factory_1971</t>
+  </si>
+  <si>
+    <t>Willy Wonka &amp; the Chocolate Factory</t>
+  </si>
+  <si>
+    <t>Mel Stuart</t>
+  </si>
+  <si>
+    <t>Fantasy, Musical, Comedy</t>
+  </si>
+  <si>
+    <t>Roald Dahl, Robert Kaufman, David Seltzer</t>
+  </si>
+  <si>
+    <t>Gene Wilder, Jack Albertson, Peter Ostrum, Roy Kinnear, Julie Dawn Cole, Leonard Stone, Denise Nickerson, Nora Denney, Paris Themmen, Ursula Reit, Michael Bollner, Diana Sowle</t>
+  </si>
+  <si>
+    <t>Arthur Ibbetson</t>
+  </si>
+  <si>
+    <t>Helen Colvig</t>
+  </si>
+  <si>
+    <t>Leslie Bricusse</t>
+  </si>
+  <si>
+    <t>Before_Sunrise_1995</t>
+  </si>
+  <si>
+    <t>Before Sunrise</t>
+  </si>
+  <si>
+    <t>Before Sunset</t>
+  </si>
+  <si>
+    <t>Before Midnight</t>
+  </si>
+  <si>
+    <t>Richard Linklater, Kim Krizan</t>
+  </si>
+  <si>
+    <t>Ethan Hawke, Julie Delpy</t>
+  </si>
+  <si>
+    <t>Fred Frith</t>
+  </si>
+  <si>
+    <t>Lee Daniel</t>
+  </si>
+  <si>
+    <t>Florentina Welley</t>
+  </si>
+  <si>
+    <t>Before_Sunset_2004</t>
+  </si>
+  <si>
+    <t>Richard Linklater, Julie Delpy, Ethan Hawke</t>
+  </si>
+  <si>
+    <t>Thierry Delettre</t>
+  </si>
+  <si>
+    <t>Igor Kipnis</t>
+  </si>
+  <si>
+    <t>Operation_Mincemeat_2021</t>
+  </si>
+  <si>
+    <t>Operation Mincemeat</t>
+  </si>
+  <si>
+    <t>Drama, War</t>
+  </si>
+  <si>
+    <t>Michelle Ashford, Ben Macintyre</t>
+  </si>
+  <si>
+    <t>Colin Firth, Matthew Macfadyen, Kelly Macdonald, Rufus Wright, Ruby Bentall, Charlotte Hamblin, Simon Russell, Beale, Jason Isaacs, Alex Jennings</t>
+  </si>
+  <si>
+    <t>Sebastian Blenkov</t>
+  </si>
+  <si>
+    <t>Andrea Flesch</t>
   </si>
 </sst>
 </file>
@@ -6315,11 +6642,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U396"/>
+  <dimension ref="A1:U410"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L14" sqref="L14"/>
+    <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D406" sqref="D406"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -31073,6 +31400,691 @@
         <v>1958</v>
       </c>
     </row>
+    <row r="397" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A397" s="4" t="s">
+        <v>1961</v>
+      </c>
+      <c r="B397" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C397" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D397" s="2" t="s">
+        <v>1962</v>
+      </c>
+      <c r="E397" s="3">
+        <v>1971</v>
+      </c>
+      <c r="F397" s="5" t="s">
+        <v>750</v>
+      </c>
+      <c r="G397" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I397" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N397" s="9">
+        <v>90</v>
+      </c>
+      <c r="O397" s="4" t="s">
+        <v>1007</v>
+      </c>
+      <c r="Q397" t="s">
+        <v>1963</v>
+      </c>
+      <c r="R397" t="s">
+        <v>1965</v>
+      </c>
+      <c r="S397" t="s">
+        <v>1966</v>
+      </c>
+      <c r="T397" t="s">
+        <v>1967</v>
+      </c>
+      <c r="U397" t="s">
+        <v>1964</v>
+      </c>
+    </row>
+    <row r="398" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A398" s="4" t="s">
+        <v>1968</v>
+      </c>
+      <c r="B398" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C398" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D398" s="2" t="s">
+        <v>1969</v>
+      </c>
+      <c r="E398" s="3">
+        <v>1987</v>
+      </c>
+      <c r="F398" s="5" t="s">
+        <v>1970</v>
+      </c>
+      <c r="G398" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I398" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N398" s="9">
+        <v>163</v>
+      </c>
+      <c r="O398" s="4" t="s">
+        <v>1633</v>
+      </c>
+      <c r="Q398" t="s">
+        <v>1972</v>
+      </c>
+      <c r="R398" t="s">
+        <v>1973</v>
+      </c>
+      <c r="S398" t="s">
+        <v>1974</v>
+      </c>
+      <c r="T398" t="s">
+        <v>1975</v>
+      </c>
+      <c r="U398" t="s">
+        <v>1971</v>
+      </c>
+    </row>
+    <row r="399" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A399" s="4" t="s">
+        <v>1976</v>
+      </c>
+      <c r="B399" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C399" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D399" s="2" t="s">
+        <v>1977</v>
+      </c>
+      <c r="E399" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F399" s="5" t="s">
+        <v>1978</v>
+      </c>
+      <c r="G399" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I399" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N399" s="9">
+        <v>105</v>
+      </c>
+      <c r="O399" s="4" t="s">
+        <v>1979</v>
+      </c>
+      <c r="Q399" t="s">
+        <v>1980</v>
+      </c>
+      <c r="R399" t="s">
+        <v>1981</v>
+      </c>
+      <c r="S399" t="s">
+        <v>1982</v>
+      </c>
+      <c r="T399" t="s">
+        <v>1983</v>
+      </c>
+      <c r="U399" t="s">
+        <v>1984</v>
+      </c>
+    </row>
+    <row r="400" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A400" s="4" t="s">
+        <v>1986</v>
+      </c>
+      <c r="B400" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C400" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D400" s="2" t="s">
+        <v>1985</v>
+      </c>
+      <c r="E400" s="3">
+        <v>2021</v>
+      </c>
+      <c r="F400" s="5" t="s">
+        <v>1987</v>
+      </c>
+      <c r="G400" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I400" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N400" s="9">
+        <v>90</v>
+      </c>
+      <c r="O400" s="4" t="s">
+        <v>1988</v>
+      </c>
+      <c r="Q400" t="s">
+        <v>1989</v>
+      </c>
+      <c r="R400" t="s">
+        <v>1990</v>
+      </c>
+      <c r="S400" t="s">
+        <v>1991</v>
+      </c>
+      <c r="T400" t="s">
+        <v>1992</v>
+      </c>
+      <c r="U400" t="s">
+        <v>1993</v>
+      </c>
+    </row>
+    <row r="401" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A401" s="4" t="s">
+        <v>1994</v>
+      </c>
+      <c r="B401" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C401" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D401" s="2" t="s">
+        <v>1995</v>
+      </c>
+      <c r="E401" s="3">
+        <v>2022</v>
+      </c>
+      <c r="F401" s="5" t="s">
+        <v>1996</v>
+      </c>
+      <c r="G401" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I401" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N401" s="9">
+        <v>105</v>
+      </c>
+      <c r="O401" s="4" t="s">
+        <v>1997</v>
+      </c>
+      <c r="Q401" t="s">
+        <v>1998</v>
+      </c>
+      <c r="R401" t="s">
+        <v>147</v>
+      </c>
+      <c r="S401" t="s">
+        <v>2000</v>
+      </c>
+      <c r="T401" t="s">
+        <v>2001</v>
+      </c>
+      <c r="U401" t="s">
+        <v>1999</v>
+      </c>
+    </row>
+    <row r="402" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A402" s="4" t="s">
+        <v>2002</v>
+      </c>
+      <c r="B402" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C402" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D402" s="2" t="s">
+        <v>2003</v>
+      </c>
+      <c r="E402" s="3">
+        <v>2023</v>
+      </c>
+      <c r="F402" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="G402" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I402" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N402" s="9">
+        <v>95</v>
+      </c>
+      <c r="O402" s="4" t="s">
+        <v>1472</v>
+      </c>
+      <c r="Q402" t="s">
+        <v>2004</v>
+      </c>
+      <c r="R402" t="s">
+        <v>1175</v>
+      </c>
+      <c r="S402" t="s">
+        <v>635</v>
+      </c>
+      <c r="T402" t="s">
+        <v>2006</v>
+      </c>
+      <c r="U402" t="s">
+        <v>2005</v>
+      </c>
+    </row>
+    <row r="403" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A403" s="4" t="s">
+        <v>2007</v>
+      </c>
+      <c r="B403" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C403" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D403" s="2" t="s">
+        <v>2008</v>
+      </c>
+      <c r="E403" s="3">
+        <v>1961</v>
+      </c>
+      <c r="F403" s="5" t="s">
+        <v>2009</v>
+      </c>
+      <c r="G403" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I403" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N403" s="9">
+        <v>153</v>
+      </c>
+      <c r="O403" s="4" t="s">
+        <v>2010</v>
+      </c>
+      <c r="Q403" t="s">
+        <v>2011</v>
+      </c>
+      <c r="R403" t="s">
+        <v>2013</v>
+      </c>
+      <c r="S403" t="s">
+        <v>2014</v>
+      </c>
+      <c r="T403" t="s">
+        <v>2015</v>
+      </c>
+      <c r="U403" t="s">
+        <v>2012</v>
+      </c>
+    </row>
+    <row r="404" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A404" s="4" t="s">
+        <v>2016</v>
+      </c>
+      <c r="B404" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C404" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D404" s="2" t="s">
+        <v>2017</v>
+      </c>
+      <c r="E404" s="3">
+        <v>2016</v>
+      </c>
+      <c r="F404" s="5" t="s">
+        <v>2018</v>
+      </c>
+      <c r="G404" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I404" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N404" s="9">
+        <v>104</v>
+      </c>
+      <c r="O404" s="4" t="s">
+        <v>936</v>
+      </c>
+      <c r="Q404" t="s">
+        <v>2018</v>
+      </c>
+      <c r="R404" t="s">
+        <v>2020</v>
+      </c>
+      <c r="S404" t="s">
+        <v>2021</v>
+      </c>
+      <c r="T404" t="s">
+        <v>2022</v>
+      </c>
+      <c r="U404" t="s">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="405" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A405" s="4" t="s">
+        <v>2023</v>
+      </c>
+      <c r="B405" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C405" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D405" s="2" t="s">
+        <v>2024</v>
+      </c>
+      <c r="E405" s="3">
+        <v>1988</v>
+      </c>
+      <c r="F405" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="G405" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I405" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K405" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="L405" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M405" s="6" t="s">
+        <v>2025</v>
+      </c>
+      <c r="N405" s="9">
+        <v>92</v>
+      </c>
+      <c r="O405" s="4" t="s">
+        <v>2026</v>
+      </c>
+      <c r="Q405" t="s">
+        <v>2027</v>
+      </c>
+      <c r="R405" t="s">
+        <v>2029</v>
+      </c>
+      <c r="S405" t="s">
+        <v>2030</v>
+      </c>
+      <c r="T405" t="s">
+        <v>2031</v>
+      </c>
+      <c r="U405" t="s">
+        <v>2028</v>
+      </c>
+    </row>
+    <row r="406" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A406" s="4" t="s">
+        <v>2032</v>
+      </c>
+      <c r="B406" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C406" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D406" s="2" t="s">
+        <v>2033</v>
+      </c>
+      <c r="E406" s="3">
+        <v>2024</v>
+      </c>
+      <c r="F406" s="5" t="s">
+        <v>2034</v>
+      </c>
+      <c r="G406" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="I406" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N406" s="9">
+        <v>104</v>
+      </c>
+      <c r="O406" s="4" t="s">
+        <v>2035</v>
+      </c>
+      <c r="Q406" t="s">
+        <v>2036</v>
+      </c>
+      <c r="R406" t="s">
+        <v>2038</v>
+      </c>
+      <c r="S406" t="s">
+        <v>2039</v>
+      </c>
+      <c r="T406" t="s">
+        <v>2040</v>
+      </c>
+      <c r="U406" t="s">
+        <v>2037</v>
+      </c>
+    </row>
+    <row r="407" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A407" s="4" t="s">
+        <v>2041</v>
+      </c>
+      <c r="B407" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C407" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D407" s="2" t="s">
+        <v>2042</v>
+      </c>
+      <c r="E407" s="3">
+        <v>1971</v>
+      </c>
+      <c r="F407" s="5" t="s">
+        <v>2043</v>
+      </c>
+      <c r="G407" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I407" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N407" s="9">
+        <v>100</v>
+      </c>
+      <c r="O407" s="4" t="s">
+        <v>2044</v>
+      </c>
+      <c r="Q407" t="s">
+        <v>2045</v>
+      </c>
+      <c r="R407" t="s">
+        <v>2049</v>
+      </c>
+      <c r="S407" t="s">
+        <v>2047</v>
+      </c>
+      <c r="T407" t="s">
+        <v>2048</v>
+      </c>
+      <c r="U407" t="s">
+        <v>2046</v>
+      </c>
+    </row>
+    <row r="408" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A408" s="4" t="s">
+        <v>2050</v>
+      </c>
+      <c r="B408" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C408" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D408" s="2" t="s">
+        <v>2051</v>
+      </c>
+      <c r="E408" s="3">
+        <v>1995</v>
+      </c>
+      <c r="F408" s="5" t="s">
+        <v>1820</v>
+      </c>
+      <c r="G408" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="I408" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="K408" s="6" t="s">
+        <v>2052</v>
+      </c>
+      <c r="L408" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M408" s="6" t="s">
+        <v>2053</v>
+      </c>
+      <c r="N408" s="9">
+        <v>101</v>
+      </c>
+      <c r="O408" s="4" t="s">
+        <v>1118</v>
+      </c>
+      <c r="Q408" t="s">
+        <v>2054</v>
+      </c>
+      <c r="R408" t="s">
+        <v>2056</v>
+      </c>
+      <c r="S408" t="s">
+        <v>2057</v>
+      </c>
+      <c r="T408" t="s">
+        <v>2058</v>
+      </c>
+      <c r="U408" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="409" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A409" s="4" t="s">
+        <v>2059</v>
+      </c>
+      <c r="B409" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C409" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D409" s="2" t="s">
+        <v>2052</v>
+      </c>
+      <c r="E409" s="3">
+        <v>2004</v>
+      </c>
+      <c r="F409" s="5" t="s">
+        <v>1820</v>
+      </c>
+      <c r="G409" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I409" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J409" s="6" t="s">
+        <v>2051</v>
+      </c>
+      <c r="L409" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="M409" s="6" t="s">
+        <v>2053</v>
+      </c>
+      <c r="N409" s="9">
+        <v>80</v>
+      </c>
+      <c r="O409" s="4" t="s">
+        <v>448</v>
+      </c>
+      <c r="Q409" t="s">
+        <v>2060</v>
+      </c>
+      <c r="R409" t="s">
+        <v>2062</v>
+      </c>
+      <c r="S409" t="s">
+        <v>2057</v>
+      </c>
+      <c r="T409" t="s">
+        <v>2061</v>
+      </c>
+      <c r="U409" t="s">
+        <v>2055</v>
+      </c>
+    </row>
+    <row r="410" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A410" s="4" t="s">
+        <v>2063</v>
+      </c>
+      <c r="B410" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C410" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D410" s="2" t="s">
+        <v>2064</v>
+      </c>
+      <c r="E410" s="3">
+        <v>2021</v>
+      </c>
+      <c r="F410" s="5" t="s">
+        <v>1001</v>
+      </c>
+      <c r="G410" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="I410" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="N410" s="9">
+        <v>128</v>
+      </c>
+      <c r="O410" s="4" t="s">
+        <v>2065</v>
+      </c>
+      <c r="Q410" t="s">
+        <v>2066</v>
+      </c>
+      <c r="R410" t="s">
+        <v>32</v>
+      </c>
+      <c r="S410" t="s">
+        <v>2068</v>
+      </c>
+      <c r="T410" t="s">
+        <v>2069</v>
+      </c>
+      <c r="U410" t="s">
+        <v>2067</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:U384" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:U394">

</xml_diff>

<commit_message>
london trip additional info update
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45AF06B7-6010-4840-9677-CF70A95EA1AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1CC71F-9A51-4F8B-B533-3E2FA79D7D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11520" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="database" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7253" uniqueCount="2070">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7256" uniqueCount="2073">
   <si>
     <t>ID</t>
   </si>
@@ -6249,6 +6249,15 @@
   </si>
   <si>
     <t>Andrea Flesch</t>
+  </si>
+  <si>
+    <t>signed by Cate Blanchett</t>
+  </si>
+  <si>
+    <t>signed by Tom Hiddleston</t>
+  </si>
+  <si>
+    <t>signed by Adrian Brody</t>
   </si>
 </sst>
 </file>
@@ -6645,8 +6654,8 @@
   <dimension ref="A1:U410"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A392" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D406" sqref="D406"/>
+      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H305" sqref="H305"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18884,7 +18893,9 @@
       <c r="G195" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H195" s="3"/>
+      <c r="H195" s="3" t="s">
+        <v>2070</v>
+      </c>
       <c r="I195" s="3" t="s">
         <v>25</v>
       </c>
@@ -25740,7 +25751,9 @@
       <c r="G305" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H305" s="3"/>
+      <c r="H305" s="3" t="s">
+        <v>2072</v>
+      </c>
       <c r="I305" s="3" t="s">
         <v>27</v>
       </c>
@@ -27710,7 +27723,9 @@
       <c r="G337" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H337" s="3"/>
+      <c r="H337" s="3" t="s">
+        <v>2071</v>
+      </c>
       <c r="I337" s="3" t="s">
         <v>27</v>
       </c>
@@ -31696,7 +31711,7 @@
         <v>2008</v>
       </c>
       <c r="E403" s="3">
-        <v>1961</v>
+        <v>2023</v>
       </c>
       <c r="F403" s="5" t="s">
         <v>2009</v>

</xml_diff>

<commit_message>
added the end we start from additional info
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B1CC71F-9A51-4F8B-B533-3E2FA79D7D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{964FF6AA-5545-4B99-AAB1-EB85341FA93B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7256" uniqueCount="2073">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7257" uniqueCount="2074">
   <si>
     <t>ID</t>
   </si>
@@ -6258,6 +6258,9 @@
   </si>
   <si>
     <t>signed by Adrian Brody</t>
+  </si>
+  <si>
+    <t>signed by Gina McKee</t>
   </si>
 </sst>
 </file>
@@ -6654,8 +6657,8 @@
   <dimension ref="A1:U410"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="109" zoomScaleNormal="130" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A293" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H305" sqref="H305"/>
+      <pane ySplit="1" topLeftCell="A283" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H295" sqref="H295"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25121,7 +25124,9 @@
       <c r="G295" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="H295" s="3"/>
+      <c r="H295" s="3" t="s">
+        <v>2073</v>
+      </c>
       <c r="I295" s="3" t="s">
         <v>27</v>
       </c>

</xml_diff>

<commit_message>
maybe fixed xmen problem
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7056826-8E67-45A6-98B1-AAA9883ECA0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE4ED28-F3A6-40C9-AAFA-481FB2BE1001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7513" uniqueCount="2200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7505" uniqueCount="2199">
   <si>
     <t>ID</t>
   </si>
@@ -5615,36 +5615,24 @@
     <t>Bryan Singer</t>
   </si>
   <si>
-    <t xml:space="preserve">X-Men United, X-Men: The Last Stand </t>
-  </si>
-  <si>
     <t>XMen_United_2003</t>
   </si>
   <si>
     <t>X-Men United</t>
   </si>
   <si>
-    <t xml:space="preserve">X-Men: The Last Stand </t>
-  </si>
-  <si>
     <t>XMen_Apocalypse_2016</t>
   </si>
   <si>
     <t>X-Men: Apocalypse</t>
   </si>
   <si>
-    <t xml:space="preserve">X-Men: Dark Pheonix, X-Men, X-Men United, X-Men: The Last Stand </t>
-  </si>
-  <si>
     <t>XMen_Dark_Pheonix_2019</t>
   </si>
   <si>
     <t>X-Men: Dark Pheonix</t>
   </si>
   <si>
-    <t>X-Men: First Class, X-Men: Days of the Future Past, X-Men: Apocalypse</t>
-  </si>
-  <si>
     <t xml:space="preserve">X-Men, X-Men United, X-Men: The Last Stand </t>
   </si>
   <si>
@@ -5657,9 +5645,6 @@
     <t>X-Men: First Class</t>
   </si>
   <si>
-    <t xml:space="preserve">X-Men: Apocalypse, X-Men: Dark Pheonix, X-Men, X-Men United, X-Men: The Last Stand </t>
-  </si>
-  <si>
     <t>XMen_First_Class_2011</t>
   </si>
   <si>
@@ -6639,6 +6624,18 @@
   </si>
   <si>
     <t>Marit Allen</t>
+  </si>
+  <si>
+    <t>X-Men: First Class, X-Men: Days of Future Past, X-Men: Apocalypse</t>
+  </si>
+  <si>
+    <t>X-Men: Dark Pheonix, X-Men, X-Men United, X-Men: The Last Stand</t>
+  </si>
+  <si>
+    <t>X-Men: Apocalypse, X-Men: Dark Pheonix, X-Men, X-Men United, X-Men: The Last Stand</t>
+  </si>
+  <si>
+    <t>X-Men United, X-Men: The Last Stand</t>
   </si>
 </sst>
 </file>
@@ -7025,8 +7022,8 @@
   <dimension ref="A1:U428"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A352" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A365" sqref="A365"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J37" sqref="J37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7368,7 +7365,7 @@
         <v>263</v>
       </c>
       <c r="U5" s="3" t="s">
-        <v>1940</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
@@ -7688,7 +7685,7 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" s="3" t="s">
-        <v>1944</v>
+        <v>1939</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -7697,13 +7694,13 @@
         <v>37</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>1941</v>
+        <v>1936</v>
       </c>
       <c r="E11" s="2">
         <v>2024</v>
       </c>
       <c r="F11" s="4" t="s">
-        <v>1945</v>
+        <v>1940</v>
       </c>
       <c r="G11" s="7" t="s">
         <v>25</v>
@@ -7718,19 +7715,19 @@
         <v>1642</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>1947</v>
+        <v>1942</v>
       </c>
       <c r="R11" s="1" t="s">
-        <v>1949</v>
+        <v>1944</v>
       </c>
       <c r="S11" s="1" t="s">
-        <v>1950</v>
+        <v>1945</v>
       </c>
       <c r="T11" s="1" t="s">
-        <v>1951</v>
+        <v>1946</v>
       </c>
       <c r="U11" s="1" t="s">
-        <v>1948</v>
+        <v>1943</v>
       </c>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.3">
@@ -8365,7 +8362,7 @@
     </row>
     <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" s="3" t="s">
-        <v>1962</v>
+        <v>1957</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>22</v>
@@ -8374,13 +8371,13 @@
         <v>23</v>
       </c>
       <c r="D22" s="1" t="s">
-        <v>1963</v>
+        <v>1958</v>
       </c>
       <c r="E22" s="2">
         <v>1987</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>1964</v>
+        <v>1959</v>
       </c>
       <c r="G22" s="7" t="s">
         <v>27</v>
@@ -8395,19 +8392,19 @@
         <v>1632</v>
       </c>
       <c r="Q22" s="1" t="s">
-        <v>1966</v>
+        <v>1961</v>
       </c>
       <c r="R22" s="1" t="s">
-        <v>1967</v>
+        <v>1962</v>
       </c>
       <c r="S22" s="1" t="s">
-        <v>1968</v>
+        <v>1963</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>1969</v>
+        <v>1964</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>1965</v>
+        <v>1960</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.3">
@@ -9011,7 +9008,7 @@
     </row>
     <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" s="3" t="s">
-        <v>1874</v>
+        <v>1869</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>22</v>
@@ -9020,13 +9017,13 @@
         <v>37</v>
       </c>
       <c r="D33" s="3" t="s">
-        <v>1875</v>
+        <v>1870</v>
       </c>
       <c r="E33" s="2">
         <v>2006</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>1876</v>
+        <v>1871</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>25</v>
@@ -9036,7 +9033,7 @@
         <v>25</v>
       </c>
       <c r="J33" s="3" t="s">
-        <v>2147</v>
+        <v>2142</v>
       </c>
       <c r="K33" s="3" t="s">
         <v>28</v>
@@ -9099,10 +9096,10 @@
         <v>25</v>
       </c>
       <c r="J34" s="3" t="s">
-        <v>2146</v>
+        <v>2141</v>
       </c>
       <c r="K34" s="3" t="s">
-        <v>1858</v>
+        <v>2198</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>25</v>
@@ -9137,7 +9134,7 @@
     </row>
     <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>1859</v>
+        <v>1858</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>22</v>
@@ -9146,7 +9143,7 @@
         <v>37</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>1860</v>
+        <v>1859</v>
       </c>
       <c r="E35" s="2">
         <v>2003</v>
@@ -9162,10 +9159,10 @@
         <v>25</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>2148</v>
+        <v>2143</v>
       </c>
       <c r="K35" s="3" t="s">
-        <v>1861</v>
+        <v>1870</v>
       </c>
       <c r="L35" s="2" t="s">
         <v>25</v>
@@ -9200,7 +9197,7 @@
     </row>
     <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" s="3" t="s">
-        <v>1869</v>
+        <v>1865</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>22</v>
@@ -9209,7 +9206,7 @@
         <v>37</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>1870</v>
+        <v>1866</v>
       </c>
       <c r="E36" s="2">
         <v>2014</v>
@@ -9225,10 +9222,10 @@
         <v>25</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>1871</v>
+        <v>1867</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>1872</v>
+        <v>2197</v>
       </c>
       <c r="L36" s="2" t="s">
         <v>25</v>
@@ -9263,7 +9260,7 @@
     </row>
     <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" s="3" t="s">
-        <v>1862</v>
+        <v>1860</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>22</v>
@@ -9272,7 +9269,7 @@
         <v>37</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>1863</v>
+        <v>1861</v>
       </c>
       <c r="E37" s="2">
         <v>2016</v>
@@ -9288,10 +9285,10 @@
         <v>25</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>2149</v>
+        <v>2144</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>1864</v>
+        <v>2196</v>
       </c>
       <c r="L37" s="2" t="s">
         <v>25</v>
@@ -9389,7 +9386,7 @@
     </row>
     <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" s="3" t="s">
-        <v>1891</v>
+        <v>1886</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>22</v>
@@ -9398,13 +9395,13 @@
         <v>37</v>
       </c>
       <c r="D39" s="3" t="s">
-        <v>1892</v>
+        <v>1887</v>
       </c>
       <c r="E39" s="2">
         <v>2016</v>
       </c>
       <c r="F39" s="3" t="s">
-        <v>1893</v>
+        <v>1888</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>25</v>
@@ -9429,10 +9426,10 @@
         <v>104</v>
       </c>
       <c r="O39" s="3" t="s">
-        <v>1894</v>
+        <v>1889</v>
       </c>
       <c r="P39" s="3" t="s">
-        <v>1895</v>
+        <v>1890</v>
       </c>
       <c r="Q39" s="3" t="s">
         <v>28</v>
@@ -10507,7 +10504,7 @@
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="3" t="s">
-        <v>2069</v>
+        <v>2064</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>22</v>
@@ -10516,7 +10513,7 @@
         <v>23</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>2068</v>
+        <v>2063</v>
       </c>
       <c r="E57" s="2">
         <v>2014</v>
@@ -10534,22 +10531,22 @@
         <v>169</v>
       </c>
       <c r="O57" s="3" t="s">
-        <v>2070</v>
+        <v>2065</v>
       </c>
       <c r="Q57" s="1" t="s">
-        <v>2071</v>
+        <v>2066</v>
       </c>
       <c r="R57" s="1" t="s">
         <v>115</v>
       </c>
       <c r="S57" s="1" t="s">
-        <v>2073</v>
+        <v>2068</v>
       </c>
       <c r="T57" s="1" t="s">
         <v>224</v>
       </c>
       <c r="U57" s="1" t="s">
-        <v>2072</v>
+        <v>2067</v>
       </c>
     </row>
     <row r="58" spans="1:21" x14ac:dyDescent="0.3">
@@ -11060,7 +11057,7 @@
     </row>
     <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="3" t="s">
-        <v>1877</v>
+        <v>1872</v>
       </c>
       <c r="B66" s="3" t="s">
         <v>22</v>
@@ -11069,13 +11066,13 @@
         <v>23</v>
       </c>
       <c r="D66" s="3" t="s">
-        <v>1878</v>
+        <v>1873</v>
       </c>
       <c r="E66" s="2">
         <v>2015</v>
       </c>
       <c r="F66" s="3" t="s">
-        <v>1879</v>
+        <v>1874</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>25</v>
@@ -11100,7 +11097,7 @@
         <v>98</v>
       </c>
       <c r="O66" s="3" t="s">
-        <v>1880</v>
+        <v>1875</v>
       </c>
       <c r="P66" s="3" t="s">
         <v>28</v>
@@ -11240,7 +11237,7 @@
         <v>543</v>
       </c>
       <c r="S68" s="3" t="s">
-        <v>1938</v>
+        <v>1933</v>
       </c>
       <c r="T68" s="3" t="s">
         <v>224</v>
@@ -11303,7 +11300,7 @@
         <v>543</v>
       </c>
       <c r="S69" s="3" t="s">
-        <v>1938</v>
+        <v>1933</v>
       </c>
       <c r="T69" s="3" t="s">
         <v>224</v>
@@ -11314,7 +11311,7 @@
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="1" t="s">
-        <v>2125</v>
+        <v>2120</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>22</v>
@@ -11323,7 +11320,7 @@
         <v>23</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>2126</v>
+        <v>2121</v>
       </c>
       <c r="E70" s="2">
         <v>2022</v>
@@ -11341,7 +11338,7 @@
         <v>189</v>
       </c>
       <c r="O70" s="1" t="s">
-        <v>2127</v>
+        <v>2122</v>
       </c>
       <c r="Q70" s="1" t="s">
         <v>539</v>
@@ -11350,13 +11347,13 @@
         <v>543</v>
       </c>
       <c r="S70" s="1" t="s">
-        <v>1938</v>
+        <v>1933</v>
       </c>
       <c r="T70" s="1" t="s">
         <v>224</v>
       </c>
       <c r="U70" s="1" t="s">
-        <v>2128</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
@@ -11884,7 +11881,7 @@
         <v>25</v>
       </c>
       <c r="H79" s="2" t="s">
-        <v>2065</v>
+        <v>2060</v>
       </c>
       <c r="I79" s="2" t="s">
         <v>27</v>
@@ -13188,7 +13185,7 @@
     </row>
     <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" s="3" t="s">
-        <v>1980</v>
+        <v>1975</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>22</v>
@@ -13197,13 +13194,13 @@
         <v>37</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>1979</v>
+        <v>1974</v>
       </c>
       <c r="E100" s="2">
         <v>2021</v>
       </c>
       <c r="F100" s="4" t="s">
-        <v>1981</v>
+        <v>1976</v>
       </c>
       <c r="G100" s="7" t="s">
         <v>25</v>
@@ -13215,22 +13212,22 @@
         <v>90</v>
       </c>
       <c r="O100" s="3" t="s">
+        <v>1977</v>
+      </c>
+      <c r="Q100" s="1" t="s">
+        <v>1978</v>
+      </c>
+      <c r="R100" s="1" t="s">
+        <v>1979</v>
+      </c>
+      <c r="S100" s="1" t="s">
+        <v>1980</v>
+      </c>
+      <c r="T100" s="1" t="s">
+        <v>1981</v>
+      </c>
+      <c r="U100" s="1" t="s">
         <v>1982</v>
-      </c>
-      <c r="Q100" s="1" t="s">
-        <v>1983</v>
-      </c>
-      <c r="R100" s="1" t="s">
-        <v>1984</v>
-      </c>
-      <c r="S100" s="1" t="s">
-        <v>1985</v>
-      </c>
-      <c r="T100" s="1" t="s">
-        <v>1986</v>
-      </c>
-      <c r="U100" s="1" t="s">
-        <v>1987</v>
       </c>
     </row>
     <row r="101" spans="1:21" x14ac:dyDescent="0.3">
@@ -14235,7 +14232,7 @@
     </row>
     <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117" s="3" t="s">
-        <v>1996</v>
+        <v>1991</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>22</v>
@@ -14244,7 +14241,7 @@
         <v>37</v>
       </c>
       <c r="D117" s="1" t="s">
-        <v>1997</v>
+        <v>1992</v>
       </c>
       <c r="E117" s="2">
         <v>2023</v>
@@ -14265,7 +14262,7 @@
         <v>1471</v>
       </c>
       <c r="Q117" s="1" t="s">
-        <v>1998</v>
+        <v>1993</v>
       </c>
       <c r="R117" s="1" t="s">
         <v>1174</v>
@@ -14274,10 +14271,10 @@
         <v>634</v>
       </c>
       <c r="T117" s="1" t="s">
-        <v>2000</v>
+        <v>1995</v>
       </c>
       <c r="U117" s="1" t="s">
-        <v>1999</v>
+        <v>1994</v>
       </c>
     </row>
     <row r="118" spans="1:21" x14ac:dyDescent="0.3">
@@ -14405,7 +14402,7 @@
     </row>
     <row r="120" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="3" t="s">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>22</v>
@@ -14414,13 +14411,13 @@
         <v>37</v>
       </c>
       <c r="D120" s="1" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
       <c r="E120" s="2">
         <v>2005</v>
       </c>
       <c r="F120" s="4" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
       <c r="G120" s="7" t="s">
         <v>25</v>
@@ -14432,7 +14429,7 @@
         <v>27</v>
       </c>
       <c r="M120" s="4" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
       <c r="N120" s="7">
         <v>86</v>
@@ -14441,16 +14438,16 @@
         <v>1446</v>
       </c>
       <c r="Q120" s="1" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
       <c r="R120" s="1" t="s">
         <v>115</v>
       </c>
       <c r="T120" s="1" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
       <c r="U120" s="1" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
     </row>
     <row r="121" spans="1:21" x14ac:dyDescent="0.3">
@@ -14644,7 +14641,7 @@
     </row>
     <row r="124" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A124" s="3" t="s">
-        <v>2026</v>
+        <v>2021</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>22</v>
@@ -14653,13 +14650,13 @@
         <v>37</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>2027</v>
+        <v>2022</v>
       </c>
       <c r="E124" s="2">
         <v>2024</v>
       </c>
       <c r="F124" s="4" t="s">
-        <v>2028</v>
+        <v>2023</v>
       </c>
       <c r="G124" s="7" t="s">
         <v>25</v>
@@ -14671,22 +14668,22 @@
         <v>104</v>
       </c>
       <c r="O124" s="3" t="s">
+        <v>2024</v>
+      </c>
+      <c r="Q124" s="1" t="s">
+        <v>2025</v>
+      </c>
+      <c r="R124" s="1" t="s">
+        <v>2027</v>
+      </c>
+      <c r="S124" s="1" t="s">
+        <v>2028</v>
+      </c>
+      <c r="T124" s="1" t="s">
         <v>2029</v>
       </c>
-      <c r="Q124" s="1" t="s">
-        <v>2030</v>
-      </c>
-      <c r="R124" s="1" t="s">
-        <v>2032</v>
-      </c>
-      <c r="S124" s="1" t="s">
-        <v>2033</v>
-      </c>
-      <c r="T124" s="1" t="s">
-        <v>2034</v>
-      </c>
       <c r="U124" s="1" t="s">
-        <v>2031</v>
+        <v>2026</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
@@ -15329,7 +15326,7 @@
         <v>25</v>
       </c>
       <c r="H135" s="2" t="s">
-        <v>2064</v>
+        <v>2059</v>
       </c>
       <c r="I135" s="2" t="s">
         <v>25</v>
@@ -15625,7 +15622,7 @@
     </row>
     <row r="140" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A140" s="3" t="s">
-        <v>1988</v>
+        <v>1983</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>22</v>
@@ -15634,13 +15631,13 @@
         <v>37</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>1989</v>
+        <v>1984</v>
       </c>
       <c r="E140" s="2">
         <v>2022</v>
       </c>
       <c r="F140" s="4" t="s">
-        <v>1990</v>
+        <v>1985</v>
       </c>
       <c r="G140" s="7" t="s">
         <v>25</v>
@@ -15652,22 +15649,22 @@
         <v>105</v>
       </c>
       <c r="O140" s="3" t="s">
-        <v>1991</v>
+        <v>1986</v>
       </c>
       <c r="Q140" s="1" t="s">
-        <v>1992</v>
+        <v>1987</v>
       </c>
       <c r="R140" s="1" t="s">
         <v>146</v>
       </c>
       <c r="S140" s="1" t="s">
-        <v>1994</v>
+        <v>1989</v>
       </c>
       <c r="T140" s="1" t="s">
-        <v>1995</v>
+        <v>1990</v>
       </c>
       <c r="U140" s="1" t="s">
-        <v>1993</v>
+        <v>1988</v>
       </c>
     </row>
     <row r="141" spans="1:21" x14ac:dyDescent="0.3">
@@ -16906,7 +16903,7 @@
     </row>
     <row r="161" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A161" s="3" t="s">
-        <v>1904</v>
+        <v>1899</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>22</v>
@@ -16915,13 +16912,13 @@
         <v>37</v>
       </c>
       <c r="D161" s="1" t="s">
-        <v>1905</v>
+        <v>1900</v>
       </c>
       <c r="E161" s="2">
         <v>1985</v>
       </c>
       <c r="F161" s="4" t="s">
-        <v>1906</v>
+        <v>1901</v>
       </c>
       <c r="G161" s="7" t="s">
         <v>27</v>
@@ -16936,19 +16933,19 @@
         <v>447</v>
       </c>
       <c r="Q161" s="1" t="s">
-        <v>1907</v>
+        <v>1902</v>
       </c>
       <c r="R161" s="1" t="s">
-        <v>1909</v>
+        <v>1904</v>
       </c>
       <c r="S161" s="1" t="s">
-        <v>1910</v>
+        <v>1905</v>
       </c>
       <c r="T161" s="1" t="s">
-        <v>1911</v>
+        <v>1906</v>
       </c>
       <c r="U161" s="1" t="s">
-        <v>1908</v>
+        <v>1903</v>
       </c>
     </row>
     <row r="162" spans="1:21" x14ac:dyDescent="0.3">
@@ -17583,7 +17580,7 @@
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A172" s="3" t="s">
-        <v>2001</v>
+        <v>1996</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>22</v>
@@ -17592,13 +17589,13 @@
         <v>23</v>
       </c>
       <c r="D172" s="1" t="s">
-        <v>2002</v>
+        <v>1997</v>
       </c>
       <c r="E172" s="2">
         <v>2023</v>
       </c>
       <c r="F172" s="4" t="s">
-        <v>2003</v>
+        <v>1998</v>
       </c>
       <c r="G172" s="7" t="s">
         <v>27</v>
@@ -17610,22 +17607,22 @@
         <v>153</v>
       </c>
       <c r="O172" s="3" t="s">
+        <v>1999</v>
+      </c>
+      <c r="Q172" s="1" t="s">
+        <v>2000</v>
+      </c>
+      <c r="R172" s="1" t="s">
+        <v>2002</v>
+      </c>
+      <c r="S172" s="1" t="s">
+        <v>2003</v>
+      </c>
+      <c r="T172" s="1" t="s">
         <v>2004</v>
       </c>
-      <c r="Q172" s="1" t="s">
-        <v>2005</v>
-      </c>
-      <c r="R172" s="1" t="s">
-        <v>2007</v>
-      </c>
-      <c r="S172" s="1" t="s">
-        <v>2008</v>
-      </c>
-      <c r="T172" s="1" t="s">
-        <v>2009</v>
-      </c>
       <c r="U172" s="1" t="s">
-        <v>2006</v>
+        <v>2001</v>
       </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
@@ -18227,13 +18224,13 @@
         <v>28</v>
       </c>
       <c r="K182" s="3" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
       <c r="L182" s="2" t="s">
         <v>27</v>
       </c>
       <c r="M182" s="3" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
       <c r="N182" s="2">
         <v>87</v>
@@ -18262,7 +18259,7 @@
     </row>
     <row r="183" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A183" s="3" t="s">
-        <v>2102</v>
+        <v>2097</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>22</v>
@@ -18271,7 +18268,7 @@
         <v>23</v>
       </c>
       <c r="D183" s="1" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
       <c r="E183" s="2">
         <v>2020</v>
@@ -18292,7 +18289,7 @@
         <v>27</v>
       </c>
       <c r="M183" s="4" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
       <c r="N183" s="7">
         <v>97</v>
@@ -18307,13 +18304,13 @@
         <v>61</v>
       </c>
       <c r="S183" s="1" t="s">
-        <v>2104</v>
+        <v>2099</v>
       </c>
       <c r="T183" s="1" t="s">
         <v>63</v>
       </c>
       <c r="U183" s="1" t="s">
-        <v>2105</v>
+        <v>2100</v>
       </c>
     </row>
     <row r="184" spans="1:21" x14ac:dyDescent="0.3">
@@ -18570,7 +18567,7 @@
     </row>
     <row r="188" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A188" s="3" t="s">
-        <v>2057</v>
+        <v>2052</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>22</v>
@@ -18579,7 +18576,7 @@
         <v>37</v>
       </c>
       <c r="D188" s="1" t="s">
-        <v>2058</v>
+        <v>2053</v>
       </c>
       <c r="E188" s="2">
         <v>2021</v>
@@ -18597,22 +18594,22 @@
         <v>128</v>
       </c>
       <c r="O188" s="3" t="s">
-        <v>2059</v>
+        <v>2054</v>
       </c>
       <c r="Q188" s="1" t="s">
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="R188" s="1" t="s">
         <v>32</v>
       </c>
       <c r="S188" s="1" t="s">
-        <v>2062</v>
+        <v>2057</v>
       </c>
       <c r="T188" s="1" t="s">
-        <v>2063</v>
+        <v>2058</v>
       </c>
       <c r="U188" s="1" t="s">
-        <v>2061</v>
+        <v>2056</v>
       </c>
     </row>
     <row r="189" spans="1:21" x14ac:dyDescent="0.3">
@@ -19110,7 +19107,7 @@
         <v>223</v>
       </c>
       <c r="S196" s="3" t="s">
-        <v>1938</v>
+        <v>1933</v>
       </c>
       <c r="T196" s="3" t="s">
         <v>224</v>
@@ -19121,7 +19118,7 @@
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A197" s="3" t="s">
-        <v>1970</v>
+        <v>1965</v>
       </c>
       <c r="B197" s="1" t="s">
         <v>22</v>
@@ -19130,13 +19127,13 @@
         <v>23</v>
       </c>
       <c r="D197" s="1" t="s">
-        <v>1971</v>
+        <v>1966</v>
       </c>
       <c r="E197" s="2">
         <v>2023</v>
       </c>
       <c r="F197" s="4" t="s">
-        <v>1972</v>
+        <v>1967</v>
       </c>
       <c r="G197" s="7" t="s">
         <v>25</v>
@@ -19148,22 +19145,22 @@
         <v>105</v>
       </c>
       <c r="O197" s="3" t="s">
+        <v>1968</v>
+      </c>
+      <c r="Q197" s="1" t="s">
+        <v>1969</v>
+      </c>
+      <c r="R197" s="1" t="s">
+        <v>1970</v>
+      </c>
+      <c r="S197" s="1" t="s">
+        <v>1971</v>
+      </c>
+      <c r="T197" s="1" t="s">
+        <v>1972</v>
+      </c>
+      <c r="U197" s="1" t="s">
         <v>1973</v>
-      </c>
-      <c r="Q197" s="1" t="s">
-        <v>1974</v>
-      </c>
-      <c r="R197" s="1" t="s">
-        <v>1975</v>
-      </c>
-      <c r="S197" s="1" t="s">
-        <v>1976</v>
-      </c>
-      <c r="T197" s="1" t="s">
-        <v>1977</v>
-      </c>
-      <c r="U197" s="1" t="s">
-        <v>1978</v>
       </c>
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.3">
@@ -19672,7 +19669,7 @@
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A206" s="1" t="s">
-        <v>2129</v>
+        <v>2124</v>
       </c>
       <c r="B206" s="1" t="s">
         <v>22</v>
@@ -19681,13 +19678,13 @@
         <v>23</v>
       </c>
       <c r="D206" s="1" t="s">
-        <v>2130</v>
+        <v>2125</v>
       </c>
       <c r="E206" s="2">
         <v>2023</v>
       </c>
       <c r="F206" s="4" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
       <c r="G206" s="7" t="s">
         <v>25</v>
@@ -19702,24 +19699,24 @@
         <v>318</v>
       </c>
       <c r="Q206" s="1" t="s">
-        <v>2132</v>
+        <v>2127</v>
       </c>
       <c r="R206" s="1" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
       <c r="S206" s="1" t="s">
-        <v>2135</v>
+        <v>2130</v>
       </c>
       <c r="T206" s="1" t="s">
-        <v>2134</v>
+        <v>2129</v>
       </c>
       <c r="U206" s="1" t="s">
-        <v>2133</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A207" s="3" t="s">
-        <v>1881</v>
+        <v>1876</v>
       </c>
       <c r="B207" s="3" t="s">
         <v>22</v>
@@ -19728,13 +19725,13 @@
         <v>23</v>
       </c>
       <c r="D207" s="3" t="s">
-        <v>1882</v>
+        <v>1877</v>
       </c>
       <c r="E207" s="2">
         <v>2012</v>
       </c>
       <c r="F207" s="3" t="s">
-        <v>1883</v>
+        <v>1878</v>
       </c>
       <c r="G207" s="2" t="s">
         <v>25</v>
@@ -19759,10 +19756,10 @@
         <v>157</v>
       </c>
       <c r="O207" s="3" t="s">
-        <v>1884</v>
+        <v>1879</v>
       </c>
       <c r="P207" s="3" t="s">
-        <v>1885</v>
+        <v>1880</v>
       </c>
       <c r="Q207" s="3" t="s">
         <v>28</v>
@@ -19782,7 +19779,7 @@
     </row>
     <row r="208" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A208" s="3" t="s">
-        <v>2010</v>
+        <v>2005</v>
       </c>
       <c r="B208" s="1" t="s">
         <v>22</v>
@@ -19791,13 +19788,13 @@
         <v>37</v>
       </c>
       <c r="D208" s="1" t="s">
-        <v>2011</v>
+        <v>2006</v>
       </c>
       <c r="E208" s="2">
         <v>2016</v>
       </c>
       <c r="F208" s="4" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="G208" s="7" t="s">
         <v>25</v>
@@ -19812,19 +19809,19 @@
         <v>935</v>
       </c>
       <c r="Q208" s="1" t="s">
-        <v>2012</v>
+        <v>2007</v>
       </c>
       <c r="R208" s="1" t="s">
-        <v>2014</v>
+        <v>2009</v>
       </c>
       <c r="S208" s="1" t="s">
-        <v>2015</v>
+        <v>2010</v>
       </c>
       <c r="T208" s="1" t="s">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="U208" s="1" t="s">
-        <v>2013</v>
+        <v>2008</v>
       </c>
     </row>
     <row r="209" spans="1:21" x14ac:dyDescent="0.3">
@@ -20196,10 +20193,10 @@
         <v>1579</v>
       </c>
       <c r="S214" s="3" t="s">
-        <v>1938</v>
+        <v>1933</v>
       </c>
       <c r="T214" s="3" t="s">
-        <v>1939</v>
+        <v>1934</v>
       </c>
       <c r="U214" s="3" t="s">
         <v>28</v>
@@ -20333,7 +20330,7 @@
     </row>
     <row r="217" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A217" s="3" t="s">
-        <v>1896</v>
+        <v>1891</v>
       </c>
       <c r="B217" s="1" t="s">
         <v>22</v>
@@ -20342,13 +20339,13 @@
         <v>37</v>
       </c>
       <c r="D217" s="1" t="s">
-        <v>1897</v>
+        <v>1892</v>
       </c>
       <c r="E217" s="2">
         <v>2010</v>
       </c>
       <c r="F217" s="4" t="s">
-        <v>1898</v>
+        <v>1893</v>
       </c>
       <c r="G217" s="7" t="s">
         <v>27</v>
@@ -20360,22 +20357,22 @@
         <v>106</v>
       </c>
       <c r="O217" s="3" t="s">
-        <v>1899</v>
+        <v>1894</v>
       </c>
       <c r="Q217" s="1" t="s">
-        <v>1900</v>
+        <v>1895</v>
       </c>
       <c r="R217" s="1" t="s">
         <v>336</v>
       </c>
       <c r="S217" s="1" t="s">
-        <v>1902</v>
+        <v>1897</v>
       </c>
       <c r="T217" s="1" t="s">
-        <v>1903</v>
+        <v>1898</v>
       </c>
       <c r="U217" s="1" t="s">
-        <v>1901</v>
+        <v>1896</v>
       </c>
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.3">
@@ -20716,7 +20713,7 @@
         <v>25</v>
       </c>
       <c r="H223" s="2" t="s">
-        <v>2067</v>
+        <v>2062</v>
       </c>
       <c r="I223" s="2" t="s">
         <v>27</v>
@@ -21946,7 +21943,7 @@
     </row>
     <row r="243" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A243" s="3" t="s">
-        <v>1943</v>
+        <v>1938</v>
       </c>
       <c r="B243" s="1" t="s">
         <v>22</v>
@@ -21955,13 +21952,13 @@
         <v>37</v>
       </c>
       <c r="D243" s="1" t="s">
-        <v>1942</v>
+        <v>1937</v>
       </c>
       <c r="E243" s="2">
         <v>2024</v>
       </c>
       <c r="F243" s="4" t="s">
-        <v>1946</v>
+        <v>1941</v>
       </c>
       <c r="G243" s="7" t="s">
         <v>27</v>
@@ -21973,19 +21970,19 @@
         <v>97</v>
       </c>
       <c r="O243" s="3" t="s">
-        <v>1899</v>
+        <v>1894</v>
       </c>
       <c r="R243" s="4" t="s">
-        <v>1946</v>
+        <v>1941</v>
       </c>
       <c r="S243" s="1" t="s">
-        <v>1953</v>
+        <v>1948</v>
       </c>
       <c r="T243" s="1" t="s">
-        <v>1954</v>
+        <v>1949</v>
       </c>
       <c r="U243" s="1" t="s">
-        <v>1952</v>
+        <v>1947</v>
       </c>
     </row>
     <row r="244" spans="1:21" x14ac:dyDescent="0.3">
@@ -22053,7 +22050,7 @@
     </row>
     <row r="245" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A245" s="3" t="s">
-        <v>1873</v>
+        <v>1868</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>22</v>
@@ -22062,7 +22059,7 @@
         <v>37</v>
       </c>
       <c r="D245" s="3" t="s">
-        <v>1871</v>
+        <v>1867</v>
       </c>
       <c r="E245" s="2">
         <v>2011</v>
@@ -22081,7 +22078,7 @@
         <v>28</v>
       </c>
       <c r="K245" s="3" t="s">
-        <v>2145</v>
+        <v>2140</v>
       </c>
       <c r="L245" s="2" t="s">
         <v>25</v>
@@ -22368,7 +22365,7 @@
     </row>
     <row r="250" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A250" s="3" t="s">
-        <v>2035</v>
+        <v>2030</v>
       </c>
       <c r="B250" s="1" t="s">
         <v>22</v>
@@ -22377,13 +22374,13 @@
         <v>37</v>
       </c>
       <c r="D250" s="1" t="s">
-        <v>2036</v>
+        <v>2031</v>
       </c>
       <c r="E250" s="2">
         <v>1971</v>
       </c>
       <c r="F250" s="4" t="s">
-        <v>2037</v>
+        <v>2032</v>
       </c>
       <c r="G250" s="7" t="s">
         <v>27</v>
@@ -22395,22 +22392,22 @@
         <v>100</v>
       </c>
       <c r="O250" s="3" t="s">
+        <v>2033</v>
+      </c>
+      <c r="Q250" s="1" t="s">
+        <v>2034</v>
+      </c>
+      <c r="R250" s="1" t="s">
         <v>2038</v>
       </c>
-      <c r="Q250" s="1" t="s">
-        <v>2039</v>
-      </c>
-      <c r="R250" s="1" t="s">
-        <v>2043</v>
-      </c>
       <c r="S250" s="1" t="s">
-        <v>2041</v>
+        <v>2036</v>
       </c>
       <c r="T250" s="1" t="s">
-        <v>2042</v>
+        <v>2037</v>
       </c>
       <c r="U250" s="1" t="s">
-        <v>2040</v>
+        <v>2035</v>
       </c>
     </row>
     <row r="251" spans="1:21" x14ac:dyDescent="0.3">
@@ -23616,7 +23613,7 @@
     </row>
     <row r="270" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A270" s="1" t="s">
-        <v>2115</v>
+        <v>2110</v>
       </c>
       <c r="B270" s="1" t="s">
         <v>90</v>
@@ -23625,13 +23622,13 @@
         <v>23</v>
       </c>
       <c r="D270" s="1" t="s">
-        <v>2118</v>
+        <v>2113</v>
       </c>
       <c r="E270" s="2">
         <v>2023</v>
       </c>
       <c r="F270" s="4" t="s">
-        <v>2116</v>
+        <v>2111</v>
       </c>
       <c r="G270" s="7" t="s">
         <v>25</v>
@@ -23643,33 +23640,33 @@
         <v>27</v>
       </c>
       <c r="M270" s="4" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
       <c r="N270" s="7">
         <v>50</v>
       </c>
       <c r="O270" s="1" t="s">
+        <v>2114</v>
+      </c>
+      <c r="Q270" s="1" t="s">
+        <v>2115</v>
+      </c>
+      <c r="R270" s="1" t="s">
+        <v>2117</v>
+      </c>
+      <c r="S270" s="1" t="s">
+        <v>2118</v>
+      </c>
+      <c r="T270" s="1" t="s">
         <v>2119</v>
       </c>
-      <c r="Q270" s="1" t="s">
-        <v>2120</v>
-      </c>
-      <c r="R270" s="1" t="s">
-        <v>2122</v>
-      </c>
-      <c r="S270" s="1" t="s">
-        <v>2123</v>
-      </c>
-      <c r="T270" s="1" t="s">
-        <v>2124</v>
-      </c>
       <c r="U270" s="1" t="s">
-        <v>2121</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="271" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A271" s="3" t="s">
-        <v>2074</v>
+        <v>2069</v>
       </c>
       <c r="B271" s="1" t="s">
         <v>22</v>
@@ -23678,13 +23675,13 @@
         <v>37</v>
       </c>
       <c r="D271" s="1" t="s">
-        <v>2075</v>
+        <v>2070</v>
       </c>
       <c r="E271" s="2">
         <v>2008</v>
       </c>
       <c r="F271" s="4" t="s">
-        <v>2076</v>
+        <v>2071</v>
       </c>
       <c r="G271" s="7" t="s">
         <v>25</v>
@@ -23699,19 +23696,19 @@
         <v>935</v>
       </c>
       <c r="Q271" s="1" t="s">
-        <v>2077</v>
+        <v>2072</v>
       </c>
       <c r="R271" s="1" t="s">
-        <v>2079</v>
+        <v>2074</v>
       </c>
       <c r="S271" s="1" t="s">
         <v>1714</v>
       </c>
       <c r="T271" s="1" t="s">
-        <v>2080</v>
+        <v>2075</v>
       </c>
       <c r="U271" s="1" t="s">
-        <v>2078</v>
+        <v>2073</v>
       </c>
     </row>
     <row r="272" spans="1:21" x14ac:dyDescent="0.3">
@@ -24709,7 +24706,7 @@
     </row>
     <row r="288" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A288" s="1" t="s">
-        <v>2137</v>
+        <v>2132</v>
       </c>
       <c r="B288" s="1" t="s">
         <v>22</v>
@@ -24718,13 +24715,13 @@
         <v>37</v>
       </c>
       <c r="D288" s="1" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
       <c r="E288" s="2">
         <v>2020</v>
       </c>
       <c r="F288" s="4" t="s">
-        <v>2139</v>
+        <v>2134</v>
       </c>
       <c r="G288" s="7" t="s">
         <v>25</v>
@@ -24736,19 +24733,19 @@
         <v>100</v>
       </c>
       <c r="O288" s="1" t="s">
-        <v>2140</v>
+        <v>2135</v>
       </c>
       <c r="Q288" s="1" t="s">
-        <v>2141</v>
+        <v>2136</v>
       </c>
       <c r="R288" s="1" t="s">
-        <v>2142</v>
+        <v>2137</v>
       </c>
       <c r="S288" s="1" t="s">
-        <v>2143</v>
+        <v>2138</v>
       </c>
       <c r="U288" s="1" t="s">
-        <v>2144</v>
+        <v>2139</v>
       </c>
     </row>
     <row r="289" spans="1:21" x14ac:dyDescent="0.3">
@@ -24816,7 +24813,7 @@
     </row>
     <row r="290" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A290" s="3" t="s">
-        <v>1912</v>
+        <v>1907</v>
       </c>
       <c r="B290" s="1" t="s">
         <v>22</v>
@@ -24825,13 +24822,13 @@
         <v>37</v>
       </c>
       <c r="D290" s="1" t="s">
-        <v>1913</v>
+        <v>1908</v>
       </c>
       <c r="E290" s="2">
         <v>2001</v>
       </c>
       <c r="F290" s="1" t="s">
-        <v>1914</v>
+        <v>1909</v>
       </c>
       <c r="G290" s="2" t="s">
         <v>25</v>
@@ -24842,7 +24839,7 @@
       </c>
       <c r="J290" s="1"/>
       <c r="K290" s="1" t="s">
-        <v>1915</v>
+        <v>1910</v>
       </c>
       <c r="L290" s="2" t="s">
         <v>25</v>
@@ -24852,27 +24849,27 @@
         <v>178</v>
       </c>
       <c r="O290" s="3" t="s">
+        <v>1911</v>
+      </c>
+      <c r="Q290" s="1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="R290" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="S290" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="T290" s="1" t="s">
         <v>1916</v>
       </c>
-      <c r="Q290" s="1" t="s">
-        <v>1917</v>
-      </c>
-      <c r="R290" s="1" t="s">
-        <v>1919</v>
-      </c>
-      <c r="S290" s="1" t="s">
-        <v>1920</v>
-      </c>
-      <c r="T290" s="1" t="s">
-        <v>1921</v>
-      </c>
       <c r="U290" s="1" t="s">
-        <v>1918</v>
+        <v>1913</v>
       </c>
     </row>
     <row r="291" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A291" s="3" t="s">
-        <v>1922</v>
+        <v>1917</v>
       </c>
       <c r="B291" s="1" t="s">
         <v>22</v>
@@ -24881,13 +24878,13 @@
         <v>37</v>
       </c>
       <c r="D291" s="1" t="s">
-        <v>1923</v>
+        <v>1918</v>
       </c>
       <c r="E291" s="2">
         <v>2002</v>
       </c>
       <c r="F291" s="1" t="s">
-        <v>1914</v>
+        <v>1909</v>
       </c>
       <c r="G291" s="2" t="s">
         <v>27</v>
@@ -24897,10 +24894,10 @@
         <v>25</v>
       </c>
       <c r="J291" s="1" t="s">
-        <v>1913</v>
+        <v>1908</v>
       </c>
       <c r="K291" s="1" t="s">
-        <v>1924</v>
+        <v>1919</v>
       </c>
       <c r="L291" s="2" t="s">
         <v>25</v>
@@ -24910,27 +24907,27 @@
         <v>179</v>
       </c>
       <c r="O291" s="3" t="s">
+        <v>1911</v>
+      </c>
+      <c r="Q291" s="1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="R291" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="S291" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="T291" s="1" t="s">
         <v>1916</v>
       </c>
-      <c r="Q291" s="1" t="s">
-        <v>1917</v>
-      </c>
-      <c r="R291" s="1" t="s">
-        <v>1919</v>
-      </c>
-      <c r="S291" s="1" t="s">
+      <c r="U291" s="1" t="s">
         <v>1920</v>
-      </c>
-      <c r="T291" s="1" t="s">
-        <v>1921</v>
-      </c>
-      <c r="U291" s="1" t="s">
-        <v>1925</v>
       </c>
     </row>
     <row r="292" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A292" s="3" t="s">
-        <v>1926</v>
+        <v>1921</v>
       </c>
       <c r="B292" s="1" t="s">
         <v>22</v>
@@ -24939,13 +24936,13 @@
         <v>37</v>
       </c>
       <c r="D292" s="1" t="s">
-        <v>1924</v>
+        <v>1919</v>
       </c>
       <c r="E292" s="2">
         <v>2003</v>
       </c>
       <c r="F292" s="1" t="s">
-        <v>1914</v>
+        <v>1909</v>
       </c>
       <c r="G292" s="2" t="s">
         <v>27</v>
@@ -24955,7 +24952,7 @@
         <v>25</v>
       </c>
       <c r="J292" s="1" t="s">
-        <v>1927</v>
+        <v>1922</v>
       </c>
       <c r="K292" s="1"/>
       <c r="L292" s="2" t="s">
@@ -24966,22 +24963,22 @@
         <v>201</v>
       </c>
       <c r="O292" s="3" t="s">
+        <v>1911</v>
+      </c>
+      <c r="Q292" s="1" t="s">
+        <v>1912</v>
+      </c>
+      <c r="R292" s="1" t="s">
+        <v>1914</v>
+      </c>
+      <c r="S292" s="1" t="s">
+        <v>1915</v>
+      </c>
+      <c r="T292" s="1" t="s">
         <v>1916</v>
       </c>
-      <c r="Q292" s="1" t="s">
-        <v>1917</v>
-      </c>
-      <c r="R292" s="1" t="s">
-        <v>1919</v>
-      </c>
-      <c r="S292" s="1" t="s">
-        <v>1920</v>
-      </c>
-      <c r="T292" s="1" t="s">
-        <v>1921</v>
-      </c>
       <c r="U292" s="1" t="s">
-        <v>1928</v>
+        <v>1923</v>
       </c>
     </row>
     <row r="293" spans="1:21" x14ac:dyDescent="0.3">
@@ -26173,7 +26170,7 @@
     </row>
     <row r="312" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A312" s="3" t="s">
-        <v>2044</v>
+        <v>2039</v>
       </c>
       <c r="B312" s="1" t="s">
         <v>22</v>
@@ -26182,7 +26179,7 @@
         <v>37</v>
       </c>
       <c r="D312" s="1" t="s">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="E312" s="2">
         <v>1995</v>
@@ -26197,13 +26194,13 @@
         <v>25</v>
       </c>
       <c r="K312" s="4" t="s">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="L312" s="7" t="s">
         <v>27</v>
       </c>
       <c r="M312" s="4" t="s">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="N312" s="7">
         <v>101</v>
@@ -26212,24 +26209,24 @@
         <v>1117</v>
       </c>
       <c r="Q312" s="1" t="s">
-        <v>2048</v>
+        <v>2043</v>
       </c>
       <c r="R312" s="1" t="s">
-        <v>2050</v>
+        <v>2045</v>
       </c>
       <c r="S312" s="1" t="s">
-        <v>2051</v>
+        <v>2046</v>
       </c>
       <c r="T312" s="1" t="s">
-        <v>2052</v>
+        <v>2047</v>
       </c>
       <c r="U312" s="1" t="s">
-        <v>2049</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="313" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A313" s="3" t="s">
-        <v>2053</v>
+        <v>2048</v>
       </c>
       <c r="B313" s="1" t="s">
         <v>22</v>
@@ -26238,7 +26235,7 @@
         <v>37</v>
       </c>
       <c r="D313" s="1" t="s">
-        <v>2046</v>
+        <v>2041</v>
       </c>
       <c r="E313" s="2">
         <v>2004</v>
@@ -26253,13 +26250,13 @@
         <v>25</v>
       </c>
       <c r="J313" s="4" t="s">
-        <v>2045</v>
+        <v>2040</v>
       </c>
       <c r="L313" s="7" t="s">
         <v>27</v>
       </c>
       <c r="M313" s="4" t="s">
-        <v>2047</v>
+        <v>2042</v>
       </c>
       <c r="N313" s="7">
         <v>80</v>
@@ -26268,19 +26265,19 @@
         <v>447</v>
       </c>
       <c r="Q313" s="1" t="s">
-        <v>2054</v>
+        <v>2049</v>
       </c>
       <c r="R313" s="1" t="s">
-        <v>2056</v>
+        <v>2051</v>
       </c>
       <c r="S313" s="1" t="s">
-        <v>2051</v>
+        <v>2046</v>
       </c>
       <c r="T313" s="1" t="s">
-        <v>2055</v>
+        <v>2050</v>
       </c>
       <c r="U313" s="1" t="s">
-        <v>2049</v>
+        <v>2044</v>
       </c>
     </row>
     <row r="314" spans="1:21" x14ac:dyDescent="0.3">
@@ -27609,7 +27606,7 @@
     </row>
     <row r="335" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A335" s="3" t="s">
-        <v>1886</v>
+        <v>1881</v>
       </c>
       <c r="B335" s="3" t="s">
         <v>22</v>
@@ -27618,7 +27615,7 @@
         <v>37</v>
       </c>
       <c r="D335" s="3" t="s">
-        <v>1887</v>
+        <v>1882</v>
       </c>
       <c r="E335" s="2">
         <v>2009</v>
@@ -27637,7 +27634,7 @@
         <v>28</v>
       </c>
       <c r="K335" s="3" t="s">
-        <v>1888</v>
+        <v>1883</v>
       </c>
       <c r="L335" s="2" t="s">
         <v>25</v>
@@ -27649,7 +27646,7 @@
         <v>84</v>
       </c>
       <c r="O335" s="3" t="s">
-        <v>1889</v>
+        <v>1884</v>
       </c>
       <c r="P335" s="3" t="s">
         <v>28</v>
@@ -27735,7 +27732,7 @@
     </row>
     <row r="337" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A337" s="3" t="s">
-        <v>1890</v>
+        <v>1885</v>
       </c>
       <c r="B337" s="3" t="s">
         <v>22</v>
@@ -27744,7 +27741,7 @@
         <v>23</v>
       </c>
       <c r="D337" s="3" t="s">
-        <v>1888</v>
+        <v>1883</v>
       </c>
       <c r="E337" s="2">
         <v>2019</v>
@@ -27760,7 +27757,7 @@
         <v>25</v>
       </c>
       <c r="J337" s="3" t="s">
-        <v>1887</v>
+        <v>1882</v>
       </c>
       <c r="K337" s="3" t="s">
         <v>28</v>
@@ -27775,7 +27772,7 @@
         <v>99</v>
       </c>
       <c r="O337" s="3" t="s">
-        <v>1889</v>
+        <v>1884</v>
       </c>
       <c r="P337" s="3" t="s">
         <v>28</v>
@@ -29001,7 +28998,7 @@
     </row>
     <row r="357" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A357" s="3" t="s">
-        <v>1865</v>
+        <v>1862</v>
       </c>
       <c r="B357" s="3" t="s">
         <v>22</v>
@@ -29010,7 +29007,7 @@
         <v>37</v>
       </c>
       <c r="D357" s="3" t="s">
-        <v>1866</v>
+        <v>1863</v>
       </c>
       <c r="E357" s="2">
         <v>2019</v>
@@ -29026,10 +29023,10 @@
         <v>25</v>
       </c>
       <c r="J357" s="3" t="s">
-        <v>1867</v>
+        <v>2195</v>
       </c>
       <c r="K357" s="3" t="s">
-        <v>1868</v>
+        <v>1864</v>
       </c>
       <c r="L357" s="2" t="s">
         <v>25</v>
@@ -29303,7 +29300,7 @@
     </row>
     <row r="362" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A362" s="1" t="s">
-        <v>2150</v>
+        <v>2145</v>
       </c>
       <c r="B362" s="1" t="s">
         <v>22</v>
@@ -29312,13 +29309,13 @@
         <v>23</v>
       </c>
       <c r="D362" s="1" t="s">
-        <v>2151</v>
+        <v>2146</v>
       </c>
       <c r="E362" s="2">
         <v>1962</v>
       </c>
       <c r="F362" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G362" s="7" t="s">
         <v>27</v>
@@ -29330,27 +29327,27 @@
         <v>153</v>
       </c>
       <c r="O362" s="1" t="s">
+        <v>2148</v>
+      </c>
+      <c r="Q362" s="1" t="s">
+        <v>2149</v>
+      </c>
+      <c r="R362" s="1" t="s">
+        <v>2151</v>
+      </c>
+      <c r="S362" s="1" t="s">
+        <v>2152</v>
+      </c>
+      <c r="T362" s="1" t="s">
         <v>2153</v>
       </c>
-      <c r="Q362" s="1" t="s">
-        <v>2154</v>
-      </c>
-      <c r="R362" s="1" t="s">
-        <v>2156</v>
-      </c>
-      <c r="S362" s="1" t="s">
-        <v>2157</v>
-      </c>
-      <c r="T362" s="1" t="s">
-        <v>2158</v>
-      </c>
       <c r="U362" s="1" t="s">
-        <v>2155</v>
+        <v>2150</v>
       </c>
     </row>
     <row r="363" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A363" s="1" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
       <c r="B363" s="1" t="s">
         <v>22</v>
@@ -29359,13 +29356,13 @@
         <v>23</v>
       </c>
       <c r="D363" s="1" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="E363" s="2">
         <v>1968</v>
       </c>
       <c r="F363" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G363" s="7" t="s">
         <v>27</v>
@@ -29377,27 +29374,27 @@
         <v>149</v>
       </c>
       <c r="O363" s="1" t="s">
+        <v>2156</v>
+      </c>
+      <c r="Q363" s="1" t="s">
+        <v>2157</v>
+      </c>
+      <c r="R363" s="1" t="s">
+        <v>2159</v>
+      </c>
+      <c r="S363" s="1" t="s">
+        <v>2158</v>
+      </c>
+      <c r="T363" s="1" t="s">
+        <v>2160</v>
+      </c>
+      <c r="U363" s="1" t="s">
         <v>2161</v>
-      </c>
-      <c r="Q363" s="1" t="s">
-        <v>2162</v>
-      </c>
-      <c r="R363" s="1" t="s">
-        <v>2164</v>
-      </c>
-      <c r="S363" s="1" t="s">
-        <v>2163</v>
-      </c>
-      <c r="T363" s="1" t="s">
-        <v>2165</v>
-      </c>
-      <c r="U363" s="1" t="s">
-        <v>2166</v>
       </c>
     </row>
     <row r="364" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A364" s="1" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="B364" s="1" t="s">
         <v>22</v>
@@ -29406,13 +29403,13 @@
         <v>23</v>
       </c>
       <c r="D364" s="1" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
       <c r="E364" s="2">
         <v>1971</v>
       </c>
       <c r="F364" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G364" s="7" t="s">
         <v>27</v>
@@ -29424,27 +29421,27 @@
         <v>136</v>
       </c>
       <c r="O364" s="1" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
       <c r="Q364" s="1" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="R364" s="1" t="s">
-        <v>2170</v>
+        <v>2165</v>
       </c>
       <c r="S364" s="1" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="T364" s="1" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="U364" s="1" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
     </row>
     <row r="365" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A365" s="1" t="s">
-        <v>2174</v>
+        <v>2169</v>
       </c>
       <c r="B365" s="1" t="s">
         <v>22</v>
@@ -29453,13 +29450,13 @@
         <v>23</v>
       </c>
       <c r="D365" s="1" t="s">
-        <v>2175</v>
+        <v>2170</v>
       </c>
       <c r="E365" s="2">
         <v>1975</v>
       </c>
       <c r="F365" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G365" s="7" t="s">
         <v>27</v>
@@ -29471,27 +29468,27 @@
         <v>185</v>
       </c>
       <c r="O365" s="1" t="s">
-        <v>2176</v>
+        <v>2171</v>
       </c>
       <c r="Q365" s="1" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="R365" s="1" t="s">
-        <v>2178</v>
+        <v>2173</v>
       </c>
       <c r="S365" s="1" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="T365" s="1" t="s">
+        <v>2167</v>
+      </c>
+      <c r="U365" s="1" t="s">
         <v>2172</v>
-      </c>
-      <c r="U365" s="1" t="s">
-        <v>2177</v>
       </c>
     </row>
     <row r="366" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A366" s="1" t="s">
-        <v>2179</v>
+        <v>2174</v>
       </c>
       <c r="B366" s="1" t="s">
         <v>22</v>
@@ -29500,13 +29497,13 @@
         <v>23</v>
       </c>
       <c r="D366" s="1" t="s">
-        <v>2180</v>
+        <v>2175</v>
       </c>
       <c r="E366" s="2">
         <v>1980</v>
       </c>
       <c r="F366" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G366" s="7" t="s">
         <v>25</v>
@@ -29518,27 +29515,27 @@
         <v>146</v>
       </c>
       <c r="O366" s="1" t="s">
-        <v>2181</v>
+        <v>2176</v>
       </c>
       <c r="Q366" s="1" t="s">
-        <v>2182</v>
+        <v>2177</v>
       </c>
       <c r="R366" s="1" t="s">
-        <v>2184</v>
+        <v>2179</v>
       </c>
       <c r="S366" s="1" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="T366" s="1" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="U366" s="1" t="s">
-        <v>2183</v>
+        <v>2178</v>
       </c>
     </row>
     <row r="367" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A367" s="1" t="s">
-        <v>2185</v>
+        <v>2180</v>
       </c>
       <c r="B367" s="1" t="s">
         <v>22</v>
@@ -29547,13 +29544,13 @@
         <v>23</v>
       </c>
       <c r="D367" s="1" t="s">
-        <v>2186</v>
+        <v>2181</v>
       </c>
       <c r="E367" s="2">
         <v>1987</v>
       </c>
       <c r="F367" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G367" s="7" t="s">
         <v>27</v>
@@ -29565,27 +29562,27 @@
         <v>116</v>
       </c>
       <c r="O367" s="1" t="s">
+        <v>2182</v>
+      </c>
+      <c r="Q367" s="1" t="s">
+        <v>2183</v>
+      </c>
+      <c r="R367" s="1" t="s">
+        <v>2185</v>
+      </c>
+      <c r="S367" s="1" t="s">
+        <v>2186</v>
+      </c>
+      <c r="T367" s="1" t="s">
         <v>2187</v>
       </c>
-      <c r="Q367" s="1" t="s">
-        <v>2188</v>
-      </c>
-      <c r="R367" s="1" t="s">
-        <v>2190</v>
-      </c>
-      <c r="S367" s="1" t="s">
-        <v>2191</v>
-      </c>
-      <c r="T367" s="1" t="s">
-        <v>2192</v>
-      </c>
       <c r="U367" s="1" t="s">
-        <v>2189</v>
+        <v>2184</v>
       </c>
     </row>
     <row r="368" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A368" s="1" t="s">
-        <v>2193</v>
+        <v>2188</v>
       </c>
       <c r="B368" s="1" t="s">
         <v>22</v>
@@ -29594,13 +29591,13 @@
         <v>23</v>
       </c>
       <c r="D368" s="1" t="s">
-        <v>2194</v>
+        <v>2189</v>
       </c>
       <c r="E368" s="2">
         <v>1999</v>
       </c>
       <c r="F368" s="4" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="G368" s="7" t="s">
         <v>27</v>
@@ -29615,19 +29612,19 @@
         <v>112</v>
       </c>
       <c r="Q368" s="1" t="s">
-        <v>2195</v>
+        <v>2190</v>
       </c>
       <c r="R368" s="1" t="s">
-        <v>2197</v>
+        <v>2192</v>
       </c>
       <c r="S368" s="1" t="s">
-        <v>2198</v>
+        <v>2193</v>
       </c>
       <c r="T368" s="1" t="s">
-        <v>2199</v>
+        <v>2194</v>
       </c>
       <c r="U368" s="1" t="s">
-        <v>2196</v>
+        <v>2191</v>
       </c>
     </row>
     <row r="369" spans="1:21" x14ac:dyDescent="0.3">
@@ -30703,7 +30700,7 @@
     </row>
     <row r="386" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A386" s="3" t="s">
-        <v>1955</v>
+        <v>1950</v>
       </c>
       <c r="B386" s="1" t="s">
         <v>22</v>
@@ -30712,7 +30709,7 @@
         <v>23</v>
       </c>
       <c r="D386" s="1" t="s">
-        <v>1956</v>
+        <v>1951</v>
       </c>
       <c r="E386" s="2">
         <v>1971</v>
@@ -30733,19 +30730,19 @@
         <v>1006</v>
       </c>
       <c r="Q386" s="1" t="s">
-        <v>1957</v>
+        <v>1952</v>
       </c>
       <c r="R386" s="1" t="s">
-        <v>1959</v>
+        <v>1954</v>
       </c>
       <c r="S386" s="1" t="s">
-        <v>1960</v>
+        <v>1955</v>
       </c>
       <c r="T386" s="1" t="s">
-        <v>1961</v>
+        <v>1956</v>
       </c>
       <c r="U386" s="1" t="s">
-        <v>1958</v>
+        <v>1953</v>
       </c>
     </row>
     <row r="387" spans="1:21" x14ac:dyDescent="0.3">
@@ -31762,7 +31759,7 @@
     </row>
     <row r="403" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A403" s="3" t="s">
-        <v>2017</v>
+        <v>2012</v>
       </c>
       <c r="B403" s="1" t="s">
         <v>22</v>
@@ -31771,7 +31768,7 @@
         <v>37</v>
       </c>
       <c r="D403" s="1" t="s">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="E403" s="2">
         <v>1988</v>
@@ -31786,7 +31783,7 @@
         <v>25</v>
       </c>
       <c r="K403" s="4" t="s">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="L403" s="7" t="s">
         <v>25</v>
@@ -31795,22 +31792,22 @@
         <v>92</v>
       </c>
       <c r="O403" s="3" t="s">
+        <v>2015</v>
+      </c>
+      <c r="Q403" s="1" t="s">
+        <v>2016</v>
+      </c>
+      <c r="R403" s="1" t="s">
+        <v>2018</v>
+      </c>
+      <c r="S403" s="1" t="s">
+        <v>2019</v>
+      </c>
+      <c r="T403" s="1" t="s">
         <v>2020</v>
       </c>
-      <c r="Q403" s="1" t="s">
-        <v>2021</v>
-      </c>
-      <c r="R403" s="1" t="s">
-        <v>2023</v>
-      </c>
-      <c r="S403" s="1" t="s">
-        <v>2024</v>
-      </c>
-      <c r="T403" s="1" t="s">
-        <v>2025</v>
-      </c>
       <c r="U403" s="1" t="s">
-        <v>2022</v>
+        <v>2017</v>
       </c>
     </row>
     <row r="404" spans="1:21" x14ac:dyDescent="0.3">
@@ -31878,7 +31875,7 @@
     </row>
     <row r="405" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A405" s="3" t="s">
-        <v>2114</v>
+        <v>2109</v>
       </c>
       <c r="B405" s="1" t="s">
         <v>90</v>
@@ -31887,7 +31884,7 @@
         <v>37</v>
       </c>
       <c r="D405" s="1" t="s">
-        <v>2106</v>
+        <v>2101</v>
       </c>
       <c r="E405" s="2">
         <v>2022</v>
@@ -31905,33 +31902,33 @@
         <v>27</v>
       </c>
       <c r="M405" s="4" t="s">
-        <v>2107</v>
+        <v>2102</v>
       </c>
       <c r="N405" s="7">
         <v>45</v>
       </c>
       <c r="O405" s="3" t="s">
+        <v>2103</v>
+      </c>
+      <c r="Q405" s="1" t="s">
+        <v>2104</v>
+      </c>
+      <c r="R405" s="1" t="s">
+        <v>2105</v>
+      </c>
+      <c r="S405" s="1" t="s">
+        <v>2106</v>
+      </c>
+      <c r="T405" s="1" t="s">
+        <v>2107</v>
+      </c>
+      <c r="U405" s="1" t="s">
         <v>2108</v>
-      </c>
-      <c r="Q405" s="1" t="s">
-        <v>2109</v>
-      </c>
-      <c r="R405" s="1" t="s">
-        <v>2110</v>
-      </c>
-      <c r="S405" s="1" t="s">
-        <v>2111</v>
-      </c>
-      <c r="T405" s="1" t="s">
-        <v>2112</v>
-      </c>
-      <c r="U405" s="1" t="s">
-        <v>2113</v>
       </c>
     </row>
     <row r="406" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A406" s="3" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="B406" s="1" t="s">
         <v>22</v>
@@ -31940,7 +31937,7 @@
         <v>37</v>
       </c>
       <c r="D406" s="1" t="s">
-        <v>2019</v>
+        <v>2014</v>
       </c>
       <c r="E406" s="2">
         <v>2024</v>
@@ -31955,7 +31952,7 @@
         <v>25</v>
       </c>
       <c r="J406" s="4" t="s">
-        <v>2018</v>
+        <v>2013</v>
       </c>
       <c r="L406" s="7" t="s">
         <v>25</v>
@@ -31964,27 +31961,27 @@
         <v>105</v>
       </c>
       <c r="O406" s="3" t="s">
-        <v>2020</v>
+        <v>2015</v>
       </c>
       <c r="Q406" s="1" t="s">
-        <v>2089</v>
+        <v>2084</v>
       </c>
       <c r="R406" s="1" t="s">
-        <v>2023</v>
+        <v>2018</v>
       </c>
       <c r="S406" s="1" t="s">
-        <v>2091</v>
+        <v>2086</v>
       </c>
       <c r="T406" s="1" t="s">
         <v>298</v>
       </c>
       <c r="U406" s="1" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
     </row>
     <row r="407" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A407" s="3" t="s">
-        <v>1929</v>
+        <v>1924</v>
       </c>
       <c r="B407" s="1" t="s">
         <v>22</v>
@@ -31993,13 +31990,13 @@
         <v>37</v>
       </c>
       <c r="D407" s="1" t="s">
-        <v>1930</v>
+        <v>1925</v>
       </c>
       <c r="E407" s="2">
         <v>2005</v>
       </c>
       <c r="F407" s="4" t="s">
-        <v>1931</v>
+        <v>1926</v>
       </c>
       <c r="G407" s="7" t="s">
         <v>25</v>
@@ -32011,7 +32008,7 @@
         <v>27</v>
       </c>
       <c r="M407" s="4" t="s">
-        <v>1932</v>
+        <v>1927</v>
       </c>
       <c r="N407" s="7">
         <v>106</v>
@@ -32020,19 +32017,19 @@
         <v>1790</v>
       </c>
       <c r="Q407" s="1" t="s">
-        <v>1933</v>
+        <v>1928</v>
       </c>
       <c r="R407" s="1" t="s">
-        <v>1935</v>
+        <v>1930</v>
       </c>
       <c r="S407" s="1" t="s">
-        <v>1936</v>
+        <v>1931</v>
       </c>
       <c r="T407" s="1" t="s">
-        <v>1937</v>
+        <v>1932</v>
       </c>
       <c r="U407" s="1" t="s">
-        <v>1934</v>
+        <v>1929</v>
       </c>
     </row>
     <row r="408" spans="1:21" x14ac:dyDescent="0.3">
@@ -32688,7 +32685,7 @@
         <v>25</v>
       </c>
       <c r="H418" s="2" t="s">
-        <v>2066</v>
+        <v>2061</v>
       </c>
       <c r="I418" s="2" t="s">
         <v>27</v>
@@ -33299,7 +33296,7 @@
     </row>
     <row r="428" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A428" s="3" t="s">
-        <v>2092</v>
+        <v>2087</v>
       </c>
       <c r="B428" s="1" t="s">
         <v>22</v>
@@ -33308,13 +33305,13 @@
         <v>37</v>
       </c>
       <c r="D428" s="1" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
       <c r="E428" s="2">
         <v>2024</v>
       </c>
       <c r="F428" s="4" t="s">
-        <v>2094</v>
+        <v>2089</v>
       </c>
       <c r="G428" s="7" t="s">
         <v>27</v>
@@ -33326,22 +33323,22 @@
         <v>102</v>
       </c>
       <c r="O428" s="3" t="s">
+        <v>2090</v>
+      </c>
+      <c r="Q428" s="1" t="s">
+        <v>2091</v>
+      </c>
+      <c r="R428" s="1" t="s">
+        <v>2093</v>
+      </c>
+      <c r="S428" s="1" t="s">
+        <v>2094</v>
+      </c>
+      <c r="T428" s="1" t="s">
         <v>2095</v>
       </c>
-      <c r="Q428" s="1" t="s">
-        <v>2096</v>
-      </c>
-      <c r="R428" s="1" t="s">
-        <v>2098</v>
-      </c>
-      <c r="S428" s="1" t="s">
-        <v>2099</v>
-      </c>
-      <c r="T428" s="1" t="s">
-        <v>2100</v>
-      </c>
       <c r="U428" s="1" t="s">
-        <v>2097</v>
+        <v>2092</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fixed naming in csv and also tag typo
</commit_message>
<xml_diff>
--- a/content/database.xlsx
+++ b/content/database.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hannah\life\dabad2_0\dabad\content\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA75449D-5C58-42CE-81B8-704418845EA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EC7A4A59-0672-47F3-9387-CBDFCA8428C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{19379007-CF45-4D83-A844-C3FD6EF3BA4D}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5768" uniqueCount="2731">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5768" uniqueCount="2730">
   <si>
     <t>ID</t>
   </si>
@@ -7081,15 +7081,6 @@
     <t>Django Unchained</t>
   </si>
   <si>
-    <t>Pirates of the Caribbean: The Curse of the Black Pearl</t>
-  </si>
-  <si>
-    <t>Pirates of the Caribbean: Dead Man's Chest</t>
-  </si>
-  <si>
-    <t>Pirates of the Caribbean: At World's End</t>
-  </si>
-  <si>
     <t>Titanic</t>
   </si>
   <si>
@@ -7585,15 +7576,6 @@
     <t>Jamie Foxx, Christoph Waltz, Leonardo DiCaprio, Kerry Washington, Samuel L. Jackson, Walton Goggins, Dennis Christopher, James Remar, David Stehen</t>
   </si>
   <si>
-    <t>Pirates_Of_The_Carribean_The_Curse_Of_The_Black_Pearl_2003</t>
-  </si>
-  <si>
-    <t>Pirates_Of_The_Carribean_Dead_Mans_Chest_2006</t>
-  </si>
-  <si>
-    <t>Pirates_Of_The_Carribean_At_Worlds_End_2007</t>
-  </si>
-  <si>
     <t>Pirates of the Carribean: Dead Man's Chest, Pirates of the Carribean: At World's End</t>
   </si>
   <si>
@@ -8182,9 +8164,6 @@
     <t>Adam Elliot</t>
   </si>
   <si>
-    <t>Animaton, Comedy, Drama</t>
-  </si>
-  <si>
     <t>Jacki Weaver, Sarah Snook, Charlotte Belsey, Agnes Davison, Mason Litsos, Daniel Agdag, Eric Bana, Kodi Smit-McPhee</t>
   </si>
   <si>
@@ -8216,6 +8195,24 @@
   </si>
   <si>
     <t>Margaret Qualley, Geraldine Viswanathan, Beanie Feldstein, Joey Slotnick, C.J. Wilson, Colman Domingo, Pedro Pascal, Bill Camp, Matt Damon</t>
+  </si>
+  <si>
+    <t>Pirates of the Carribbean: The Curse of the Black Pearl</t>
+  </si>
+  <si>
+    <t>Pirates of the Carribbean: Dead Man's Chest</t>
+  </si>
+  <si>
+    <t>Pirates of the Carribbean: At World's End</t>
+  </si>
+  <si>
+    <t>Pirates_Of_The_Carribbean_At_Worlds_End_2007</t>
+  </si>
+  <si>
+    <t>Pirates_Of_The_Carribbean_Dead_Mans_Chest_2006</t>
+  </si>
+  <si>
+    <t>Pirates_Of_The_Carribbean_The_Curse_Of_The_Black_Pearl_2003</t>
   </si>
 </sst>
 </file>
@@ -9092,9 +9089,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A95FB3FF-36B5-4204-8D1D-937EE61C148B}">
   <dimension ref="A1:U507"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="108" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A399" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F476" sqref="F476"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="108" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9221,7 +9218,7 @@
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>2716</v>
+        <v>2710</v>
       </c>
       <c r="B3" t="s">
         <v>22</v>
@@ -9230,13 +9227,13 @@
         <v>53</v>
       </c>
       <c r="D3" t="s">
-        <v>2717</v>
+        <v>2711</v>
       </c>
       <c r="E3" s="3">
         <v>2024</v>
       </c>
       <c r="F3" t="s">
-        <v>2718</v>
+        <v>2712</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>31</v>
@@ -9248,19 +9245,19 @@
         <v>95</v>
       </c>
       <c r="O3" t="s">
-        <v>2719</v>
+        <v>2248</v>
       </c>
       <c r="Q3" t="s">
-        <v>2718</v>
+        <v>2712</v>
       </c>
       <c r="R3" t="s">
-        <v>2721</v>
+        <v>2714</v>
       </c>
       <c r="S3" t="s">
-        <v>2722</v>
+        <v>2715</v>
       </c>
       <c r="U3" t="s">
-        <v>2720</v>
+        <v>2713</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.3">
@@ -9479,7 +9476,7 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>2594</v>
+        <v>2588</v>
       </c>
       <c r="B9" t="s">
         <v>22</v>
@@ -9488,7 +9485,7 @@
         <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>2375</v>
+        <v>2372</v>
       </c>
       <c r="E9" s="3">
         <v>2002</v>
@@ -9509,19 +9506,19 @@
         <v>1048</v>
       </c>
       <c r="Q9" t="s">
-        <v>2668</v>
+        <v>2662</v>
       </c>
       <c r="R9" t="s">
-        <v>2446</v>
+        <v>2443</v>
       </c>
       <c r="S9" t="s">
-        <v>2670</v>
+        <v>2664</v>
       </c>
       <c r="T9" t="s">
         <v>2336</v>
       </c>
       <c r="U9" t="s">
-        <v>2669</v>
+        <v>2663</v>
       </c>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.3">
@@ -9792,7 +9789,7 @@
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>2625</v>
+        <v>2619</v>
       </c>
       <c r="B17" t="s">
         <v>22</v>
@@ -9801,13 +9798,13 @@
         <v>23</v>
       </c>
       <c r="D17" t="s">
-        <v>2383</v>
+        <v>2380</v>
       </c>
       <c r="E17" s="3">
         <v>2008</v>
       </c>
       <c r="F17" t="s">
-        <v>2707</v>
+        <v>2701</v>
       </c>
       <c r="G17" s="3" t="s">
         <v>31</v>
@@ -9819,22 +9816,22 @@
         <v>112</v>
       </c>
       <c r="O17" t="s">
-        <v>2708</v>
+        <v>2702</v>
       </c>
       <c r="Q17" t="s">
-        <v>2709</v>
+        <v>2703</v>
       </c>
       <c r="R17" t="s">
-        <v>2711</v>
+        <v>2705</v>
       </c>
       <c r="S17" t="s">
         <v>882</v>
       </c>
       <c r="T17" t="s">
-        <v>2712</v>
+        <v>2706</v>
       </c>
       <c r="U17" t="s">
-        <v>2710</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.3">
@@ -9871,7 +9868,7 @@
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>2597</v>
+        <v>2591</v>
       </c>
       <c r="B19" t="s">
         <v>22</v>
@@ -9880,7 +9877,7 @@
         <v>23</v>
       </c>
       <c r="D19" t="s">
-        <v>2381</v>
+        <v>2378</v>
       </c>
       <c r="E19" s="3">
         <v>2005</v>
@@ -9898,13 +9895,13 @@
         <v>134</v>
       </c>
       <c r="O19" t="s">
-        <v>2692</v>
+        <v>2686</v>
       </c>
       <c r="Q19" t="s">
-        <v>2693</v>
+        <v>2687</v>
       </c>
       <c r="R19" t="s">
-        <v>2695</v>
+        <v>2689</v>
       </c>
       <c r="S19" t="s">
         <v>130</v>
@@ -9913,7 +9910,7 @@
         <v>1908</v>
       </c>
       <c r="U19" t="s">
-        <v>2694</v>
+        <v>2688</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.3">
@@ -10108,7 +10105,7 @@
     </row>
     <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>2455</v>
+        <v>2452</v>
       </c>
       <c r="B25" t="s">
         <v>22</v>
@@ -10117,13 +10114,13 @@
         <v>23</v>
       </c>
       <c r="D25" t="s">
-        <v>2385</v>
+        <v>2382</v>
       </c>
       <c r="E25" s="3">
         <v>2008</v>
       </c>
       <c r="F25" t="s">
-        <v>2456</v>
+        <v>2453</v>
       </c>
       <c r="G25" s="3" t="s">
         <v>25</v>
@@ -10138,19 +10135,19 @@
         <v>1886</v>
       </c>
       <c r="Q25" t="s">
+        <v>2454</v>
+      </c>
+      <c r="R25" t="s">
+        <v>2456</v>
+      </c>
+      <c r="S25" t="s">
         <v>2457</v>
       </c>
-      <c r="R25" t="s">
-        <v>2459</v>
-      </c>
-      <c r="S25" t="s">
-        <v>2460</v>
-      </c>
       <c r="T25" t="s">
-        <v>2461</v>
+        <v>2458</v>
       </c>
       <c r="U25" t="s">
-        <v>2458</v>
+        <v>2455</v>
       </c>
     </row>
     <row r="26" spans="1:21" x14ac:dyDescent="0.3">
@@ -10205,7 +10202,7 @@
     </row>
     <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>2587</v>
+        <v>2581</v>
       </c>
       <c r="B27" t="s">
         <v>22</v>
@@ -10214,13 +10211,13 @@
         <v>23</v>
       </c>
       <c r="D27" t="s">
-        <v>2364</v>
+        <v>2361</v>
       </c>
       <c r="E27" s="3">
         <v>2013</v>
       </c>
       <c r="F27" t="s">
-        <v>2598</v>
+        <v>2592</v>
       </c>
       <c r="G27" s="3" t="s">
         <v>25</v>
@@ -10232,22 +10229,22 @@
         <v>114</v>
       </c>
       <c r="O27" t="s">
-        <v>2599</v>
+        <v>2593</v>
       </c>
       <c r="Q27" t="s">
-        <v>2600</v>
+        <v>2594</v>
       </c>
       <c r="R27" t="s">
         <v>912</v>
       </c>
       <c r="S27" t="s">
-        <v>2490</v>
+        <v>2487</v>
       </c>
       <c r="T27" t="s">
         <v>723</v>
       </c>
       <c r="U27" t="s">
-        <v>2601</v>
+        <v>2595</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.3">
@@ -10982,7 +10979,7 @@
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>2472</v>
+        <v>2469</v>
       </c>
       <c r="B45" t="s">
         <v>22</v>
@@ -10991,7 +10988,7 @@
         <v>23</v>
       </c>
       <c r="D45" t="s">
-        <v>2362</v>
+        <v>2359</v>
       </c>
       <c r="E45" s="3">
         <v>2018</v>
@@ -11012,24 +11009,24 @@
         <v>1232</v>
       </c>
       <c r="Q45" t="s">
-        <v>2572</v>
+        <v>2566</v>
       </c>
       <c r="R45" t="s">
-        <v>2573</v>
+        <v>2567</v>
       </c>
       <c r="S45" t="s">
-        <v>2440</v>
+        <v>2437</v>
       </c>
       <c r="T45" t="s">
-        <v>2574</v>
+        <v>2568</v>
       </c>
       <c r="U45" t="s">
-        <v>2575</v>
+        <v>2569</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>2436</v>
+        <v>2433</v>
       </c>
       <c r="B46" t="s">
         <v>22</v>
@@ -11038,7 +11035,7 @@
         <v>23</v>
       </c>
       <c r="D46" t="s">
-        <v>2388</v>
+        <v>2385</v>
       </c>
       <c r="E46" s="3">
         <v>2008</v>
@@ -11056,22 +11053,22 @@
         <v>121</v>
       </c>
       <c r="O46" t="s">
-        <v>2437</v>
+        <v>2434</v>
       </c>
       <c r="Q46" t="s">
-        <v>2438</v>
+        <v>2435</v>
       </c>
       <c r="R46" t="s">
         <v>2083</v>
       </c>
       <c r="S46" t="s">
-        <v>2440</v>
+        <v>2437</v>
       </c>
       <c r="T46" t="s">
-        <v>2441</v>
+        <v>2438</v>
       </c>
       <c r="U46" t="s">
-        <v>2439</v>
+        <v>2436</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
@@ -11266,7 +11263,7 @@
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>2465</v>
+        <v>2462</v>
       </c>
       <c r="B52" t="s">
         <v>22</v>
@@ -11281,7 +11278,7 @@
         <v>2014</v>
       </c>
       <c r="F52" t="s">
-        <v>2499</v>
+        <v>2496</v>
       </c>
       <c r="G52" s="3" t="s">
         <v>25</v>
@@ -11290,13 +11287,13 @@
         <v>31</v>
       </c>
       <c r="K52" s="5" t="s">
-        <v>2506</v>
+        <v>2503</v>
       </c>
       <c r="L52" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M52" t="s">
-        <v>2508</v>
+        <v>2505</v>
       </c>
       <c r="N52" s="3">
         <v>101</v>
@@ -11305,24 +11302,24 @@
         <v>1349</v>
       </c>
       <c r="Q52" t="s">
-        <v>2500</v>
+        <v>2497</v>
       </c>
       <c r="R52" t="s">
-        <v>2502</v>
+        <v>2499</v>
       </c>
       <c r="S52" t="s">
         <v>2208</v>
       </c>
       <c r="T52" t="s">
-        <v>2503</v>
+        <v>2500</v>
       </c>
       <c r="U52" t="s">
-        <v>2501</v>
+        <v>2498</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>2504</v>
+        <v>2501</v>
       </c>
       <c r="B53" t="s">
         <v>22</v>
@@ -11337,7 +11334,7 @@
         <v>2017</v>
       </c>
       <c r="F53" t="s">
-        <v>2499</v>
+        <v>2496</v>
       </c>
       <c r="G53" s="3" t="s">
         <v>25</v>
@@ -11355,7 +11352,7 @@
         <v>25</v>
       </c>
       <c r="M53" t="s">
-        <v>2508</v>
+        <v>2505</v>
       </c>
       <c r="N53" s="3">
         <v>122</v>
@@ -11364,24 +11361,24 @@
         <v>1349</v>
       </c>
       <c r="Q53" t="s">
+        <v>2497</v>
+      </c>
+      <c r="R53" t="s">
+        <v>2499</v>
+      </c>
+      <c r="S53" t="s">
+        <v>2507</v>
+      </c>
+      <c r="T53" t="s">
         <v>2500</v>
       </c>
-      <c r="R53" t="s">
-        <v>2502</v>
-      </c>
-      <c r="S53" t="s">
-        <v>2510</v>
-      </c>
-      <c r="T53" t="s">
-        <v>2503</v>
-      </c>
       <c r="U53" t="s">
-        <v>2509</v>
+        <v>2506</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>2512</v>
+        <v>2509</v>
       </c>
       <c r="B54" t="s">
         <v>22</v>
@@ -11390,13 +11387,13 @@
         <v>23</v>
       </c>
       <c r="D54" t="s">
-        <v>2511</v>
+        <v>2508</v>
       </c>
       <c r="E54" s="3">
         <v>2019</v>
       </c>
       <c r="F54" t="s">
-        <v>2499</v>
+        <v>2496</v>
       </c>
       <c r="G54" s="3" t="s">
         <v>25</v>
@@ -11405,13 +11402,13 @@
         <v>31</v>
       </c>
       <c r="J54" t="s">
-        <v>2507</v>
+        <v>2504</v>
       </c>
       <c r="L54" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M54" t="s">
-        <v>2508</v>
+        <v>2505</v>
       </c>
       <c r="N54" s="3">
         <v>130</v>
@@ -11420,19 +11417,19 @@
         <v>1349</v>
       </c>
       <c r="Q54" t="s">
-        <v>2514</v>
+        <v>2511</v>
       </c>
       <c r="R54" t="s">
-        <v>2502</v>
+        <v>2499</v>
       </c>
       <c r="S54" t="s">
+        <v>2507</v>
+      </c>
+      <c r="T54" t="s">
+        <v>2500</v>
+      </c>
+      <c r="U54" t="s">
         <v>2510</v>
-      </c>
-      <c r="T54" t="s">
-        <v>2503</v>
-      </c>
-      <c r="U54" t="s">
-        <v>2513</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.3">
@@ -11712,7 +11709,7 @@
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>2589</v>
+        <v>2583</v>
       </c>
       <c r="B62" t="s">
         <v>22</v>
@@ -11721,13 +11718,13 @@
         <v>23</v>
       </c>
       <c r="D62" t="s">
-        <v>2366</v>
+        <v>2363</v>
       </c>
       <c r="E62" s="3">
         <v>2006</v>
       </c>
       <c r="F62" t="s">
-        <v>2613</v>
+        <v>2607</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>25</v>
@@ -11742,19 +11739,19 @@
         <v>1232</v>
       </c>
       <c r="Q62" t="s">
-        <v>2614</v>
+        <v>2608</v>
       </c>
       <c r="R62" t="s">
-        <v>2616</v>
+        <v>2610</v>
       </c>
       <c r="S62" t="s">
-        <v>2617</v>
+        <v>2611</v>
       </c>
       <c r="T62" t="s">
-        <v>2618</v>
+        <v>2612</v>
       </c>
       <c r="U62" t="s">
-        <v>2615</v>
+        <v>2609</v>
       </c>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
@@ -12268,7 +12265,7 @@
     </row>
     <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>2596</v>
+        <v>2590</v>
       </c>
       <c r="B76" t="s">
         <v>22</v>
@@ -12277,7 +12274,7 @@
         <v>23</v>
       </c>
       <c r="D76" t="s">
-        <v>2377</v>
+        <v>2374</v>
       </c>
       <c r="E76" s="3">
         <v>2004</v>
@@ -12295,10 +12292,10 @@
         <v>132</v>
       </c>
       <c r="O76" t="s">
-        <v>2657</v>
+        <v>2651</v>
       </c>
       <c r="Q76" t="s">
-        <v>2678</v>
+        <v>2672</v>
       </c>
       <c r="R76" t="s">
         <v>341</v>
@@ -12307,10 +12304,10 @@
         <v>712</v>
       </c>
       <c r="T76" t="s">
-        <v>2679</v>
+        <v>2673</v>
       </c>
       <c r="U76" t="s">
-        <v>2677</v>
+        <v>2671</v>
       </c>
     </row>
     <row r="77" spans="1:21" x14ac:dyDescent="0.3">
@@ -12778,7 +12775,7 @@
     </row>
     <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
-        <v>2592</v>
+        <v>2586</v>
       </c>
       <c r="B88" t="s">
         <v>22</v>
@@ -12787,13 +12784,13 @@
         <v>23</v>
       </c>
       <c r="D88" t="s">
-        <v>2370</v>
+        <v>2367</v>
       </c>
       <c r="E88" s="3">
         <v>2012</v>
       </c>
       <c r="F88" t="s">
-        <v>2638</v>
+        <v>2632</v>
       </c>
       <c r="G88" s="3" t="s">
         <v>25</v>
@@ -12808,7 +12805,7 @@
         <v>87</v>
       </c>
       <c r="Q88" t="s">
-        <v>2639</v>
+        <v>2633</v>
       </c>
       <c r="R88" t="s">
         <v>2242</v>
@@ -12817,15 +12814,15 @@
         <v>2084</v>
       </c>
       <c r="T88" t="s">
-        <v>2640</v>
+        <v>2634</v>
       </c>
       <c r="U88" t="s">
-        <v>2641</v>
+        <v>2635</v>
       </c>
     </row>
     <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
-        <v>2588</v>
+        <v>2582</v>
       </c>
       <c r="B89" t="s">
         <v>22</v>
@@ -12834,13 +12831,13 @@
         <v>23</v>
       </c>
       <c r="D89" t="s">
-        <v>2365</v>
+        <v>2362</v>
       </c>
       <c r="E89" s="3">
         <v>2016</v>
       </c>
       <c r="F89" t="s">
-        <v>2604</v>
+        <v>2598</v>
       </c>
       <c r="G89" s="3" t="s">
         <v>25</v>
@@ -12852,22 +12849,22 @@
         <v>109</v>
       </c>
       <c r="O89" t="s">
-        <v>2605</v>
+        <v>2599</v>
       </c>
       <c r="Q89" t="s">
-        <v>2604</v>
+        <v>2598</v>
       </c>
       <c r="R89" t="s">
-        <v>2607</v>
+        <v>2601</v>
       </c>
       <c r="S89" t="s">
-        <v>2608</v>
+        <v>2602</v>
       </c>
       <c r="T89" t="s">
-        <v>2609</v>
+        <v>2603</v>
       </c>
       <c r="U89" t="s">
-        <v>2606</v>
+        <v>2600</v>
       </c>
     </row>
     <row r="90" spans="1:21" x14ac:dyDescent="0.3">
@@ -12968,7 +12965,7 @@
     </row>
     <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
-        <v>2595</v>
+        <v>2589</v>
       </c>
       <c r="B93" t="s">
         <v>22</v>
@@ -12977,7 +12974,7 @@
         <v>23</v>
       </c>
       <c r="D93" t="s">
-        <v>2376</v>
+        <v>2373</v>
       </c>
       <c r="E93" s="3">
         <v>2008</v>
@@ -12995,22 +12992,22 @@
         <v>109</v>
       </c>
       <c r="O93" t="s">
-        <v>2671</v>
+        <v>2665</v>
       </c>
       <c r="Q93" t="s">
-        <v>2673</v>
+        <v>2667</v>
       </c>
       <c r="R93" t="s">
-        <v>2674</v>
+        <v>2668</v>
       </c>
       <c r="S93" t="s">
-        <v>2675</v>
+        <v>2669</v>
       </c>
       <c r="T93" t="s">
-        <v>2676</v>
+        <v>2670</v>
       </c>
       <c r="U93" t="s">
-        <v>2672</v>
+        <v>2666</v>
       </c>
     </row>
     <row r="94" spans="1:21" x14ac:dyDescent="0.3">
@@ -14194,7 +14191,7 @@
     </row>
     <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
-        <v>2468</v>
+        <v>2465</v>
       </c>
       <c r="B124" t="s">
         <v>22</v>
@@ -14203,13 +14200,13 @@
         <v>23</v>
       </c>
       <c r="D124" t="s">
-        <v>2356</v>
+        <v>2353</v>
       </c>
       <c r="E124" s="3">
         <v>2017</v>
       </c>
       <c r="F124" t="s">
-        <v>2536</v>
+        <v>2530</v>
       </c>
       <c r="G124" s="3" t="s">
         <v>31</v>
@@ -14224,19 +14221,19 @@
         <v>728</v>
       </c>
       <c r="Q124" t="s">
-        <v>2536</v>
+        <v>2530</v>
       </c>
       <c r="R124" t="s">
-        <v>2538</v>
+        <v>2532</v>
       </c>
       <c r="S124" t="s">
         <v>618</v>
       </c>
       <c r="T124" t="s">
-        <v>2539</v>
+        <v>2533</v>
       </c>
       <c r="U124" t="s">
-        <v>2537</v>
+        <v>2531</v>
       </c>
     </row>
     <row r="125" spans="1:21" x14ac:dyDescent="0.3">
@@ -14573,7 +14570,7 @@
     </row>
     <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
-        <v>2723</v>
+        <v>2716</v>
       </c>
       <c r="B132" t="s">
         <v>22</v>
@@ -14582,13 +14579,13 @@
         <v>53</v>
       </c>
       <c r="D132" t="s">
-        <v>2724</v>
+        <v>2717</v>
       </c>
       <c r="E132" s="3">
         <v>2024</v>
       </c>
       <c r="F132" t="s">
-        <v>2725</v>
+        <v>2718</v>
       </c>
       <c r="G132" s="3" t="s">
         <v>25</v>
@@ -14600,22 +14597,22 @@
         <v>84</v>
       </c>
       <c r="O132" t="s">
-        <v>2726</v>
+        <v>2719</v>
       </c>
       <c r="Q132" t="s">
-        <v>2727</v>
+        <v>2720</v>
       </c>
       <c r="R132" t="s">
         <v>1159</v>
       </c>
       <c r="S132" t="s">
-        <v>2728</v>
+        <v>2721</v>
       </c>
       <c r="T132" t="s">
-        <v>2729</v>
+        <v>2722</v>
       </c>
       <c r="U132" t="s">
-        <v>2730</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.3">
@@ -15031,7 +15028,7 @@
     </row>
     <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
-        <v>2704</v>
+        <v>2698</v>
       </c>
       <c r="B142" t="s">
         <v>22</v>
@@ -15040,7 +15037,7 @@
         <v>23</v>
       </c>
       <c r="D142" t="s">
-        <v>2703</v>
+        <v>2697</v>
       </c>
       <c r="E142" s="3">
         <v>2011</v>
@@ -15061,7 +15058,7 @@
         <v>860</v>
       </c>
       <c r="Q142" t="s">
-        <v>2705</v>
+        <v>2699</v>
       </c>
       <c r="R142" t="s">
         <v>665</v>
@@ -15073,7 +15070,7 @@
         <v>2322</v>
       </c>
       <c r="U142" t="s">
-        <v>2706</v>
+        <v>2700</v>
       </c>
     </row>
     <row r="143" spans="1:21" x14ac:dyDescent="0.3">
@@ -15227,7 +15224,7 @@
     </row>
     <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
-        <v>2471</v>
+        <v>2468</v>
       </c>
       <c r="B147" t="s">
         <v>22</v>
@@ -15236,13 +15233,13 @@
         <v>23</v>
       </c>
       <c r="D147" t="s">
-        <v>2396</v>
+        <v>2393</v>
       </c>
       <c r="E147" s="3">
         <v>2002</v>
       </c>
       <c r="F147" t="s">
-        <v>2562</v>
+        <v>2556</v>
       </c>
       <c r="G147" s="3" t="s">
         <v>25</v>
@@ -15254,19 +15251,19 @@
         <v>65</v>
       </c>
       <c r="O147" t="s">
-        <v>2563</v>
+        <v>2557</v>
       </c>
       <c r="Q147" t="s">
-        <v>2564</v>
+        <v>2558</v>
       </c>
       <c r="R147" t="s">
-        <v>2566</v>
+        <v>2560</v>
       </c>
       <c r="S147" t="s">
-        <v>2567</v>
+        <v>2561</v>
       </c>
       <c r="U147" t="s">
-        <v>2565</v>
+        <v>2559</v>
       </c>
     </row>
     <row r="148" spans="1:21" x14ac:dyDescent="0.3">
@@ -15541,7 +15538,7 @@
     </row>
     <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
-        <v>2520</v>
+        <v>2729</v>
       </c>
       <c r="B154" t="s">
         <v>22</v>
@@ -15550,13 +15547,13 @@
         <v>23</v>
       </c>
       <c r="D154" t="s">
-        <v>2352</v>
+        <v>2724</v>
       </c>
       <c r="E154" s="3">
         <v>2003</v>
       </c>
       <c r="F154" t="s">
-        <v>2528</v>
+        <v>2522</v>
       </c>
       <c r="G154" s="3" t="s">
         <v>31</v>
@@ -15565,13 +15562,13 @@
         <v>31</v>
       </c>
       <c r="K154" t="s">
-        <v>2523</v>
+        <v>2517</v>
       </c>
       <c r="L154" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M154" t="s">
-        <v>2527</v>
+        <v>2521</v>
       </c>
       <c r="N154" s="3">
         <v>143</v>
@@ -15580,24 +15577,24 @@
         <v>1806</v>
       </c>
       <c r="Q154" t="s">
-        <v>2529</v>
+        <v>2523</v>
       </c>
       <c r="R154" t="s">
-        <v>2534</v>
+        <v>2528</v>
       </c>
       <c r="S154" t="s">
         <v>1660</v>
       </c>
       <c r="T154" t="s">
-        <v>2533</v>
+        <v>2527</v>
       </c>
       <c r="U154" t="s">
-        <v>2531</v>
+        <v>2525</v>
       </c>
     </row>
     <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
-        <v>2521</v>
+        <v>2728</v>
       </c>
       <c r="B155" t="s">
         <v>22</v>
@@ -15606,13 +15603,13 @@
         <v>23</v>
       </c>
       <c r="D155" t="s">
-        <v>2353</v>
+        <v>2725</v>
       </c>
       <c r="E155" s="3">
         <v>2006</v>
       </c>
       <c r="F155" t="s">
-        <v>2528</v>
+        <v>2522</v>
       </c>
       <c r="G155" s="3" t="s">
         <v>31</v>
@@ -15621,16 +15618,16 @@
         <v>31</v>
       </c>
       <c r="J155" t="s">
-        <v>2525</v>
+        <v>2519</v>
       </c>
       <c r="K155" t="s">
-        <v>2524</v>
+        <v>2518</v>
       </c>
       <c r="L155" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M155" t="s">
-        <v>2527</v>
+        <v>2521</v>
       </c>
       <c r="N155" s="3">
         <v>151</v>
@@ -15639,7 +15636,7 @@
         <v>1806</v>
       </c>
       <c r="Q155" t="s">
-        <v>2529</v>
+        <v>2523</v>
       </c>
       <c r="R155" t="s">
         <v>319</v>
@@ -15648,15 +15645,15 @@
         <v>1660</v>
       </c>
       <c r="T155" t="s">
-        <v>2533</v>
+        <v>2527</v>
       </c>
       <c r="U155" t="s">
-        <v>2530</v>
+        <v>2524</v>
       </c>
     </row>
     <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
-        <v>2522</v>
+        <v>2727</v>
       </c>
       <c r="B156" t="s">
         <v>22</v>
@@ -15665,13 +15662,13 @@
         <v>23</v>
       </c>
       <c r="D156" t="s">
-        <v>2354</v>
+        <v>2726</v>
       </c>
       <c r="E156" s="3">
         <v>2007</v>
       </c>
       <c r="F156" t="s">
-        <v>2528</v>
+        <v>2522</v>
       </c>
       <c r="G156" s="3" t="s">
         <v>31</v>
@@ -15680,13 +15677,13 @@
         <v>31</v>
       </c>
       <c r="J156" t="s">
-        <v>2526</v>
+        <v>2520</v>
       </c>
       <c r="L156" s="3" t="s">
         <v>25</v>
       </c>
       <c r="M156" t="s">
-        <v>2527</v>
+        <v>2521</v>
       </c>
       <c r="N156" s="3">
         <v>169</v>
@@ -15695,7 +15692,7 @@
         <v>1806</v>
       </c>
       <c r="Q156" t="s">
-        <v>2529</v>
+        <v>2523</v>
       </c>
       <c r="R156" t="s">
         <v>319</v>
@@ -15704,15 +15701,15 @@
         <v>1660</v>
       </c>
       <c r="T156" t="s">
-        <v>2533</v>
+        <v>2527</v>
       </c>
       <c r="U156" t="s">
-        <v>2532</v>
+        <v>2526</v>
       </c>
     </row>
     <row r="157" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
-        <v>2591</v>
+        <v>2585</v>
       </c>
       <c r="B157" t="s">
         <v>22</v>
@@ -15721,13 +15718,13 @@
         <v>23</v>
       </c>
       <c r="D157" t="s">
-        <v>2368</v>
+        <v>2365</v>
       </c>
       <c r="E157" s="3">
         <v>2011</v>
       </c>
       <c r="F157" t="s">
-        <v>2528</v>
+        <v>2522</v>
       </c>
       <c r="G157" s="3" t="s">
         <v>25</v>
@@ -15739,10 +15736,10 @@
         <v>107</v>
       </c>
       <c r="O157" t="s">
-        <v>2627</v>
+        <v>2621</v>
       </c>
       <c r="Q157" t="s">
-        <v>2629</v>
+        <v>2623</v>
       </c>
       <c r="R157" t="s">
         <v>319</v>
@@ -15751,10 +15748,10 @@
         <v>1718</v>
       </c>
       <c r="T157" t="s">
-        <v>2630</v>
+        <v>2624</v>
       </c>
       <c r="U157" t="s">
-        <v>2628</v>
+        <v>2622</v>
       </c>
     </row>
     <row r="158" spans="1:21" x14ac:dyDescent="0.3">
@@ -16172,7 +16169,7 @@
     </row>
     <row r="168" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
-        <v>2549</v>
+        <v>2543</v>
       </c>
       <c r="B168" t="s">
         <v>22</v>
@@ -16181,7 +16178,7 @@
         <v>23</v>
       </c>
       <c r="D168" t="s">
-        <v>2397</v>
+        <v>2394</v>
       </c>
       <c r="E168" s="3">
         <v>2017</v>
@@ -16199,22 +16196,22 @@
         <v>126</v>
       </c>
       <c r="O168" t="s">
-        <v>2576</v>
+        <v>2570</v>
       </c>
       <c r="Q168" t="s">
-        <v>2577</v>
+        <v>2571</v>
       </c>
       <c r="R168" t="s">
         <v>247</v>
       </c>
       <c r="S168" t="s">
-        <v>2579</v>
+        <v>2573</v>
       </c>
       <c r="T168" t="s">
-        <v>2580</v>
+        <v>2574</v>
       </c>
       <c r="U168" t="s">
-        <v>2578</v>
+        <v>2572</v>
       </c>
     </row>
     <row r="169" spans="1:21" x14ac:dyDescent="0.3">
@@ -16251,7 +16248,7 @@
     </row>
     <row r="170" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
-        <v>2542</v>
+        <v>2536</v>
       </c>
       <c r="B170" t="s">
         <v>22</v>
@@ -16260,13 +16257,13 @@
         <v>23</v>
       </c>
       <c r="D170" t="s">
-        <v>2358</v>
+        <v>2355</v>
       </c>
       <c r="E170" s="3">
         <v>1989</v>
       </c>
       <c r="F170" t="s">
-        <v>2543</v>
+        <v>2537</v>
       </c>
       <c r="G170" s="3" t="s">
         <v>25</v>
@@ -16281,21 +16278,21 @@
         <v>26</v>
       </c>
       <c r="Q170" t="s">
-        <v>2543</v>
+        <v>2537</v>
       </c>
       <c r="R170" t="s">
-        <v>2544</v>
+        <v>2538</v>
       </c>
       <c r="S170" t="s">
-        <v>2545</v>
+        <v>2539</v>
       </c>
       <c r="U170" t="s">
-        <v>2546</v>
+        <v>2540</v>
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
-        <v>2470</v>
+        <v>2467</v>
       </c>
       <c r="B171" t="s">
         <v>22</v>
@@ -16304,13 +16301,13 @@
         <v>23</v>
       </c>
       <c r="D171" t="s">
-        <v>2360</v>
+        <v>2357</v>
       </c>
       <c r="E171" s="3">
         <v>2016</v>
       </c>
       <c r="F171" t="s">
-        <v>2555</v>
+        <v>2549</v>
       </c>
       <c r="G171" s="3" t="s">
         <v>31</v>
@@ -16322,22 +16319,22 @@
         <v>96</v>
       </c>
       <c r="O171" t="s">
-        <v>2556</v>
+        <v>2550</v>
       </c>
       <c r="Q171" t="s">
-        <v>2557</v>
+        <v>2551</v>
       </c>
       <c r="R171" t="s">
-        <v>2559</v>
+        <v>2553</v>
       </c>
       <c r="S171" t="s">
-        <v>2560</v>
+        <v>2554</v>
       </c>
       <c r="T171" t="s">
-        <v>2561</v>
+        <v>2555</v>
       </c>
       <c r="U171" t="s">
-        <v>2558</v>
+        <v>2552</v>
       </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
@@ -16729,7 +16726,7 @@
     </row>
     <row r="181" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A181" t="s">
-        <v>2467</v>
+        <v>2464</v>
       </c>
       <c r="B181" t="s">
         <v>22</v>
@@ -16738,7 +16735,7 @@
         <v>23</v>
       </c>
       <c r="D181" t="s">
-        <v>2355</v>
+        <v>2352</v>
       </c>
       <c r="E181" s="3">
         <v>1997</v>
@@ -16765,13 +16762,13 @@
         <v>850</v>
       </c>
       <c r="S181" t="s">
-        <v>2447</v>
+        <v>2444</v>
       </c>
       <c r="T181" t="s">
         <v>1227</v>
       </c>
       <c r="U181" t="s">
-        <v>2535</v>
+        <v>2529</v>
       </c>
     </row>
     <row r="182" spans="1:21" x14ac:dyDescent="0.3">
@@ -17192,7 +17189,7 @@
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A192" t="s">
-        <v>2428</v>
+        <v>2425</v>
       </c>
       <c r="B192" t="s">
         <v>22</v>
@@ -17201,13 +17198,13 @@
         <v>23</v>
       </c>
       <c r="D192" t="s">
-        <v>2389</v>
+        <v>2386</v>
       </c>
       <c r="E192" s="3">
         <v>2004</v>
       </c>
       <c r="F192" t="s">
-        <v>2429</v>
+        <v>2426</v>
       </c>
       <c r="G192" s="3" t="s">
         <v>25</v>
@@ -17219,22 +17216,22 @@
         <v>125</v>
       </c>
       <c r="O192" t="s">
+        <v>2427</v>
+      </c>
+      <c r="Q192" t="s">
+        <v>2428</v>
+      </c>
+      <c r="R192" t="s">
         <v>2430</v>
       </c>
-      <c r="Q192" t="s">
+      <c r="S192" t="s">
         <v>2431</v>
       </c>
-      <c r="R192" t="s">
-        <v>2433</v>
-      </c>
-      <c r="S192" t="s">
-        <v>2434</v>
-      </c>
       <c r="T192" t="s">
-        <v>2435</v>
+        <v>2432</v>
       </c>
       <c r="U192" t="s">
-        <v>2432</v>
+        <v>2429</v>
       </c>
     </row>
     <row r="193" spans="1:21" x14ac:dyDescent="0.3">
@@ -17321,7 +17318,7 @@
     </row>
     <row r="195" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A195" t="s">
-        <v>2626</v>
+        <v>2620</v>
       </c>
       <c r="B195" t="s">
         <v>22</v>
@@ -17330,13 +17327,13 @@
         <v>23</v>
       </c>
       <c r="D195" t="s">
-        <v>2384</v>
+        <v>2381</v>
       </c>
       <c r="E195" s="3">
         <v>1989</v>
       </c>
       <c r="F195" t="s">
-        <v>2713</v>
+        <v>2707</v>
       </c>
       <c r="G195" s="3" t="s">
         <v>25</v>
@@ -17348,13 +17345,13 @@
         <v>97</v>
       </c>
       <c r="O195" t="s">
-        <v>2451</v>
+        <v>2448</v>
       </c>
       <c r="Q195" t="s">
         <v>980</v>
       </c>
       <c r="R195" t="s">
-        <v>2715</v>
+        <v>2709</v>
       </c>
       <c r="S195" t="s">
         <v>2058</v>
@@ -17363,7 +17360,7 @@
         <v>833</v>
       </c>
       <c r="U195" t="s">
-        <v>2714</v>
+        <v>2708</v>
       </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.3">
@@ -17447,7 +17444,7 @@
     </row>
     <row r="198" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A198" t="s">
-        <v>2411</v>
+        <v>2408</v>
       </c>
       <c r="B198" t="s">
         <v>22</v>
@@ -17456,13 +17453,13 @@
         <v>23</v>
       </c>
       <c r="D198" t="s">
-        <v>2391</v>
+        <v>2388</v>
       </c>
       <c r="E198" s="3">
         <v>2024</v>
       </c>
       <c r="F198" t="s">
-        <v>2398</v>
+        <v>2395</v>
       </c>
       <c r="G198" s="3" t="s">
         <v>31</v>
@@ -17477,19 +17474,19 @@
         <v>1443</v>
       </c>
       <c r="Q198" t="s">
-        <v>2398</v>
+        <v>2395</v>
       </c>
       <c r="R198" t="s">
-        <v>2415</v>
+        <v>2412</v>
       </c>
       <c r="S198" t="s">
-        <v>2413</v>
+        <v>2410</v>
       </c>
       <c r="T198" t="s">
-        <v>2414</v>
+        <v>2411</v>
       </c>
       <c r="U198" t="s">
-        <v>2412</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="199" spans="1:21" x14ac:dyDescent="0.3">
@@ -17579,7 +17576,7 @@
     </row>
     <row r="201" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A201" t="s">
-        <v>2449</v>
+        <v>2446</v>
       </c>
       <c r="B201" t="s">
         <v>22</v>
@@ -17588,13 +17585,13 @@
         <v>23</v>
       </c>
       <c r="D201" t="s">
-        <v>2386</v>
+        <v>2383</v>
       </c>
       <c r="E201" s="3">
         <v>2004</v>
       </c>
       <c r="F201" t="s">
-        <v>2450</v>
+        <v>2447</v>
       </c>
       <c r="G201" s="3" t="s">
         <v>25</v>
@@ -17606,22 +17603,22 @@
         <v>99</v>
       </c>
       <c r="O201" t="s">
-        <v>2451</v>
+        <v>2448</v>
       </c>
       <c r="Q201" t="s">
         <v>273</v>
       </c>
       <c r="R201" t="s">
-        <v>2453</v>
+        <v>2450</v>
       </c>
       <c r="S201" t="s">
         <v>882</v>
       </c>
       <c r="T201" t="s">
-        <v>2454</v>
+        <v>2451</v>
       </c>
       <c r="U201" t="s">
-        <v>2452</v>
+        <v>2449</v>
       </c>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.3">
@@ -17676,7 +17673,7 @@
     </row>
     <row r="203" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A203" t="s">
-        <v>2593</v>
+        <v>2587</v>
       </c>
       <c r="B203" t="s">
         <v>22</v>
@@ -17685,7 +17682,7 @@
         <v>23</v>
       </c>
       <c r="D203" t="s">
-        <v>2372</v>
+        <v>2369</v>
       </c>
       <c r="E203" s="3">
         <v>2007</v>
@@ -17706,19 +17703,19 @@
         <v>860</v>
       </c>
       <c r="Q203" t="s">
-        <v>2648</v>
+        <v>2642</v>
       </c>
       <c r="R203" t="s">
         <v>2262</v>
       </c>
       <c r="S203" t="s">
-        <v>2649</v>
+        <v>2643</v>
       </c>
       <c r="T203" t="s">
         <v>777</v>
       </c>
       <c r="U203" t="s">
-        <v>2647</v>
+        <v>2641</v>
       </c>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.3">
@@ -17758,7 +17755,7 @@
     </row>
     <row r="205" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A205" t="s">
-        <v>2654</v>
+        <v>2648</v>
       </c>
       <c r="B205" t="s">
         <v>22</v>
@@ -17767,13 +17764,13 @@
         <v>23</v>
       </c>
       <c r="D205" t="s">
-        <v>2374</v>
+        <v>2371</v>
       </c>
       <c r="E205" s="3">
         <v>1976</v>
       </c>
       <c r="F205" t="s">
-        <v>2655</v>
+        <v>2649</v>
       </c>
       <c r="G205" s="3" t="s">
         <v>25</v>
@@ -17785,28 +17782,28 @@
         <v>25</v>
       </c>
       <c r="M205" t="s">
-        <v>2656</v>
+        <v>2650</v>
       </c>
       <c r="N205" s="3">
         <v>120</v>
       </c>
       <c r="O205" t="s">
-        <v>2657</v>
+        <v>2651</v>
       </c>
       <c r="Q205" t="s">
-        <v>2658</v>
+        <v>2652</v>
       </c>
       <c r="R205" t="s">
-        <v>2660</v>
+        <v>2654</v>
       </c>
       <c r="S205" t="s">
-        <v>2661</v>
+        <v>2655</v>
       </c>
       <c r="T205" t="s">
-        <v>2662</v>
+        <v>2656</v>
       </c>
       <c r="U205" t="s">
-        <v>2659</v>
+        <v>2653</v>
       </c>
     </row>
     <row r="206" spans="1:21" x14ac:dyDescent="0.3">
@@ -17844,7 +17841,7 @@
         <v>977</v>
       </c>
       <c r="T206" t="s">
-        <v>2618</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="207" spans="1:21" x14ac:dyDescent="0.3">
@@ -18303,7 +18300,7 @@
     </row>
     <row r="218" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A218" t="s">
-        <v>2622</v>
+        <v>2616</v>
       </c>
       <c r="B218" t="s">
         <v>22</v>
@@ -18312,13 +18309,13 @@
         <v>23</v>
       </c>
       <c r="D218" t="s">
-        <v>2373</v>
+        <v>2370</v>
       </c>
       <c r="E218" s="3">
         <v>2011</v>
       </c>
       <c r="F218" t="s">
-        <v>2650</v>
+        <v>2644</v>
       </c>
       <c r="G218" s="3" t="s">
         <v>25</v>
@@ -18330,10 +18327,10 @@
         <v>119</v>
       </c>
       <c r="O218" t="s">
-        <v>2651</v>
+        <v>2645</v>
       </c>
       <c r="Q218" t="s">
-        <v>2652</v>
+        <v>2646</v>
       </c>
       <c r="R218" t="s">
         <v>1659</v>
@@ -18345,7 +18342,7 @@
         <v>321</v>
       </c>
       <c r="U218" t="s">
-        <v>2653</v>
+        <v>2647</v>
       </c>
     </row>
     <row r="219" spans="1:21" x14ac:dyDescent="0.3">
@@ -18467,7 +18464,7 @@
     </row>
     <row r="222" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A222" t="s">
-        <v>2505</v>
+        <v>2502</v>
       </c>
       <c r="B222" t="s">
         <v>22</v>
@@ -18476,7 +18473,7 @@
         <v>23</v>
       </c>
       <c r="D222" t="s">
-        <v>2363</v>
+        <v>2360</v>
       </c>
       <c r="E222" s="3">
         <v>2016</v>
@@ -18494,28 +18491,28 @@
         <v>25</v>
       </c>
       <c r="M222" t="s">
-        <v>2581</v>
+        <v>2575</v>
       </c>
       <c r="N222" s="3">
         <v>129</v>
       </c>
       <c r="O222" t="s">
-        <v>2582</v>
+        <v>2576</v>
       </c>
       <c r="Q222" t="s">
-        <v>2583</v>
+        <v>2577</v>
       </c>
       <c r="R222" t="s">
         <v>617</v>
       </c>
       <c r="S222" t="s">
-        <v>2585</v>
+        <v>2579</v>
       </c>
       <c r="T222" t="s">
-        <v>2586</v>
+        <v>2580</v>
       </c>
       <c r="U222" t="s">
-        <v>2584</v>
+        <v>2578</v>
       </c>
     </row>
     <row r="223" spans="1:21" x14ac:dyDescent="0.3">
@@ -20054,7 +20051,7 @@
     </row>
     <row r="261" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A261" t="s">
-        <v>2417</v>
+        <v>2414</v>
       </c>
       <c r="B261" t="s">
         <v>22</v>
@@ -20063,13 +20060,13 @@
         <v>23</v>
       </c>
       <c r="D261" t="s">
-        <v>2416</v>
+        <v>2413</v>
       </c>
       <c r="E261" s="3">
         <v>2022</v>
       </c>
       <c r="F261" t="s">
-        <v>2399</v>
+        <v>2396</v>
       </c>
       <c r="G261" s="3" t="s">
         <v>31</v>
@@ -20084,7 +20081,7 @@
         <v>1443</v>
       </c>
       <c r="Q261" t="s">
-        <v>2399</v>
+        <v>2396</v>
       </c>
       <c r="R261" t="s">
         <v>1159</v>
@@ -20093,10 +20090,10 @@
         <v>2243</v>
       </c>
       <c r="T261" t="s">
-        <v>2419</v>
+        <v>2416</v>
       </c>
       <c r="U261" t="s">
-        <v>2418</v>
+        <v>2415</v>
       </c>
     </row>
     <row r="262" spans="1:21" x14ac:dyDescent="0.3">
@@ -20922,7 +20919,7 @@
     </row>
     <row r="284" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A284" t="s">
-        <v>2492</v>
+        <v>2489</v>
       </c>
       <c r="B284" t="s">
         <v>22</v>
@@ -20937,7 +20934,7 @@
         <v>2009</v>
       </c>
       <c r="F284" t="s">
-        <v>2493</v>
+        <v>2490</v>
       </c>
       <c r="G284" s="3" t="s">
         <v>25</v>
@@ -20952,19 +20949,19 @@
         <v>204</v>
       </c>
       <c r="Q284" t="s">
+        <v>2491</v>
+      </c>
+      <c r="R284" t="s">
+        <v>2493</v>
+      </c>
+      <c r="S284" t="s">
         <v>2494</v>
       </c>
-      <c r="R284" t="s">
-        <v>2496</v>
-      </c>
-      <c r="S284" t="s">
-        <v>2497</v>
-      </c>
       <c r="T284" t="s">
-        <v>2498</v>
+        <v>2495</v>
       </c>
       <c r="U284" t="s">
-        <v>2495</v>
+        <v>2492</v>
       </c>
     </row>
     <row r="285" spans="1:21" x14ac:dyDescent="0.3">
@@ -21903,7 +21900,7 @@
     </row>
     <row r="308" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A308" t="s">
-        <v>2548</v>
+        <v>2542</v>
       </c>
       <c r="B308" t="s">
         <v>22</v>
@@ -21912,7 +21909,7 @@
         <v>23</v>
       </c>
       <c r="D308" t="s">
-        <v>2361</v>
+        <v>2358</v>
       </c>
       <c r="E308" s="3">
         <v>2013</v>
@@ -21930,13 +21927,13 @@
         <v>25</v>
       </c>
       <c r="M308" t="s">
-        <v>2568</v>
+        <v>2562</v>
       </c>
       <c r="N308" s="3">
         <v>161</v>
       </c>
       <c r="O308" t="s">
-        <v>2569</v>
+        <v>2563</v>
       </c>
       <c r="Q308" t="s">
         <v>781</v>
@@ -21948,10 +21945,10 @@
         <v>1518</v>
       </c>
       <c r="T308" t="s">
-        <v>2570</v>
+        <v>2564</v>
       </c>
       <c r="U308" t="s">
-        <v>2571</v>
+        <v>2565</v>
       </c>
     </row>
     <row r="309" spans="1:21" x14ac:dyDescent="0.3">
@@ -22345,7 +22342,7 @@
     </row>
     <row r="319" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A319" t="s">
-        <v>2466</v>
+        <v>2463</v>
       </c>
       <c r="B319" t="s">
         <v>22</v>
@@ -22360,7 +22357,7 @@
         <v>2012</v>
       </c>
       <c r="F319" t="s">
-        <v>2515</v>
+        <v>2512</v>
       </c>
       <c r="G319" s="3" t="s">
         <v>25</v>
@@ -22372,27 +22369,27 @@
         <v>165</v>
       </c>
       <c r="O319" t="s">
-        <v>2516</v>
+        <v>2513</v>
       </c>
       <c r="Q319" t="s">
+        <v>2512</v>
+      </c>
+      <c r="R319" t="s">
+        <v>2514</v>
+      </c>
+      <c r="S319" t="s">
         <v>2515</v>
-      </c>
-      <c r="R319" t="s">
-        <v>2517</v>
-      </c>
-      <c r="S319" t="s">
-        <v>2518</v>
       </c>
       <c r="T319" t="s">
         <v>2029</v>
       </c>
       <c r="U319" t="s">
-        <v>2519</v>
+        <v>2516</v>
       </c>
     </row>
     <row r="320" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A320" t="s">
-        <v>2469</v>
+        <v>2466</v>
       </c>
       <c r="B320" t="s">
         <v>22</v>
@@ -22401,13 +22398,13 @@
         <v>23</v>
       </c>
       <c r="D320" t="s">
-        <v>2357</v>
+        <v>2354</v>
       </c>
       <c r="E320" s="3">
         <v>2015</v>
       </c>
       <c r="F320" t="s">
-        <v>2515</v>
+        <v>2512</v>
       </c>
       <c r="G320" s="3" t="s">
         <v>25</v>
@@ -22422,19 +22419,19 @@
         <v>922</v>
       </c>
       <c r="Q320" t="s">
+        <v>2512</v>
+      </c>
+      <c r="R320" t="s">
+        <v>2534</v>
+      </c>
+      <c r="S320" t="s">
         <v>2515</v>
       </c>
-      <c r="R320" t="s">
-        <v>2540</v>
-      </c>
-      <c r="S320" t="s">
-        <v>2518</v>
-      </c>
       <c r="T320" t="s">
-        <v>2539</v>
+        <v>2533</v>
       </c>
       <c r="U320" t="s">
-        <v>2541</v>
+        <v>2535</v>
       </c>
     </row>
     <row r="321" spans="1:21" x14ac:dyDescent="0.3">
@@ -22486,7 +22483,7 @@
     </row>
     <row r="322" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A322" t="s">
-        <v>2547</v>
+        <v>2541</v>
       </c>
       <c r="B322" t="s">
         <v>22</v>
@@ -22495,13 +22492,13 @@
         <v>23</v>
       </c>
       <c r="D322" t="s">
-        <v>2359</v>
+        <v>2356</v>
       </c>
       <c r="E322" s="3">
         <v>1998</v>
       </c>
       <c r="F322" t="s">
-        <v>2550</v>
+        <v>2544</v>
       </c>
       <c r="G322" s="3" t="s">
         <v>25</v>
@@ -22513,22 +22510,22 @@
         <v>132</v>
       </c>
       <c r="O322" t="s">
-        <v>2551</v>
+        <v>2545</v>
       </c>
       <c r="Q322" t="s">
-        <v>2550</v>
+        <v>2544</v>
       </c>
       <c r="R322" t="s">
-        <v>2553</v>
+        <v>2547</v>
       </c>
       <c r="S322" t="s">
-        <v>2554</v>
+        <v>2548</v>
       </c>
       <c r="T322" t="s">
         <v>145</v>
       </c>
       <c r="U322" t="s">
-        <v>2552</v>
+        <v>2546</v>
       </c>
     </row>
     <row r="323" spans="1:21" x14ac:dyDescent="0.3">
@@ -22612,7 +22609,7 @@
     </row>
     <row r="325" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A325" t="s">
-        <v>2404</v>
+        <v>2401</v>
       </c>
       <c r="B325" t="s">
         <v>22</v>
@@ -22621,13 +22618,13 @@
         <v>23</v>
       </c>
       <c r="D325" t="s">
-        <v>2392</v>
+        <v>2389</v>
       </c>
       <c r="E325" s="3">
         <v>2021</v>
       </c>
       <c r="F325" t="s">
-        <v>2400</v>
+        <v>2397</v>
       </c>
       <c r="G325" s="3" t="s">
         <v>31</v>
@@ -22639,22 +22636,22 @@
         <v>144</v>
       </c>
       <c r="O325" t="s">
-        <v>2657</v>
+        <v>2651</v>
       </c>
       <c r="Q325" t="s">
-        <v>2401</v>
+        <v>2398</v>
       </c>
       <c r="R325" t="s">
         <v>288</v>
       </c>
       <c r="S325" t="s">
-        <v>2403</v>
+        <v>2400</v>
       </c>
       <c r="T325" t="s">
         <v>2029</v>
       </c>
       <c r="U325" t="s">
-        <v>2402</v>
+        <v>2399</v>
       </c>
     </row>
     <row r="326" spans="1:21" x14ac:dyDescent="0.3">
@@ -23456,7 +23453,7 @@
     </row>
     <row r="345" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A345" t="s">
-        <v>2590</v>
+        <v>2584</v>
       </c>
       <c r="B345" t="s">
         <v>22</v>
@@ -23465,7 +23462,7 @@
         <v>23</v>
       </c>
       <c r="D345" t="s">
-        <v>2367</v>
+        <v>2364</v>
       </c>
       <c r="E345" s="3">
         <v>2005</v>
@@ -23486,7 +23483,7 @@
         <v>860</v>
       </c>
       <c r="Q345" t="s">
-        <v>2619</v>
+        <v>2613</v>
       </c>
       <c r="R345" t="s">
         <v>831</v>
@@ -23498,7 +23495,7 @@
         <v>914</v>
       </c>
       <c r="U345" t="s">
-        <v>2620</v>
+        <v>2614</v>
       </c>
     </row>
     <row r="346" spans="1:21" x14ac:dyDescent="0.3">
@@ -23535,7 +23532,7 @@
     </row>
     <row r="347" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A347" t="s">
-        <v>2612</v>
+        <v>2606</v>
       </c>
       <c r="B347" t="s">
         <v>22</v>
@@ -23544,13 +23541,13 @@
         <v>23</v>
       </c>
       <c r="D347" t="s">
-        <v>2380</v>
+        <v>2377</v>
       </c>
       <c r="E347" s="3">
         <v>2012</v>
       </c>
       <c r="F347" t="s">
-        <v>2689</v>
+        <v>2683</v>
       </c>
       <c r="G347" s="3" t="s">
         <v>25</v>
@@ -23562,10 +23559,10 @@
         <v>111</v>
       </c>
       <c r="O347" t="s">
-        <v>2657</v>
+        <v>2651</v>
       </c>
       <c r="Q347" t="s">
-        <v>2690</v>
+        <v>2684</v>
       </c>
       <c r="R347" t="s">
         <v>993</v>
@@ -23574,15 +23571,15 @@
         <v>712</v>
       </c>
       <c r="T347" t="s">
-        <v>2679</v>
+        <v>2673</v>
       </c>
       <c r="U347" t="s">
-        <v>2691</v>
+        <v>2685</v>
       </c>
     </row>
     <row r="348" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A348" t="s">
-        <v>2442</v>
+        <v>2439</v>
       </c>
       <c r="B348" t="s">
         <v>22</v>
@@ -23591,13 +23588,13 @@
         <v>23</v>
       </c>
       <c r="D348" t="s">
-        <v>2387</v>
+        <v>2384</v>
       </c>
       <c r="E348" s="3">
         <v>2010</v>
       </c>
       <c r="F348" t="s">
-        <v>2443</v>
+        <v>2440</v>
       </c>
       <c r="G348" s="3" t="s">
         <v>31</v>
@@ -23612,19 +23609,19 @@
         <v>579</v>
       </c>
       <c r="Q348" t="s">
+        <v>2441</v>
+      </c>
+      <c r="R348" t="s">
+        <v>2443</v>
+      </c>
+      <c r="S348" t="s">
         <v>2444</v>
       </c>
-      <c r="R348" t="s">
-        <v>2446</v>
-      </c>
-      <c r="S348" t="s">
-        <v>2447</v>
-      </c>
       <c r="T348" t="s">
-        <v>2448</v>
+        <v>2445</v>
       </c>
       <c r="U348" t="s">
-        <v>2445</v>
+        <v>2442</v>
       </c>
     </row>
     <row r="349" spans="1:21" x14ac:dyDescent="0.3">
@@ -23869,7 +23866,7 @@
     </row>
     <row r="355" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A355" t="s">
-        <v>2462</v>
+        <v>2459</v>
       </c>
       <c r="B355" t="s">
         <v>22</v>
@@ -23884,7 +23881,7 @@
         <v>2004</v>
       </c>
       <c r="F355" t="s">
-        <v>2473</v>
+        <v>2470</v>
       </c>
       <c r="G355" s="3" t="s">
         <v>25</v>
@@ -23896,22 +23893,22 @@
         <v>100</v>
       </c>
       <c r="O355" t="s">
+        <v>2471</v>
+      </c>
+      <c r="Q355" t="s">
+        <v>2475</v>
+      </c>
+      <c r="R355" t="s">
+        <v>2473</v>
+      </c>
+      <c r="S355" t="s">
         <v>2474</v>
       </c>
-      <c r="Q355" t="s">
-        <v>2478</v>
-      </c>
-      <c r="R355" t="s">
-        <v>2476</v>
-      </c>
-      <c r="S355" t="s">
-        <v>2477</v>
-      </c>
       <c r="T355" t="s">
-        <v>2441</v>
+        <v>2438</v>
       </c>
       <c r="U355" t="s">
-        <v>2475</v>
+        <v>2472</v>
       </c>
     </row>
     <row r="356" spans="1:21" x14ac:dyDescent="0.3">
@@ -24626,7 +24623,7 @@
     </row>
     <row r="372" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A372" t="s">
-        <v>2464</v>
+        <v>2461</v>
       </c>
       <c r="B372" t="s">
         <v>22</v>
@@ -24641,7 +24638,7 @@
         <v>2007</v>
       </c>
       <c r="F372" t="s">
-        <v>2486</v>
+        <v>2483</v>
       </c>
       <c r="G372" s="3" t="s">
         <v>25</v>
@@ -24656,19 +24653,19 @@
         <v>773</v>
       </c>
       <c r="Q372" t="s">
+        <v>2484</v>
+      </c>
+      <c r="R372" t="s">
+        <v>2486</v>
+      </c>
+      <c r="S372" t="s">
         <v>2487</v>
       </c>
-      <c r="R372" t="s">
-        <v>2489</v>
-      </c>
-      <c r="S372" t="s">
-        <v>2490</v>
-      </c>
       <c r="T372" t="s">
-        <v>2491</v>
+        <v>2488</v>
       </c>
       <c r="U372" t="s">
-        <v>2488</v>
+        <v>2485</v>
       </c>
     </row>
     <row r="373" spans="1:21" x14ac:dyDescent="0.3">
@@ -24764,7 +24761,7 @@
     </row>
     <row r="375" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A375" t="s">
-        <v>2611</v>
+        <v>2605</v>
       </c>
       <c r="B375" t="s">
         <v>22</v>
@@ -24773,13 +24770,13 @@
         <v>23</v>
       </c>
       <c r="D375" t="s">
-        <v>2378</v>
+        <v>2375</v>
       </c>
       <c r="E375" s="3">
         <v>2007</v>
       </c>
       <c r="F375" t="s">
-        <v>2680</v>
+        <v>2674</v>
       </c>
       <c r="G375" s="3" t="s">
         <v>31</v>
@@ -24794,19 +24791,19 @@
         <v>556</v>
       </c>
       <c r="Q375" t="s">
-        <v>2680</v>
+        <v>2674</v>
       </c>
       <c r="R375" t="s">
-        <v>2681</v>
+        <v>2675</v>
       </c>
       <c r="S375" t="s">
-        <v>2683</v>
+        <v>2677</v>
       </c>
       <c r="T375" t="s">
         <v>1161</v>
       </c>
       <c r="U375" t="s">
-        <v>2682</v>
+        <v>2676</v>
       </c>
     </row>
     <row r="376" spans="1:21" x14ac:dyDescent="0.3">
@@ -24893,7 +24890,7 @@
     </row>
     <row r="378" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A378" t="s">
-        <v>2621</v>
+        <v>2615</v>
       </c>
       <c r="B378" t="s">
         <v>22</v>
@@ -24902,13 +24899,13 @@
         <v>23</v>
       </c>
       <c r="D378" t="s">
-        <v>2369</v>
+        <v>2366</v>
       </c>
       <c r="E378" s="3">
         <v>2016</v>
       </c>
       <c r="F378" t="s">
-        <v>2631</v>
+        <v>2625</v>
       </c>
       <c r="G378" s="3" t="s">
         <v>31</v>
@@ -24920,28 +24917,28 @@
         <v>25</v>
       </c>
       <c r="M378" t="s">
-        <v>2632</v>
+        <v>2626</v>
       </c>
       <c r="N378" s="3">
         <v>123</v>
       </c>
       <c r="O378" t="s">
-        <v>2637</v>
+        <v>2631</v>
       </c>
       <c r="Q378" t="s">
-        <v>2634</v>
+        <v>2628</v>
       </c>
       <c r="R378" t="s">
-        <v>2635</v>
+        <v>2629</v>
       </c>
       <c r="S378" t="s">
-        <v>2617</v>
+        <v>2611</v>
       </c>
       <c r="T378" t="s">
-        <v>2636</v>
+        <v>2630</v>
       </c>
       <c r="U378" t="s">
-        <v>2633</v>
+        <v>2627</v>
       </c>
     </row>
     <row r="379" spans="1:21" x14ac:dyDescent="0.3">
@@ -25353,7 +25350,7 @@
     </row>
     <row r="389" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A389" t="s">
-        <v>2463</v>
+        <v>2460</v>
       </c>
       <c r="B389" t="s">
         <v>22</v>
@@ -25368,7 +25365,7 @@
         <v>2018</v>
       </c>
       <c r="F389" t="s">
-        <v>2479</v>
+        <v>2476</v>
       </c>
       <c r="G389" s="3" t="s">
         <v>25</v>
@@ -25381,7 +25378,7 @@
         <v>25</v>
       </c>
       <c r="M389" s="5" t="s">
-        <v>2485</v>
+        <v>2482</v>
       </c>
       <c r="N389" s="3">
         <v>91</v>
@@ -25390,19 +25387,19 @@
         <v>171</v>
       </c>
       <c r="Q389" t="s">
+        <v>2477</v>
+      </c>
+      <c r="R389" t="s">
+        <v>2478</v>
+      </c>
+      <c r="S389" t="s">
+        <v>2479</v>
+      </c>
+      <c r="T389" t="s">
         <v>2480</v>
       </c>
-      <c r="R389" t="s">
+      <c r="U389" t="s">
         <v>2481</v>
-      </c>
-      <c r="S389" t="s">
-        <v>2482</v>
-      </c>
-      <c r="T389" t="s">
-        <v>2483</v>
-      </c>
-      <c r="U389" t="s">
-        <v>2484</v>
       </c>
     </row>
     <row r="390" spans="1:21" x14ac:dyDescent="0.3">
@@ -26731,7 +26728,7 @@
     </row>
     <row r="422" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A422" t="s">
-        <v>2405</v>
+        <v>2402</v>
       </c>
       <c r="B422" t="s">
         <v>22</v>
@@ -26740,13 +26737,13 @@
         <v>23</v>
       </c>
       <c r="D422" t="s">
-        <v>2393</v>
+        <v>2390</v>
       </c>
       <c r="E422" s="3">
         <v>2023</v>
       </c>
       <c r="F422" t="s">
-        <v>2406</v>
+        <v>2403</v>
       </c>
       <c r="G422" s="3" t="s">
         <v>25</v>
@@ -26761,19 +26758,19 @@
         <v>623</v>
       </c>
       <c r="Q422" t="s">
-        <v>2407</v>
+        <v>2404</v>
       </c>
       <c r="R422" t="s">
-        <v>2409</v>
+        <v>2406</v>
       </c>
       <c r="S422" t="s">
         <v>2243</v>
       </c>
       <c r="T422" t="s">
-        <v>2410</v>
+        <v>2407</v>
       </c>
       <c r="U422" t="s">
-        <v>2408</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="423" spans="1:21" x14ac:dyDescent="0.3">
@@ -27221,7 +27218,7 @@
     </row>
     <row r="433" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A433" t="s">
-        <v>2623</v>
+        <v>2617</v>
       </c>
       <c r="B433" t="s">
         <v>22</v>
@@ -27230,13 +27227,13 @@
         <v>23</v>
       </c>
       <c r="D433" t="s">
-        <v>2379</v>
+        <v>2376</v>
       </c>
       <c r="E433" s="3">
         <v>2012</v>
       </c>
       <c r="F433" t="s">
-        <v>2684</v>
+        <v>2678</v>
       </c>
       <c r="G433" s="3" t="s">
         <v>25</v>
@@ -27251,19 +27248,19 @@
         <v>1711</v>
       </c>
       <c r="Q433" t="s">
-        <v>2685</v>
+        <v>2679</v>
       </c>
       <c r="R433" t="s">
-        <v>2573</v>
+        <v>2567</v>
       </c>
       <c r="S433" t="s">
-        <v>2686</v>
+        <v>2680</v>
       </c>
       <c r="T433" t="s">
-        <v>2687</v>
+        <v>2681</v>
       </c>
       <c r="U433" t="s">
-        <v>2688</v>
+        <v>2682</v>
       </c>
     </row>
     <row r="434" spans="1:21" x14ac:dyDescent="0.3">
@@ -27845,7 +27842,7 @@
     </row>
     <row r="448" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A448" t="s">
-        <v>2610</v>
+        <v>2604</v>
       </c>
       <c r="B448" t="s">
         <v>22</v>
@@ -27854,13 +27851,13 @@
         <v>23</v>
       </c>
       <c r="D448" t="s">
-        <v>2371</v>
+        <v>2368</v>
       </c>
       <c r="E448" s="3">
         <v>2011</v>
       </c>
       <c r="F448" t="s">
-        <v>2642</v>
+        <v>2636</v>
       </c>
       <c r="G448" s="3" t="s">
         <v>25</v>
@@ -27872,19 +27869,19 @@
         <v>94</v>
       </c>
       <c r="O448" t="s">
-        <v>2643</v>
+        <v>2637</v>
       </c>
       <c r="Q448" t="s">
-        <v>2642</v>
+        <v>2636</v>
       </c>
       <c r="S448" t="s">
-        <v>2645</v>
+        <v>2639</v>
       </c>
       <c r="T448" t="s">
-        <v>2646</v>
+        <v>2640</v>
       </c>
       <c r="U448" t="s">
-        <v>2644</v>
+        <v>2638</v>
       </c>
     </row>
     <row r="449" spans="1:21" x14ac:dyDescent="0.3">
@@ -27921,7 +27918,7 @@
     </row>
     <row r="450" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A450" t="s">
-        <v>2395</v>
+        <v>2392</v>
       </c>
       <c r="B450" t="s">
         <v>22</v>
@@ -27930,7 +27927,7 @@
         <v>53</v>
       </c>
       <c r="D450" t="s">
-        <v>2394</v>
+        <v>2391</v>
       </c>
       <c r="E450" s="3">
         <v>2025</v>
@@ -28014,7 +28011,7 @@
     </row>
     <row r="453" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A453" t="s">
-        <v>2603</v>
+        <v>2597</v>
       </c>
       <c r="B453" t="s">
         <v>22</v>
@@ -28041,22 +28038,22 @@
         <v>117</v>
       </c>
       <c r="O453" t="s">
-        <v>2663</v>
+        <v>2657</v>
       </c>
       <c r="Q453" t="s">
-        <v>2664</v>
+        <v>2658</v>
       </c>
       <c r="R453" t="s">
-        <v>2666</v>
+        <v>2660</v>
       </c>
       <c r="S453" t="s">
-        <v>2667</v>
+        <v>2661</v>
       </c>
       <c r="T453" t="s">
         <v>802</v>
       </c>
       <c r="U453" t="s">
-        <v>2665</v>
+        <v>2659</v>
       </c>
     </row>
     <row r="454" spans="1:21" x14ac:dyDescent="0.3">
@@ -28963,7 +28960,7 @@
     </row>
     <row r="473" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A473" t="s">
-        <v>2624</v>
+        <v>2618</v>
       </c>
       <c r="B473" t="s">
         <v>397</v>
@@ -28972,13 +28969,13 @@
         <v>23</v>
       </c>
       <c r="D473" t="s">
-        <v>2382</v>
+        <v>2379</v>
       </c>
       <c r="E473" s="3">
         <v>2009</v>
       </c>
       <c r="F473" t="s">
-        <v>2696</v>
+        <v>2690</v>
       </c>
       <c r="G473" s="3" t="s">
         <v>31</v>
@@ -28990,7 +28987,7 @@
         <v>25</v>
       </c>
       <c r="M473" t="s">
-        <v>2697</v>
+        <v>2691</v>
       </c>
       <c r="N473" s="3">
         <v>22</v>
@@ -28999,19 +28996,19 @@
         <v>171</v>
       </c>
       <c r="Q473" t="s">
-        <v>2698</v>
+        <v>2692</v>
       </c>
       <c r="R473" t="s">
-        <v>2700</v>
+        <v>2694</v>
       </c>
       <c r="S473" t="s">
-        <v>2701</v>
+        <v>2695</v>
       </c>
       <c r="T473" t="s">
-        <v>2702</v>
+        <v>2696</v>
       </c>
       <c r="U473" t="s">
-        <v>2699</v>
+        <v>2693</v>
       </c>
     </row>
     <row r="474" spans="1:21" x14ac:dyDescent="0.3">
@@ -30256,7 +30253,7 @@
     </row>
     <row r="503" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A503" t="s">
-        <v>2420</v>
+        <v>2417</v>
       </c>
       <c r="B503" t="s">
         <v>397</v>
@@ -30265,19 +30262,19 @@
         <v>23</v>
       </c>
       <c r="D503" t="s">
-        <v>2390</v>
+        <v>2387</v>
       </c>
       <c r="E503" s="3">
         <v>1993</v>
       </c>
       <c r="F503" t="s">
-        <v>2421</v>
+        <v>2418</v>
       </c>
       <c r="G503" s="3" t="s">
         <v>31</v>
       </c>
       <c r="H503" t="s">
-        <v>2602</v>
+        <v>2596</v>
       </c>
       <c r="I503" s="3" t="s">
         <v>31</v>
@@ -30287,7 +30284,7 @@
         <v>25</v>
       </c>
       <c r="M503" s="5" t="s">
-        <v>2422</v>
+        <v>2419</v>
       </c>
       <c r="N503" s="3">
         <v>22</v>
@@ -30296,19 +30293,19 @@
         <v>1540</v>
       </c>
       <c r="Q503" t="s">
+        <v>2421</v>
+      </c>
+      <c r="R503" t="s">
+        <v>2422</v>
+      </c>
+      <c r="S503" t="s">
+        <v>2423</v>
+      </c>
+      <c r="T503" t="s">
         <v>2424</v>
       </c>
-      <c r="R503" t="s">
-        <v>2425</v>
-      </c>
-      <c r="S503" t="s">
-        <v>2426</v>
-      </c>
-      <c r="T503" t="s">
-        <v>2427</v>
-      </c>
       <c r="U503" t="s">
-        <v>2423</v>
+        <v>2420</v>
       </c>
     </row>
     <row r="504" spans="1:21" x14ac:dyDescent="0.3">

</xml_diff>